<commit_message>
Agregar nuevos datos de criptomonedas y actualizar predicciones: incluir PAX Gold, Solv Protocol BTC, y Aerodrome Finance con sus respectivos gráficos y detalles.
</commit_message>
<xml_diff>
--- a/data/predicciones_criptos.xlsx
+++ b/data/predicciones_criptos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1538,13 +1538,9 @@
         <v>39.17162961148887</v>
       </c>
       <c r="J29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>🟢 Rendimiento mensual superior al 30%</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4041,13 +4037,9 @@
         <v>40.64601967701537</v>
       </c>
       <c r="J96" t="b">
-        <v>1</v>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>📊 Subida mensual fuerte + tendencia semanal positiva</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4119,9 +4111,1821 @@
         <v>40.59617452460589</v>
       </c>
       <c r="J98" t="b">
-        <v>0</v>
-      </c>
-      <c r="K98" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>🟢 Rendimiento mensual superior al 30%</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>PAX Gold</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>paxg</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/9519/large/paxgold.png?1696509604</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>/charts/paxg_chart.png</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>931501024</v>
+      </c>
+      <c r="F99" t="n">
+        <v>3334.09</v>
+      </c>
+      <c r="G99" t="n">
+        <v>-0.7453123512414841</v>
+      </c>
+      <c r="H99" t="n">
+        <v>-0.444625610405908</v>
+      </c>
+      <c r="I99" t="n">
+        <v>-0.886004824973551</v>
+      </c>
+      <c r="J99" t="b">
+        <v>0</v>
+      </c>
+      <c r="K99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Solv Protocol BTC</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>solvbtc</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/36800/large/solvBTC.png?1719810684</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>/charts/solvbtc_chart.png</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>926497438</v>
+      </c>
+      <c r="F100" t="n">
+        <v>109560</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0.284884133536832</v>
+      </c>
+      <c r="H100" t="n">
+        <v>2.168828028781043</v>
+      </c>
+      <c r="I100" t="n">
+        <v>3.555667558073679</v>
+      </c>
+      <c r="J100" t="b">
+        <v>0</v>
+      </c>
+      <c r="K100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>SyrupUSDC</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>syrupusdc</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54658/large/SyrupUSDCO.png?1748850129</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="n">
+        <v>924795748</v>
+      </c>
+      <c r="F101" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G101" t="n">
+        <v>-0.0460048104494</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.041372400634743</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0.4724804904481411</v>
+      </c>
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>dogwifhat</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>wif</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/33566/large/dogwifhat.jpg?1702499428</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>/charts/wif_chart.png</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>901941065</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.904585</v>
+      </c>
+      <c r="G102" t="n">
+        <v>1.517137268054306</v>
+      </c>
+      <c r="H102" t="n">
+        <v>19.9198995507424</v>
+      </c>
+      <c r="I102" t="n">
+        <v>-10.54919185994349</v>
+      </c>
+      <c r="J102" t="b">
+        <v>0</v>
+      </c>
+      <c r="K102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Wrapped BNB</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>wbnb</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12591/large/binance-coin-logo.png?1696512401</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>/charts/wbnb_chart.png</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>884419359</v>
+      </c>
+      <c r="F103" t="n">
+        <v>661.73</v>
+      </c>
+      <c r="G103" t="n">
+        <v>-0.215802075720544</v>
+      </c>
+      <c r="H103" t="n">
+        <v>2.470726676938155</v>
+      </c>
+      <c r="I103" t="n">
+        <v>-0.405621828180371</v>
+      </c>
+      <c r="J103" t="b">
+        <v>0</v>
+      </c>
+      <c r="K103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Renzo Restaked ETH</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>ezeth</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/34753/large/Ezeth_logo_circle.png?1713496404</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>/charts/ezeth_chart.png</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>871517806</v>
+      </c>
+      <c r="F104" t="n">
+        <v>2728.79</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0.4474272372153331</v>
+      </c>
+      <c r="H104" t="n">
+        <v>7.104305974894171</v>
+      </c>
+      <c r="I104" t="n">
+        <v>-0.472745469733487</v>
+      </c>
+      <c r="J104" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Immutable</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>imx</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/17233/large/immutableX-symbol-BLK-RGB.png?1696516787</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>/charts/imx_chart.png</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>865865666</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.464059</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0.6293704622054971</v>
+      </c>
+      <c r="H105" t="n">
+        <v>15.68068724124131</v>
+      </c>
+      <c r="I105" t="n">
+        <v>-21.35993819296908</v>
+      </c>
+      <c r="J105" t="b">
+        <v>0</v>
+      </c>
+      <c r="K105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>The Graph</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>grt</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/13397/large/Graph_Token.png?1696513159</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>/charts/grt_chart.png</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>862423528</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.08734399999999999</v>
+      </c>
+      <c r="G106" t="n">
+        <v>-0.317923107829118</v>
+      </c>
+      <c r="H106" t="n">
+        <v>10.7127602711823</v>
+      </c>
+      <c r="I106" t="n">
+        <v>-12.05145357858769</v>
+      </c>
+      <c r="J106" t="b">
+        <v>0</v>
+      </c>
+      <c r="K106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>PayPal USD</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>pyusd</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/31212/large/PYUSD_Logo_%282%29.png?1696530039</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="n">
+        <v>860550774</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.999833</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0.006196817731039</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0.03206048656595301</v>
+      </c>
+      <c r="I107" t="n">
+        <v>0.033132497713418</v>
+      </c>
+      <c r="J107" t="b">
+        <v>0</v>
+      </c>
+      <c r="K107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>clBTC</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>clbtc</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54164/large/clBTC.png?1738482999</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="n">
+        <v>847997864</v>
+      </c>
+      <c r="F108" t="n">
+        <v>109813</v>
+      </c>
+      <c r="G108" t="n">
+        <v>-0.6040075842988011</v>
+      </c>
+      <c r="H108" t="n">
+        <v>4.19795732612783</v>
+      </c>
+      <c r="I108" t="n">
+        <v>3.210592754855558</v>
+      </c>
+      <c r="J108" t="b">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Story</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54035/large/Transparent_bg.png?1738075331</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="n">
+        <v>836269646</v>
+      </c>
+      <c r="F109" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="G109" t="n">
+        <v>-1.51677065032162</v>
+      </c>
+      <c r="H109" t="n">
+        <v>-1.378305942576083</v>
+      </c>
+      <c r="I109" t="n">
+        <v>-30.95391225794541</v>
+      </c>
+      <c r="J109" t="b">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Tether Gold</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>xaut</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/10481/large/Tether_Gold.png?1696510471</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="n">
+        <v>820361359</v>
+      </c>
+      <c r="F110" t="n">
+        <v>3327.71</v>
+      </c>
+      <c r="G110" t="n">
+        <v>-0.6529421989609181</v>
+      </c>
+      <c r="H110" t="n">
+        <v>-0.233965257406147</v>
+      </c>
+      <c r="I110" t="n">
+        <v>-0.8559408883874851</v>
+      </c>
+      <c r="J110" t="b">
+        <v>0</v>
+      </c>
+      <c r="K110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Vaulta</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55616/large/Vaulta_CEX_Icon_Circle_-_cmc.png?1746859132</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="n">
+        <v>783377155</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.497361</v>
+      </c>
+      <c r="G111" t="n">
+        <v>-0.560944488996868</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.812238342539765</v>
+      </c>
+      <c r="I111" t="n">
+        <v>-23.79567837798205</v>
+      </c>
+      <c r="J111" t="b">
+        <v>0</v>
+      </c>
+      <c r="K111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Jupiter Staked SOL</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>jupsol</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/37482/large/jupsol.png?1714473916</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="n">
+        <v>761706486</v>
+      </c>
+      <c r="F112" t="n">
+        <v>170.11</v>
+      </c>
+      <c r="G112" t="n">
+        <v>-0.900527521731026</v>
+      </c>
+      <c r="H112" t="n">
+        <v>7.413048766936116</v>
+      </c>
+      <c r="I112" t="n">
+        <v>-4.710091465596649</v>
+      </c>
+      <c r="J112" t="b">
+        <v>0</v>
+      </c>
+      <c r="K112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Marinade Staked SOL</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>msol</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/17752/large/mSOL.png?1696517278</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="n">
+        <v>753297624</v>
+      </c>
+      <c r="F113" t="n">
+        <v>198.31</v>
+      </c>
+      <c r="G113" t="n">
+        <v>-0.259626734996708</v>
+      </c>
+      <c r="H113" t="n">
+        <v>7.456483426104222</v>
+      </c>
+      <c r="I113" t="n">
+        <v>-4.6416719509699</v>
+      </c>
+      <c r="J113" t="b">
+        <v>0</v>
+      </c>
+      <c r="K113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Liquid Staked ETH</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>lseth</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/28848/large/LsETH-receipt-token-circle.png?1696527824</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="n">
+        <v>750309330</v>
+      </c>
+      <c r="F114" t="n">
+        <v>2801.68</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0.375674861583247</v>
+      </c>
+      <c r="H114" t="n">
+        <v>6.897076639062129</v>
+      </c>
+      <c r="I114" t="n">
+        <v>-0.9974912922329411</v>
+      </c>
+      <c r="J114" t="b">
+        <v>0</v>
+      </c>
+      <c r="K114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>FLOKI</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>floki</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/16746/large/PNG_image.png?1696516318</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="n">
+        <v>748337597</v>
+      </c>
+      <c r="F115" t="n">
+        <v>7.745000000000001e-05</v>
+      </c>
+      <c r="G115" t="n">
+        <v>-1.423775905710172</v>
+      </c>
+      <c r="H115" t="n">
+        <v>12.17243658571348</v>
+      </c>
+      <c r="I115" t="n">
+        <v>-11.99413656009944</v>
+      </c>
+      <c r="J115" t="b">
+        <v>0</v>
+      </c>
+      <c r="K115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>PancakeSwap</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>cake</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12632/large/pancakeswap-cake-logo_%281%29.png?1696512440</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="n">
+        <v>742426989</v>
+      </c>
+      <c r="F116" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="G116" t="n">
+        <v>-2.505064450600476</v>
+      </c>
+      <c r="H116" t="n">
+        <v>8.61544776580573</v>
+      </c>
+      <c r="I116" t="n">
+        <v>-4.60285756728105</v>
+      </c>
+      <c r="J116" t="b">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Jito</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>jto</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/33228/large/jto.png?1701137022</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="n">
+        <v>740777820</v>
+      </c>
+      <c r="F117" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.248765514258712</v>
+      </c>
+      <c r="H117" t="n">
+        <v>10.59200097913748</v>
+      </c>
+      <c r="I117" t="n">
+        <v>14.84465584220405</v>
+      </c>
+      <c r="J117" t="b">
+        <v>0</v>
+      </c>
+      <c r="K117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Curve DAO</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>crv</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12124/large/Curve.png?1696511967</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="n">
+        <v>732819849</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.535118</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0.7842574238279111</v>
+      </c>
+      <c r="H118" t="n">
+        <v>7.545302319068738</v>
+      </c>
+      <c r="I118" t="n">
+        <v>-22.94800177825459</v>
+      </c>
+      <c r="J118" t="b">
+        <v>0</v>
+      </c>
+      <c r="K118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Theta Network</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/2538/large/theta-token-logo.png?1696503349</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="n">
+        <v>716548048</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.7169719999999999</v>
+      </c>
+      <c r="G119" t="n">
+        <v>-0.363838052559835</v>
+      </c>
+      <c r="H119" t="n">
+        <v>8.769252518930209</v>
+      </c>
+      <c r="I119" t="n">
+        <v>-9.472587278947795</v>
+      </c>
+      <c r="J119" t="b">
+        <v>0</v>
+      </c>
+      <c r="K119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>OUSG</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>ousg</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/29023/large/OUSG.png?1696527993</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="n">
+        <v>709547187</v>
+      </c>
+      <c r="F120" t="n">
+        <v>111.65</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0.011080613595834</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0.07710188622960701</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0.328982893169922</v>
+      </c>
+      <c r="J120" t="b">
+        <v>0</v>
+      </c>
+      <c r="K120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Lido DAO</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>ldo</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/13573/large/Lido_DAO.png?1696513326</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="n">
+        <v>692120963</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0.772608</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0.10251078973077</v>
+      </c>
+      <c r="H121" t="n">
+        <v>13.15236436430647</v>
+      </c>
+      <c r="I121" t="n">
+        <v>-11.02243559720266</v>
+      </c>
+      <c r="J121" t="b">
+        <v>0</v>
+      </c>
+      <c r="K121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Superstate Short Duration U.S. Government Securities Fund (USTB)</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>ustb</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/35012/large/ustb.jpeg?1707102680</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="n">
+        <v>681013251</v>
+      </c>
+      <c r="F122" t="n">
+        <v>10.73</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0.011179856879205</v>
+      </c>
+      <c r="H122" t="n">
+        <v>0.077984976355118</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0.335258106868906</v>
+      </c>
+      <c r="J122" t="b">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Stables Labs USDX</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>usdx</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/50360/large/USDX200px.png?1731906044</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="n">
+        <v>672427818</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0.998745</v>
+      </c>
+      <c r="G123" t="n">
+        <v>0.027689055825637</v>
+      </c>
+      <c r="H123" t="n">
+        <v>0.04304037571289401</v>
+      </c>
+      <c r="I123" t="n">
+        <v>-0.136757934768491</v>
+      </c>
+      <c r="J123" t="b">
+        <v>0</v>
+      </c>
+      <c r="K123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>GALA</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>gala</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12493/large/GALA_token_image_-_200PNG.png?1709725869</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="n">
+        <v>665495349</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0.01476492</v>
+      </c>
+      <c r="G124" t="n">
+        <v>-0.8906971251350531</v>
+      </c>
+      <c r="H124" t="n">
+        <v>10.83331917303243</v>
+      </c>
+      <c r="I124" t="n">
+        <v>-15.09085053026243</v>
+      </c>
+      <c r="J124" t="b">
+        <v>0</v>
+      </c>
+      <c r="K124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Aerodrome Finance</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>aero</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/31745/large/token.png?1696530564</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr"/>
+      <c r="E125" t="n">
+        <v>661285549</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0.773211</v>
+      </c>
+      <c r="G125" t="n">
+        <v>-3.246732994797752</v>
+      </c>
+      <c r="H125" t="n">
+        <v>-0.816320815490978</v>
+      </c>
+      <c r="I125" t="n">
+        <v>41.49245405224639</v>
+      </c>
+      <c r="J125" t="b">
+        <v>1</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>🟢 Rendimiento mensual superior al 30%</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Zcash</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>zec</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/486/large/circle-zcash-color.png?1696501740</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="n">
+        <v>644045295</v>
+      </c>
+      <c r="F126" t="n">
+        <v>39.88</v>
+      </c>
+      <c r="G126" t="n">
+        <v>2.66662516097577</v>
+      </c>
+      <c r="H126" t="n">
+        <v>2.085575944971349</v>
+      </c>
+      <c r="I126" t="n">
+        <v>-24.78709225575369</v>
+      </c>
+      <c r="J126" t="b">
+        <v>0</v>
+      </c>
+      <c r="K126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Ethereum Name Service</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>ens</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/19785/large/ENS.jpg?1727872989</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="n">
+        <v>642978611</v>
+      </c>
+      <c r="F127" t="n">
+        <v>19.39</v>
+      </c>
+      <c r="G127" t="n">
+        <v>-0.178512202811252</v>
+      </c>
+      <c r="H127" t="n">
+        <v>5.990936382396931</v>
+      </c>
+      <c r="I127" t="n">
+        <v>-12.01198978132464</v>
+      </c>
+      <c r="J127" t="b">
+        <v>0</v>
+      </c>
+      <c r="K127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Wrapped HYPE</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>whype</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54469/large/_UP3jBsi_400x400.jpg?1739905920</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr"/>
+      <c r="E128" t="n">
+        <v>641618045</v>
+      </c>
+      <c r="F128" t="n">
+        <v>40.54</v>
+      </c>
+      <c r="G128" t="n">
+        <v>3.53321854772128</v>
+      </c>
+      <c r="H128" t="n">
+        <v>11.89403058381308</v>
+      </c>
+      <c r="I128" t="n">
+        <v>10.32845530727019</v>
+      </c>
+      <c r="J128" t="b">
+        <v>0</v>
+      </c>
+      <c r="K128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Ondo US Dollar Yield</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>usdy</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/31700/large/usdy_%281%29.png?1696530524</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="n">
+        <v>636321110</v>
+      </c>
+      <c r="F129" t="n">
+        <v>1.094</v>
+      </c>
+      <c r="G129" t="n">
+        <v>-0.003516661968156</v>
+      </c>
+      <c r="H129" t="n">
+        <v>0.55934805474961</v>
+      </c>
+      <c r="I129" t="n">
+        <v>0.291718394792253</v>
+      </c>
+      <c r="J129" t="b">
+        <v>0</v>
+      </c>
+      <c r="K129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>IOTA</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>iota</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/692/large/IOTA_Thumbnail_%281%29.png?1743772896</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr"/>
+      <c r="E130" t="n">
+        <v>629695757</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0.162898</v>
+      </c>
+      <c r="G130" t="n">
+        <v>-1.14506020037874</v>
+      </c>
+      <c r="H130" t="n">
+        <v>7.619131332112297</v>
+      </c>
+      <c r="I130" t="n">
+        <v>-14.29250112611476</v>
+      </c>
+      <c r="J130" t="b">
+        <v>0</v>
+      </c>
+      <c r="K130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>The Sandbox</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>sand</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12129/large/sandbox_logo.jpg?1696511971</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr"/>
+      <c r="E131" t="n">
+        <v>621512296</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0.254115</v>
+      </c>
+      <c r="G131" t="n">
+        <v>-0.6710463138810581</v>
+      </c>
+      <c r="H131" t="n">
+        <v>5.817146924442918</v>
+      </c>
+      <c r="I131" t="n">
+        <v>-10.70190728863598</v>
+      </c>
+      <c r="J131" t="b">
+        <v>0</v>
+      </c>
+      <c r="K131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>JasmyCoin</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>jasmy</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/13876/large/JASMY200x200.jpg?1696513620</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr"/>
+      <c r="E132" t="n">
+        <v>610555196</v>
+      </c>
+      <c r="F132" t="n">
+        <v>0.01261748</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0.53571463309804</v>
+      </c>
+      <c r="H132" t="n">
+        <v>-0.342003509163069</v>
+      </c>
+      <c r="I132" t="n">
+        <v>-17.93144710419026</v>
+      </c>
+      <c r="J132" t="b">
+        <v>0</v>
+      </c>
+      <c r="K132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>BitTorrent</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>btt</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/22457/large/btt_logo.png?1696521780</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr"/>
+      <c r="E133" t="n">
+        <v>606646077</v>
+      </c>
+      <c r="F133" t="n">
+        <v>6.152219999999999e-07</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0.339818401702815</v>
+      </c>
+      <c r="H133" t="n">
+        <v>5.113657618773733</v>
+      </c>
+      <c r="I133" t="n">
+        <v>-11.84038380620835</v>
+      </c>
+      <c r="J133" t="b">
+        <v>0</v>
+      </c>
+      <c r="K133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Solv Protocol Staked BTC</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>xsolvbtc</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39384/large/xSolvBTC.png?1744170824</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr"/>
+      <c r="E134" t="n">
+        <v>600817362</v>
+      </c>
+      <c r="F134" t="n">
+        <v>109266</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0.324547013123505</v>
+      </c>
+      <c r="H134" t="n">
+        <v>2.132196171127348</v>
+      </c>
+      <c r="I134" t="n">
+        <v>3.540209073782324</v>
+      </c>
+      <c r="J134" t="b">
+        <v>0</v>
+      </c>
+      <c r="K134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Pyth Network</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>pyth</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/31924/large/pyth.png?1701245725</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr"/>
+      <c r="E135" t="n">
+        <v>594140910</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0.103359</v>
+      </c>
+      <c r="G135" t="n">
+        <v>-0.413264895799994</v>
+      </c>
+      <c r="H135" t="n">
+        <v>14.54490467315602</v>
+      </c>
+      <c r="I135" t="n">
+        <v>-16.29308794843877</v>
+      </c>
+      <c r="J135" t="b">
+        <v>0</v>
+      </c>
+      <c r="K135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Walrus</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>wal</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54914/large/WAL_logo.png?1742494301</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="n">
+        <v>591407504</v>
+      </c>
+      <c r="F136" t="n">
+        <v>0.428358</v>
+      </c>
+      <c r="G136" t="n">
+        <v>2.109521574103647</v>
+      </c>
+      <c r="H136" t="n">
+        <v>12.27153968371148</v>
+      </c>
+      <c r="I136" t="n">
+        <v>-15.02450785457585</v>
+      </c>
+      <c r="J136" t="b">
+        <v>0</v>
+      </c>
+      <c r="K136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Usual USD</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>usd0</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/38272/large/USD0LOGO.png?1716962811</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr"/>
+      <c r="E137" t="n">
+        <v>587250382</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0.9976389999999999</v>
+      </c>
+      <c r="G137" t="n">
+        <v>-0.047490027992804</v>
+      </c>
+      <c r="H137" t="n">
+        <v>0.018061743609765</v>
+      </c>
+      <c r="I137" t="n">
+        <v>-0.014208629442008</v>
+      </c>
+      <c r="J137" t="b">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Saros</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>saros</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/34594/large/saros-token-logo.png?1705476813</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="n">
+        <v>583017324</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0.222097</v>
+      </c>
+      <c r="G138" t="n">
+        <v>-0.9840296113547461</v>
+      </c>
+      <c r="H138" t="n">
+        <v>-0.8882427944465761</v>
+      </c>
+      <c r="I138" t="n">
+        <v>11.25593167573568</v>
+      </c>
+      <c r="J138" t="b">
+        <v>0</v>
+      </c>
+      <c r="K138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Tezos</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>xtz</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/976/large/Tezos-logo.png?1696502091</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="n">
+        <v>580881333</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.553721</v>
+      </c>
+      <c r="G139" t="n">
+        <v>0.6549720326863591</v>
+      </c>
+      <c r="H139" t="n">
+        <v>6.572785674708788</v>
+      </c>
+      <c r="I139" t="n">
+        <v>-5.75363722103801</v>
+      </c>
+      <c r="J139" t="b">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Raydium</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>ray</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/13928/large/PSigc4ie_400x400.jpg?1696513668</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="n">
+        <v>580428364</v>
+      </c>
+      <c r="F140" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="G140" t="n">
+        <v>1.572331735282084</v>
+      </c>
+      <c r="H140" t="n">
+        <v>12.58347310484763</v>
+      </c>
+      <c r="I140" t="n">
+        <v>-12.82041010078382</v>
+      </c>
+      <c r="J140" t="b">
+        <v>0</v>
+      </c>
+      <c r="K140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Pendle</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>pendle</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/15069/large/Pendle_Logo_Normal-03.png?1696514728</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="n">
+        <v>578586628</v>
+      </c>
+      <c r="F141" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="G141" t="n">
+        <v>-0.897602962103848</v>
+      </c>
+      <c r="H141" t="n">
+        <v>5.410836795141299</v>
+      </c>
+      <c r="I141" t="n">
+        <v>-18.03660376374422</v>
+      </c>
+      <c r="J141" t="b">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Super OETH</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>superoeth</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39828/large/Super_OETH.png?1724208268</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="n">
+        <v>577119870</v>
+      </c>
+      <c r="F142" t="n">
+        <v>2591.14</v>
+      </c>
+      <c r="G142" t="n">
+        <v>0.482470651680607</v>
+      </c>
+      <c r="H142" t="n">
+        <v>6.93376866311213</v>
+      </c>
+      <c r="I142" t="n">
+        <v>-1.195133519969543</v>
+      </c>
+      <c r="J142" t="b">
+        <v>0</v>
+      </c>
+      <c r="K142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>tBTC</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>tbtc</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/11224/large/0x18084fba666a33d37592fa2633fd49a74dd93a88.png?1696511155</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr"/>
+      <c r="E143" t="n">
+        <v>576046393</v>
+      </c>
+      <c r="F143" t="n">
+        <v>109459</v>
+      </c>
+      <c r="G143" t="n">
+        <v>0.217928953475294</v>
+      </c>
+      <c r="H143" t="n">
+        <v>2.123615580480281</v>
+      </c>
+      <c r="I143" t="n">
+        <v>3.450990652030833</v>
+      </c>
+      <c r="J143" t="b">
+        <v>0</v>
+      </c>
+      <c r="K143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Maple Finance</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>syrup</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/51232/large/_syrup_token_logo.png?1747292046</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="n">
+        <v>575514317</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0.535905</v>
+      </c>
+      <c r="G144" t="n">
+        <v>-4.261941017426841</v>
+      </c>
+      <c r="H144" t="n">
+        <v>-11.00890582666198</v>
+      </c>
+      <c r="I144" t="n">
+        <v>20.92562740792459</v>
+      </c>
+      <c r="J144" t="b">
+        <v>0</v>
+      </c>
+      <c r="K144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Mantle Restaked ETH</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>cmeth</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/51114/large/symbol.png?1730117724</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr"/>
+      <c r="E145" t="n">
+        <v>555602261</v>
+      </c>
+      <c r="F145" t="n">
+        <v>2763.22</v>
+      </c>
+      <c r="G145" t="n">
+        <v>0.4065430904621921</v>
+      </c>
+      <c r="H145" t="n">
+        <v>6.794553248211018</v>
+      </c>
+      <c r="I145" t="n">
+        <v>-1.190735470056644</v>
+      </c>
+      <c r="J145" t="b">
+        <v>0</v>
+      </c>
+      <c r="K145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>cgETH Hashkey Cloud</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>cgeth.hashkey</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54162/large/Cgeth_Hashkey.png?1738482570</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr"/>
+      <c r="E146" t="n">
+        <v>546626167</v>
+      </c>
+      <c r="F146" t="n">
+        <v>2733.98</v>
+      </c>
+      <c r="G146" t="n">
+        <v>2.054946801074354</v>
+      </c>
+      <c r="H146" t="n">
+        <v>7.621076690833775</v>
+      </c>
+      <c r="I146" t="n">
+        <v>-0.07278821187809001</v>
+      </c>
+      <c r="J146" t="b">
+        <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Agregar Moo Deng a los datos de criptomonedas y actualizar puntajes en predicciones
</commit_message>
<xml_diff>
--- a/data/predicciones_criptos.xlsx
+++ b/data/predicciones_criptos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L288"/>
+  <dimension ref="A1:L289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,7 +576,7 @@
         <v>-1.413630270690066</v>
       </c>
       <c r="J3" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
@@ -984,7 +984,7 @@
         <v>3.310589202212904</v>
       </c>
       <c r="J13" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
@@ -1144,7 +1144,7 @@
         <v>22.08120425105527</v>
       </c>
       <c r="J17" t="n">
-        <v>0.04</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K17" t="b">
         <v>0</v>
@@ -1224,7 +1224,7 @@
         <v>2.186606821604448</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K19" t="b">
         <v>0</v>
@@ -1304,7 +1304,7 @@
         <v>-11.83220447784404</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K21" t="b">
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>39.17162961148887</v>
       </c>
       <c r="J29" t="n">
-        <v>0.08</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K29" t="b">
         <v>0</v>
@@ -2184,7 +2184,7 @@
         <v>-0.436590730021708</v>
       </c>
       <c r="J43" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K43" t="b">
         <v>0</v>
@@ -2960,7 +2960,7 @@
         <v>-23.37237596293679</v>
       </c>
       <c r="J62" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K62" t="b">
         <v>0</v>
@@ -3320,7 +3320,7 @@
         <v>-9.083725837365744</v>
       </c>
       <c r="J71" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K71" t="b">
         <v>0</v>
@@ -3440,7 +3440,7 @@
         <v>34.02739822198766</v>
       </c>
       <c r="J74" t="n">
-        <v>0.7</v>
+        <v>0.7066666666666667</v>
       </c>
       <c r="K74" t="b">
         <v>1</v>
@@ -3724,7 +3724,7 @@
         <v>-5.46076904273847</v>
       </c>
       <c r="J81" t="n">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="K81" t="b">
         <v>0</v>
@@ -3844,7 +3844,7 @@
         <v>3.4530988051059</v>
       </c>
       <c r="J84" t="n">
-        <v>0.09333333333333334</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="K84" t="b">
         <v>0</v>
@@ -3964,7 +3964,7 @@
         <v>-7.558543714704253</v>
       </c>
       <c r="J87" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K87" t="b">
         <v>0</v>
@@ -4004,7 +4004,7 @@
         <v>-29.16914736896904</v>
       </c>
       <c r="J88" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K88" t="b">
         <v>0</v>
@@ -4324,7 +4324,7 @@
         <v>40.64601967701537</v>
       </c>
       <c r="J96" t="n">
-        <v>0.76</v>
+        <v>0.8133333333333334</v>
       </c>
       <c r="K96" t="b">
         <v>1</v>
@@ -4368,7 +4368,7 @@
         <v>-1.157675008301329</v>
       </c>
       <c r="J97" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K97" t="b">
         <v>0</v>
@@ -4408,7 +4408,7 @@
         <v>40.59617452460589</v>
       </c>
       <c r="J98" t="n">
-        <v>0.2</v>
+        <v>0.1933333333333333</v>
       </c>
       <c r="K98" t="b">
         <v>0</v>
@@ -4580,7 +4580,7 @@
         <v>-10.54919185994349</v>
       </c>
       <c r="J102" t="n">
-        <v>0.02</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K102" t="b">
         <v>0</v>
@@ -5516,7 +5516,7 @@
         <v>41.49245405224639</v>
       </c>
       <c r="J125" t="n">
-        <v>0.22</v>
+        <v>0.1733333333333333</v>
       </c>
       <c r="K125" t="b">
         <v>0</v>
@@ -5556,7 +5556,7 @@
         <v>-24.78709225575369</v>
       </c>
       <c r="J126" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K126" t="b">
         <v>0</v>
@@ -5636,7 +5636,7 @@
         <v>10.32845530727019</v>
       </c>
       <c r="J128" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K128" t="b">
         <v>0</v>
@@ -5796,7 +5796,7 @@
         <v>-17.93144710419026</v>
       </c>
       <c r="J132" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K132" t="b">
         <v>0</v>
@@ -6036,7 +6036,7 @@
         <v>11.25593167573568</v>
       </c>
       <c r="J138" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K138" t="b">
         <v>0</v>
@@ -6276,7 +6276,7 @@
         <v>20.92562740792459</v>
       </c>
       <c r="J144" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="K144" t="b">
         <v>0</v>
@@ -6316,7 +6316,7 @@
         <v>-1.190735470056644</v>
       </c>
       <c r="J145" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K145" t="b">
         <v>0</v>
@@ -6568,7 +6568,7 @@
         <v>-5.36541250128957</v>
       </c>
       <c r="J151" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K151" t="b">
         <v>0</v>
@@ -6768,7 +6768,7 @@
         <v>10.33620816364243</v>
       </c>
       <c r="J156" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K156" t="b">
         <v>0</v>
@@ -7448,7 +7448,7 @@
         <v>66.6628647616337</v>
       </c>
       <c r="J173" t="n">
-        <v>0.7866666666666666</v>
+        <v>0.76</v>
       </c>
       <c r="K173" t="b">
         <v>1</v>
@@ -7532,7 +7532,7 @@
         <v>-6.442915211862388</v>
       </c>
       <c r="J175" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K175" t="b">
         <v>0</v>
@@ -8172,7 +8172,7 @@
         <v>-35.88781794455505</v>
       </c>
       <c r="J191" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K191" t="b">
         <v>0</v>
@@ -8700,7 +8700,7 @@
         <v>-4.853434536256496</v>
       </c>
       <c r="J204" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K204" t="b">
         <v>0</v>
@@ -8820,7 +8820,7 @@
         <v>-0.813922570496419</v>
       </c>
       <c r="J207" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K207" t="b">
         <v>0</v>
@@ -9100,7 +9100,7 @@
         <v>-22.68415905786022</v>
       </c>
       <c r="J214" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K214" t="b">
         <v>0</v>
@@ -9140,7 +9140,7 @@
         <v>-3.287565598806175</v>
       </c>
       <c r="J215" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K215" t="b">
         <v>0</v>
@@ -9180,7 +9180,7 @@
         <v>-4.940289975299794</v>
       </c>
       <c r="J216" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K216" t="b">
         <v>0</v>
@@ -9220,7 +9220,7 @@
         <v>3.945279934292688</v>
       </c>
       <c r="J217" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K217" t="b">
         <v>0</v>
@@ -9304,7 +9304,7 @@
         <v>0.02617310131229</v>
       </c>
       <c r="J219" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K219" t="b">
         <v>0</v>
@@ -9384,7 +9384,7 @@
         <v>-14.5006863679377</v>
       </c>
       <c r="J221" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K221" t="b">
         <v>0</v>
@@ -9824,7 +9824,7 @@
         <v>-21.8776275833068</v>
       </c>
       <c r="J232" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.02</v>
       </c>
       <c r="K232" t="b">
         <v>0</v>
@@ -9944,7 +9944,7 @@
         <v>-27.32384950826589</v>
       </c>
       <c r="J235" t="n">
-        <v>0.04666666666666667</v>
+        <v>0.06</v>
       </c>
       <c r="K235" t="b">
         <v>0</v>
@@ -10024,7 +10024,7 @@
         <v>-43.76879679502572</v>
       </c>
       <c r="J237" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.04</v>
       </c>
       <c r="K237" t="b">
         <v>0</v>
@@ -10064,7 +10064,7 @@
         <v>-2.501966759931275</v>
       </c>
       <c r="J238" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K238" t="b">
         <v>0</v>
@@ -10228,7 +10228,7 @@
         <v>-8.159484776092002</v>
       </c>
       <c r="J242" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K242" t="b">
         <v>0</v>
@@ -10428,7 +10428,7 @@
         <v>2525.507647713709</v>
       </c>
       <c r="J247" t="n">
-        <v>0.58</v>
+        <v>0.5733333333333334</v>
       </c>
       <c r="K247" t="b">
         <v>1</v>
@@ -10672,7 +10672,7 @@
         <v>-16.15281694130593</v>
       </c>
       <c r="J253" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K253" t="b">
         <v>0</v>
@@ -11032,7 +11032,7 @@
         <v>29.82231551932909</v>
       </c>
       <c r="J262" t="n">
-        <v>0.82</v>
+        <v>0.74</v>
       </c>
       <c r="K262" t="b">
         <v>1</v>
@@ -11236,7 +11236,7 @@
         <v>28.88513513513513</v>
       </c>
       <c r="J267" t="n">
-        <v>0.12</v>
+        <v>0.09333333333333334</v>
       </c>
       <c r="K267" t="b">
         <v>0</v>
@@ -11396,7 +11396,7 @@
         <v>18.71815613677644</v>
       </c>
       <c r="J271" t="n">
-        <v>0</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K271" t="b">
         <v>0</v>
@@ -11876,7 +11876,7 @@
         <v>-4.227749140768728</v>
       </c>
       <c r="J283" t="n">
-        <v>0.04666666666666667</v>
+        <v>0.02</v>
       </c>
       <c r="K283" t="b">
         <v>0</v>
@@ -12076,12 +12076,56 @@
         <v>5.559773032294486</v>
       </c>
       <c r="J288" t="n">
-        <v>0.02666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K288" t="b">
         <v>0</v>
       </c>
       <c r="L288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Moo Deng</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>moodeng</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/50264/large/MOODENG.jpg?1726726975</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>/charts/moodeng_chart.png</t>
+        </is>
+      </c>
+      <c r="E289" t="n">
+        <v>188745454</v>
+      </c>
+      <c r="F289" t="n">
+        <v>0.189982</v>
+      </c>
+      <c r="G289" t="n">
+        <v>12.6837776520067</v>
+      </c>
+      <c r="H289" t="n">
+        <v>40.4236651718855</v>
+      </c>
+      <c r="I289" t="n">
+        <v>-12.48789007620941</v>
+      </c>
+      <c r="J289" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K289" t="b">
+        <v>0</v>
+      </c>
+      <c r="L289" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: Update cryptocurrency predictions and recommendations
- Modified existing cryptocurrency predictions in `criptos_predichas.json` with updated scores and reasons.
- Added new cryptocurrencies with detailed predictions and reasons.
- Introduced a new image file `proyeccion.png` for visual representation.
- Created a new recommendations JSON file `recomendaciones.json` with detailed investment suggestions.
- Added a new text file `ultima_pagina.txt` to track pagination.
- Implemented `extractor.py` script to fetch and store cryptocurrency data from the CoinGecko API.
- Developed `modelo_general.py` for training a Random Forest model to predict cryptocurrency performance.
- Created `modelo_portafolio.py` for generating investment portfolio recommendations based on user-defined parameters.
</commit_message>
<xml_diff>
--- a/data/predicciones_criptos.xlsx
+++ b/data/predicciones_criptos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L289"/>
+  <dimension ref="A1:L384"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,7 +576,7 @@
         <v>-1.413630270690066</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
@@ -1144,7 +1144,7 @@
         <v>22.08120425105527</v>
       </c>
       <c r="J17" t="n">
-        <v>0.05333333333333334</v>
+        <v>0.1066666666666667</v>
       </c>
       <c r="K17" t="b">
         <v>0</v>
@@ -1304,7 +1304,7 @@
         <v>-11.83220447784404</v>
       </c>
       <c r="J21" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K21" t="b">
         <v>0</v>
@@ -1384,7 +1384,7 @@
         <v>-10.71042061533567</v>
       </c>
       <c r="J23" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K23" t="b">
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>39.17162961148887</v>
       </c>
       <c r="J29" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.04</v>
       </c>
       <c r="K29" t="b">
         <v>0</v>
@@ -2184,7 +2184,7 @@
         <v>-0.436590730021708</v>
       </c>
       <c r="J43" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K43" t="b">
         <v>0</v>
@@ -2224,7 +2224,7 @@
         <v>-14.88173006709638</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K44" t="b">
         <v>0</v>
@@ -2636,7 +2636,7 @@
         <v>-13.60086853440658</v>
       </c>
       <c r="J54" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K54" t="b">
         <v>0</v>
@@ -2756,7 +2756,7 @@
         <v>-19.01774212095845</v>
       </c>
       <c r="J57" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K57" t="b">
         <v>0</v>
@@ -3040,7 +3040,7 @@
         <v>3.672065484066418</v>
       </c>
       <c r="J64" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K64" t="b">
         <v>0</v>
@@ -3280,7 +3280,7 @@
         <v>-22.95847335923886</v>
       </c>
       <c r="J70" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K70" t="b">
         <v>0</v>
@@ -3440,14 +3440,14 @@
         <v>34.02739822198766</v>
       </c>
       <c r="J74" t="n">
-        <v>0.7066666666666667</v>
+        <v>0.76</v>
       </c>
       <c r="K74" t="b">
         <v>1</v>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Rendimiento mensual superior al 30</t>
+          <t>Buen rendimiento mensual (+30%) | Buena puntuacion en analisis multivariable</t>
         </is>
       </c>
     </row>
@@ -3484,7 +3484,7 @@
         <v>-0.002877455154935</v>
       </c>
       <c r="J75" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K75" t="b">
         <v>0</v>
@@ -3524,7 +3524,7 @@
         <v>-0.035522872151087</v>
       </c>
       <c r="J76" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K76" t="b">
         <v>0</v>
@@ -3724,7 +3724,7 @@
         <v>-5.46076904273847</v>
       </c>
       <c r="J81" t="n">
-        <v>0.04</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K81" t="b">
         <v>0</v>
@@ -3844,7 +3844,7 @@
         <v>3.4530988051059</v>
       </c>
       <c r="J84" t="n">
-        <v>0.07333333333333333</v>
+        <v>0.09333333333333334</v>
       </c>
       <c r="K84" t="b">
         <v>0</v>
@@ -3964,7 +3964,7 @@
         <v>-7.558543714704253</v>
       </c>
       <c r="J87" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K87" t="b">
         <v>0</v>
@@ -4004,7 +4004,7 @@
         <v>-29.16914736896904</v>
       </c>
       <c r="J88" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K88" t="b">
         <v>0</v>
@@ -4164,7 +4164,7 @@
         <v>-20.73487845027156</v>
       </c>
       <c r="J92" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K92" t="b">
         <v>0</v>
@@ -4204,7 +4204,7 @@
         <v>-16.34997855450167</v>
       </c>
       <c r="J93" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K93" t="b">
         <v>0</v>
@@ -4244,7 +4244,7 @@
         <v>-1.190710980089554</v>
       </c>
       <c r="J94" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K94" t="b">
         <v>0</v>
@@ -4284,7 +4284,7 @@
         <v>-0.021382708202666</v>
       </c>
       <c r="J95" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K95" t="b">
         <v>0</v>
@@ -4324,14 +4324,14 @@
         <v>40.64601967701537</v>
       </c>
       <c r="J96" t="n">
-        <v>0.8133333333333334</v>
+        <v>0.8066666666666666</v>
       </c>
       <c r="K96" t="b">
         <v>1</v>
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>Rendimiento mensual superior al 30 | Tendencia semanal positiva</t>
+          <t>Buen rendimiento mensual (+30%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
         </is>
       </c>
     </row>
@@ -4368,7 +4368,7 @@
         <v>-1.157675008301329</v>
       </c>
       <c r="J97" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K97" t="b">
         <v>0</v>
@@ -4408,7 +4408,7 @@
         <v>40.59617452460589</v>
       </c>
       <c r="J98" t="n">
-        <v>0.1933333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="K98" t="b">
         <v>0</v>
@@ -4580,7 +4580,7 @@
         <v>-10.54919185994349</v>
       </c>
       <c r="J102" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K102" t="b">
         <v>0</v>
@@ -5156,7 +5156,7 @@
         <v>-4.60285756728105</v>
       </c>
       <c r="J116" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K116" t="b">
         <v>0</v>
@@ -5356,7 +5356,7 @@
         <v>-11.02243559720266</v>
       </c>
       <c r="J121" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K121" t="b">
         <v>0</v>
@@ -5396,7 +5396,7 @@
         <v>0.335258106868906</v>
       </c>
       <c r="J122" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K122" t="b">
         <v>0</v>
@@ -5516,7 +5516,7 @@
         <v>41.49245405224639</v>
       </c>
       <c r="J125" t="n">
-        <v>0.1733333333333333</v>
+        <v>0.08666666666666667</v>
       </c>
       <c r="K125" t="b">
         <v>0</v>
@@ -5556,7 +5556,7 @@
         <v>-24.78709225575369</v>
       </c>
       <c r="J126" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K126" t="b">
         <v>0</v>
@@ -5636,7 +5636,7 @@
         <v>10.32845530727019</v>
       </c>
       <c r="J128" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K128" t="b">
         <v>0</v>
@@ -5796,7 +5796,7 @@
         <v>-17.93144710419026</v>
       </c>
       <c r="J132" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K132" t="b">
         <v>0</v>
@@ -6036,7 +6036,7 @@
         <v>11.25593167573568</v>
       </c>
       <c r="J138" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K138" t="b">
         <v>0</v>
@@ -6276,7 +6276,7 @@
         <v>20.92562740792459</v>
       </c>
       <c r="J144" t="n">
-        <v>0.07333333333333333</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K144" t="b">
         <v>0</v>
@@ -6316,7 +6316,7 @@
         <v>-1.190735470056644</v>
       </c>
       <c r="J145" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K145" t="b">
         <v>0</v>
@@ -6568,7 +6568,7 @@
         <v>-5.36541250128957</v>
       </c>
       <c r="J151" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K151" t="b">
         <v>0</v>
@@ -6768,7 +6768,7 @@
         <v>10.33620816364243</v>
       </c>
       <c r="J156" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K156" t="b">
         <v>0</v>
@@ -7448,14 +7448,14 @@
         <v>66.6628647616337</v>
       </c>
       <c r="J173" t="n">
-        <v>0.76</v>
+        <v>0.52</v>
       </c>
       <c r="K173" t="b">
         <v>1</v>
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>Crecimiento mensual superior al 60 | Tendencia semanal positiva</t>
+          <t>Crecimiento mensual sobresaliente (+60%) | Fuerte tendencia semanal (+10%)</t>
         </is>
       </c>
     </row>
@@ -7492,7 +7492,7 @@
         <v>5.317709580767196</v>
       </c>
       <c r="J174" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K174" t="b">
         <v>0</v>
@@ -8052,7 +8052,7 @@
         <v>-2.090806463705334</v>
       </c>
       <c r="J188" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K188" t="b">
         <v>0</v>
@@ -8172,7 +8172,7 @@
         <v>-35.88781794455505</v>
       </c>
       <c r="J191" t="n">
-        <v>0.05333333333333334</v>
+        <v>0.02</v>
       </c>
       <c r="K191" t="b">
         <v>0</v>
@@ -8212,7 +8212,7 @@
         <v>-24.11678545003828</v>
       </c>
       <c r="J192" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K192" t="b">
         <v>0</v>
@@ -8252,7 +8252,7 @@
         <v>-12.26553879250178</v>
       </c>
       <c r="J193" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K193" t="b">
         <v>0</v>
@@ -8540,7 +8540,7 @@
         <v>1.046832409288845</v>
       </c>
       <c r="J200" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K200" t="b">
         <v>0</v>
@@ -8620,7 +8620,7 @@
         <v>-7.532973615214416</v>
       </c>
       <c r="J202" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K202" t="b">
         <v>0</v>
@@ -8660,7 +8660,7 @@
         <v>-15.68666441754651</v>
       </c>
       <c r="J203" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K203" t="b">
         <v>0</v>
@@ -8700,7 +8700,7 @@
         <v>-4.853434536256496</v>
       </c>
       <c r="J204" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K204" t="b">
         <v>0</v>
@@ -8740,7 +8740,7 @@
         <v>-14.9165130167515</v>
       </c>
       <c r="J205" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K205" t="b">
         <v>0</v>
@@ -8820,7 +8820,7 @@
         <v>-0.813922570496419</v>
       </c>
       <c r="J207" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K207" t="b">
         <v>0</v>
@@ -9100,7 +9100,7 @@
         <v>-22.68415905786022</v>
       </c>
       <c r="J214" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="K214" t="b">
         <v>0</v>
@@ -9180,7 +9180,7 @@
         <v>-4.940289975299794</v>
       </c>
       <c r="J216" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K216" t="b">
         <v>0</v>
@@ -9260,14 +9260,14 @@
         <v>26.22562127291115</v>
       </c>
       <c r="J218" t="n">
-        <v>0.6333333333333333</v>
+        <v>0.6533333333333333</v>
       </c>
       <c r="K218" t="b">
         <v>1</v>
       </c>
       <c r="L218" t="inlineStr">
         <is>
-          <t>Recomendacion por analisis multivariable</t>
+          <t>Buena puntuacion en analisis multivariable</t>
         </is>
       </c>
     </row>
@@ -9304,7 +9304,7 @@
         <v>0.02617310131229</v>
       </c>
       <c r="J219" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K219" t="b">
         <v>0</v>
@@ -9344,7 +9344,7 @@
         <v>-11.54370801710428</v>
       </c>
       <c r="J220" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K220" t="b">
         <v>0</v>
@@ -9384,7 +9384,7 @@
         <v>-14.5006863679377</v>
       </c>
       <c r="J221" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K221" t="b">
         <v>0</v>
@@ -9424,7 +9424,7 @@
         <v>-13.46085981617814</v>
       </c>
       <c r="J222" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K222" t="b">
         <v>0</v>
@@ -9464,7 +9464,7 @@
         <v>3.561986898496721</v>
       </c>
       <c r="J223" t="n">
-        <v>0</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K223" t="b">
         <v>0</v>
@@ -9504,7 +9504,7 @@
         <v>-0.4917969429396941</v>
       </c>
       <c r="J224" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K224" t="b">
         <v>0</v>
@@ -9744,7 +9744,7 @@
         <v>3.497110880270336</v>
       </c>
       <c r="J230" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K230" t="b">
         <v>0</v>
@@ -9824,7 +9824,7 @@
         <v>-21.8776275833068</v>
       </c>
       <c r="J232" t="n">
-        <v>0.02</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K232" t="b">
         <v>0</v>
@@ -9944,7 +9944,7 @@
         <v>-27.32384950826589</v>
       </c>
       <c r="J235" t="n">
-        <v>0.06</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K235" t="b">
         <v>0</v>
@@ -10024,7 +10024,7 @@
         <v>-43.76879679502572</v>
       </c>
       <c r="J237" t="n">
-        <v>0.04</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K237" t="b">
         <v>0</v>
@@ -10064,7 +10064,7 @@
         <v>-2.501966759931275</v>
       </c>
       <c r="J238" t="n">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K238" t="b">
         <v>0</v>
@@ -10228,7 +10228,7 @@
         <v>-8.159484776092002</v>
       </c>
       <c r="J242" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K242" t="b">
         <v>0</v>
@@ -10428,14 +10428,14 @@
         <v>2525.507647713709</v>
       </c>
       <c r="J247" t="n">
-        <v>0.5733333333333334</v>
+        <v>0.8133333333333334</v>
       </c>
       <c r="K247" t="b">
         <v>1</v>
       </c>
       <c r="L247" t="inlineStr">
         <is>
-          <t>Crecimiento mensual superior al 60 | Tendencia semanal positiva</t>
+          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
         </is>
       </c>
     </row>
@@ -10672,7 +10672,7 @@
         <v>-16.15281694130593</v>
       </c>
       <c r="J253" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K253" t="b">
         <v>0</v>
@@ -10952,7 +10952,7 @@
         <v>0.0008543484464590001</v>
       </c>
       <c r="J260" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K260" t="b">
         <v>0</v>
@@ -10992,7 +10992,7 @@
         <v>-2.31383761637606</v>
       </c>
       <c r="J261" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K261" t="b">
         <v>0</v>
@@ -11032,14 +11032,14 @@
         <v>29.82231551932909</v>
       </c>
       <c r="J262" t="n">
-        <v>0.74</v>
+        <v>0.86</v>
       </c>
       <c r="K262" t="b">
         <v>1</v>
       </c>
       <c r="L262" t="inlineStr">
         <is>
-          <t>Tendencia semanal positiva</t>
+          <t>Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
         </is>
       </c>
     </row>
@@ -11076,7 +11076,7 @@
         <v>-6.86437034928737</v>
       </c>
       <c r="J263" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K263" t="b">
         <v>0</v>
@@ -11116,7 +11116,7 @@
         <v>-14.56847243700389</v>
       </c>
       <c r="J264" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K264" t="b">
         <v>0</v>
@@ -11156,7 +11156,7 @@
         <v>-19.0911853939931</v>
       </c>
       <c r="J265" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K265" t="b">
         <v>0</v>
@@ -11236,7 +11236,7 @@
         <v>28.88513513513513</v>
       </c>
       <c r="J267" t="n">
-        <v>0.09333333333333334</v>
+        <v>0.06</v>
       </c>
       <c r="K267" t="b">
         <v>0</v>
@@ -11276,7 +11276,7 @@
         <v>-33.35010980697314</v>
       </c>
       <c r="J268" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K268" t="b">
         <v>0</v>
@@ -11316,7 +11316,7 @@
         <v>-7.061042783279207</v>
       </c>
       <c r="J269" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K269" t="b">
         <v>0</v>
@@ -11396,7 +11396,7 @@
         <v>18.71815613677644</v>
       </c>
       <c r="J271" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.06</v>
       </c>
       <c r="K271" t="b">
         <v>0</v>
@@ -11476,7 +11476,7 @@
         <v>-17.97829771807034</v>
       </c>
       <c r="J273" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K273" t="b">
         <v>0</v>
@@ -11556,7 +11556,7 @@
         <v>-18.32687472125039</v>
       </c>
       <c r="J275" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K275" t="b">
         <v>0</v>
@@ -11676,7 +11676,7 @@
         <v>-12.35924248375612</v>
       </c>
       <c r="J278" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K278" t="b">
         <v>0</v>
@@ -11876,7 +11876,7 @@
         <v>-4.227749140768728</v>
       </c>
       <c r="J283" t="n">
-        <v>0.02</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K283" t="b">
         <v>0</v>
@@ -11956,7 +11956,7 @@
         <v>-16.00654861182379</v>
       </c>
       <c r="J285" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K285" t="b">
         <v>0</v>
@@ -12076,7 +12076,7 @@
         <v>5.559773032294486</v>
       </c>
       <c r="J288" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K288" t="b">
         <v>0</v>
@@ -12120,12 +12120,3872 @@
         <v>-12.48789007620941</v>
       </c>
       <c r="J289" t="n">
-        <v>0.08</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K289" t="b">
         <v>0</v>
       </c>
       <c r="L289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>WEMIX</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>wemix</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12998/large/wemixcoin_color_200.png?1696512788</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr"/>
+      <c r="E290" t="n">
+        <v>185559861</v>
+      </c>
+      <c r="F290" t="n">
+        <v>0.409828</v>
+      </c>
+      <c r="G290" t="n">
+        <v>-4.074858309121512</v>
+      </c>
+      <c r="H290" t="n">
+        <v>8.525242184137417</v>
+      </c>
+      <c r="I290" t="n">
+        <v>-1.129843369938731</v>
+      </c>
+      <c r="J290" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K290" t="b">
+        <v>0</v>
+      </c>
+      <c r="L290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>GoMining Token</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>gomining</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/15662/large/GoMining_Logo.png?1714757256</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>/charts/gomining_chart.png</t>
+        </is>
+      </c>
+      <c r="E291" t="n">
+        <v>173556334</v>
+      </c>
+      <c r="F291" t="n">
+        <v>0.426237</v>
+      </c>
+      <c r="G291" t="n">
+        <v>0.330268659792173</v>
+      </c>
+      <c r="H291" t="n">
+        <v>0.839172278745255</v>
+      </c>
+      <c r="I291" t="n">
+        <v>0.477208580444714</v>
+      </c>
+      <c r="J291" t="n">
+        <v>0</v>
+      </c>
+      <c r="K291" t="b">
+        <v>0</v>
+      </c>
+      <c r="L291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Tribe</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>tribe</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/14575/large/tribe.PNG?1696514256</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>/charts/tribe_chart.png</t>
+        </is>
+      </c>
+      <c r="E292" t="n">
+        <v>172810499</v>
+      </c>
+      <c r="F292" t="n">
+        <v>0.378956</v>
+      </c>
+      <c r="G292" t="n">
+        <v>1.072489896337324</v>
+      </c>
+      <c r="H292" t="n">
+        <v>0.4329803423174861</v>
+      </c>
+      <c r="I292" t="n">
+        <v>-6.855098801741073</v>
+      </c>
+      <c r="J292" t="n">
+        <v>0</v>
+      </c>
+      <c r="K292" t="b">
+        <v>0</v>
+      </c>
+      <c r="L292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>yearn.finance</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>yfi</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/11849/large/yearn.jpg?1696511720</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>/charts/yfi_chart.png</t>
+        </is>
+      </c>
+      <c r="E293" t="n">
+        <v>171813237</v>
+      </c>
+      <c r="F293" t="n">
+        <v>5084.35</v>
+      </c>
+      <c r="G293" t="n">
+        <v>-2.567881858139967</v>
+      </c>
+      <c r="H293" t="n">
+        <v>-0.9313022698150201</v>
+      </c>
+      <c r="I293" t="n">
+        <v>-3.233286290414927</v>
+      </c>
+      <c r="J293" t="n">
+        <v>0</v>
+      </c>
+      <c r="K293" t="b">
+        <v>0</v>
+      </c>
+      <c r="L293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Verus</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>vrsc</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/6769/large/Screenshot_33.png?1696507103</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr"/>
+      <c r="E294" t="n">
+        <v>171688399</v>
+      </c>
+      <c r="F294" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="G294" t="n">
+        <v>-3.115551402275422</v>
+      </c>
+      <c r="H294" t="n">
+        <v>-1.605995396509903</v>
+      </c>
+      <c r="I294" t="n">
+        <v>-13.98363746428585</v>
+      </c>
+      <c r="J294" t="n">
+        <v>0</v>
+      </c>
+      <c r="K294" t="b">
+        <v>0</v>
+      </c>
+      <c r="L294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>VeThor</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>vtho</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/5230/large/VETHO.png?1742383301</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr"/>
+      <c r="E295" t="n">
+        <v>171043911</v>
+      </c>
+      <c r="F295" t="n">
+        <v>0.00187141</v>
+      </c>
+      <c r="G295" t="n">
+        <v>-2.195481153753927</v>
+      </c>
+      <c r="H295" t="n">
+        <v>-3.599888404608408</v>
+      </c>
+      <c r="I295" t="n">
+        <v>-11.52695523853806</v>
+      </c>
+      <c r="J295" t="n">
+        <v>0</v>
+      </c>
+      <c r="K295" t="b">
+        <v>0</v>
+      </c>
+      <c r="L295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Aster Staked BNB</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>asbnb</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54129/large/asBNB.png?1744789305</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr"/>
+      <c r="E296" t="n">
+        <v>168050967</v>
+      </c>
+      <c r="F296" t="n">
+        <v>683.63</v>
+      </c>
+      <c r="G296" t="n">
+        <v>-0.6216099566378051</v>
+      </c>
+      <c r="H296" t="n">
+        <v>0.543031744860314</v>
+      </c>
+      <c r="I296" t="n">
+        <v>-0.756420963240059</v>
+      </c>
+      <c r="J296" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K296" t="b">
+        <v>0</v>
+      </c>
+      <c r="L296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Blur</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>blur</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/28453/large/blur.png?1696527448</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr"/>
+      <c r="E297" t="n">
+        <v>166274431</v>
+      </c>
+      <c r="F297" t="n">
+        <v>0.068939</v>
+      </c>
+      <c r="G297" t="n">
+        <v>-2.774499539906756</v>
+      </c>
+      <c r="H297" t="n">
+        <v>-3.430576857333929</v>
+      </c>
+      <c r="I297" t="n">
+        <v>-21.41862298043247</v>
+      </c>
+      <c r="J297" t="n">
+        <v>0</v>
+      </c>
+      <c r="K297" t="b">
+        <v>0</v>
+      </c>
+      <c r="L297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Siacoin</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>sc</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/289/large/siacoin.png?1696501638</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr"/>
+      <c r="E298" t="n">
+        <v>165574678</v>
+      </c>
+      <c r="F298" t="n">
+        <v>0.00295574</v>
+      </c>
+      <c r="G298" t="n">
+        <v>-1.217426611143195</v>
+      </c>
+      <c r="H298" t="n">
+        <v>1.439606322154472</v>
+      </c>
+      <c r="I298" t="n">
+        <v>-9.803630780273743</v>
+      </c>
+      <c r="J298" t="n">
+        <v>0</v>
+      </c>
+      <c r="K298" t="b">
+        <v>0</v>
+      </c>
+      <c r="L298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Elixir deUSD</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>deusd</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39494/large/deUSD_Logo_%281%29.png?1723689002</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr"/>
+      <c r="E299" t="n">
+        <v>164889411</v>
+      </c>
+      <c r="F299" t="n">
+        <v>0.999976</v>
+      </c>
+      <c r="G299" t="n">
+        <v>0.004379949435302</v>
+      </c>
+      <c r="H299" t="n">
+        <v>0.07610912182964301</v>
+      </c>
+      <c r="I299" t="n">
+        <v>0.026114110530444</v>
+      </c>
+      <c r="J299" t="n">
+        <v>0</v>
+      </c>
+      <c r="K299" t="b">
+        <v>0</v>
+      </c>
+      <c r="L299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>OriginTrail</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>trac</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/1877/large/TRAC.jpg?1696502873</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr"/>
+      <c r="E300" t="n">
+        <v>164831931</v>
+      </c>
+      <c r="F300" t="n">
+        <v>0.329964</v>
+      </c>
+      <c r="G300" t="n">
+        <v>1.114455360110832</v>
+      </c>
+      <c r="H300" t="n">
+        <v>2.093108781475263</v>
+      </c>
+      <c r="I300" t="n">
+        <v>-14.1267229746276</v>
+      </c>
+      <c r="J300" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K300" t="b">
+        <v>0</v>
+      </c>
+      <c r="L300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>ai16z</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>ai16z</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/51090/large/AI16Z.jpg?1730027175</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr"/>
+      <c r="E301" t="n">
+        <v>164059630</v>
+      </c>
+      <c r="F301" t="n">
+        <v>0.149301</v>
+      </c>
+      <c r="G301" t="n">
+        <v>-4.461143143977305</v>
+      </c>
+      <c r="H301" t="n">
+        <v>-4.328120041396573</v>
+      </c>
+      <c r="I301" t="n">
+        <v>-30.79976552723882</v>
+      </c>
+      <c r="J301" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K301" t="b">
+        <v>0</v>
+      </c>
+      <c r="L301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>MimboGameGroup</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>mgg</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/66393/large/mimbo.jpg?1749367847</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr"/>
+      <c r="E302" t="n">
+        <v>163868562</v>
+      </c>
+      <c r="F302" t="n">
+        <v>0.00142995</v>
+      </c>
+      <c r="G302" t="n">
+        <v>-0.29810477188049</v>
+      </c>
+      <c r="H302" t="n">
+        <v>4.753293726069501</v>
+      </c>
+      <c r="I302" t="n">
+        <v>21.18961591278832</v>
+      </c>
+      <c r="J302" t="n">
+        <v>0.4066666666666667</v>
+      </c>
+      <c r="K302" t="b">
+        <v>1</v>
+      </c>
+      <c r="L302" t="inlineStr">
+        <is>
+          <t>Recomendacion por analisis multivariable</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Celo</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>celo</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/11090/large/InjXBNx9_400x400.jpg?1696511031</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr"/>
+      <c r="E303" t="n">
+        <v>163834584</v>
+      </c>
+      <c r="F303" t="n">
+        <v>0.285304</v>
+      </c>
+      <c r="G303" t="n">
+        <v>4.503680001612967</v>
+      </c>
+      <c r="H303" t="n">
+        <v>9.239199423787975</v>
+      </c>
+      <c r="I303" t="n">
+        <v>-8.65285976745222</v>
+      </c>
+      <c r="J303" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="K303" t="b">
+        <v>0</v>
+      </c>
+      <c r="L303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>KOGE</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>koge</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/13827/large/bnb48.png?1696513570</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr"/>
+      <c r="E304" t="n">
+        <v>162576242</v>
+      </c>
+      <c r="F304" t="n">
+        <v>47.98</v>
+      </c>
+      <c r="G304" t="n">
+        <v>-0.278688018973484</v>
+      </c>
+      <c r="H304" t="n">
+        <v>-0.071940739560775</v>
+      </c>
+      <c r="I304" t="n">
+        <v>-24.41997290272294</v>
+      </c>
+      <c r="J304" t="n">
+        <v>0</v>
+      </c>
+      <c r="K304" t="b">
+        <v>0</v>
+      </c>
+      <c r="L304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>ZetaChain</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>zeta</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/26718/large/Twitter_icon.png?1696525788</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr"/>
+      <c r="E305" t="n">
+        <v>161708649</v>
+      </c>
+      <c r="F305" t="n">
+        <v>0.174827</v>
+      </c>
+      <c r="G305" t="n">
+        <v>-1.784245873844842</v>
+      </c>
+      <c r="H305" t="n">
+        <v>-0.8613007897986761</v>
+      </c>
+      <c r="I305" t="n">
+        <v>-17.54381302839132</v>
+      </c>
+      <c r="J305" t="n">
+        <v>0</v>
+      </c>
+      <c r="K305" t="b">
+        <v>0</v>
+      </c>
+      <c r="L305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Nervos Network</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>ckb</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/9566/large/Nervos_White.png?1696509646</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr"/>
+      <c r="E306" t="n">
+        <v>161257757</v>
+      </c>
+      <c r="F306" t="n">
+        <v>0.00344303</v>
+      </c>
+      <c r="G306" t="n">
+        <v>-2.18474340691503</v>
+      </c>
+      <c r="H306" t="n">
+        <v>0.710715206254076</v>
+      </c>
+      <c r="I306" t="n">
+        <v>-15.16888882484637</v>
+      </c>
+      <c r="J306" t="n">
+        <v>0</v>
+      </c>
+      <c r="K306" t="b">
+        <v>0</v>
+      </c>
+      <c r="L306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Aave USDC (Sonic)</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>asonusdc</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55659/large/aSonUSDC_200x200.png?1746866473</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr"/>
+      <c r="E307" t="n">
+        <v>159691061</v>
+      </c>
+      <c r="F307" t="n">
+        <v>0.999691</v>
+      </c>
+      <c r="G307" t="n">
+        <v>-0.031596365228788</v>
+      </c>
+      <c r="H307" t="n">
+        <v>-0.011687185412838</v>
+      </c>
+      <c r="I307" t="n">
+        <v>-0.02777123232285</v>
+      </c>
+      <c r="J307" t="n">
+        <v>0</v>
+      </c>
+      <c r="K307" t="b">
+        <v>0</v>
+      </c>
+      <c r="L307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Steakhouse USDC Morpho Vault</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>steakusdc</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/51473/large/steakUSDC.png?1731396462</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr"/>
+      <c r="E308" t="n">
+        <v>158831815</v>
+      </c>
+      <c r="F308" t="n">
+        <v>1.091</v>
+      </c>
+      <c r="G308" t="n">
+        <v>0.012734817960278</v>
+      </c>
+      <c r="H308" t="n">
+        <v>0.059582168070502</v>
+      </c>
+      <c r="I308" t="n">
+        <v>0.330852639830966</v>
+      </c>
+      <c r="J308" t="n">
+        <v>0</v>
+      </c>
+      <c r="K308" t="b">
+        <v>0</v>
+      </c>
+      <c r="L308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Wrapped fragSOL</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>wfragsol</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54574/large/wfragSOL.png?1740494202</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr"/>
+      <c r="E309" t="n">
+        <v>158416336</v>
+      </c>
+      <c r="F309" t="n">
+        <v>156.97</v>
+      </c>
+      <c r="G309" t="n">
+        <v>-2.228924229766797</v>
+      </c>
+      <c r="H309" t="n">
+        <v>-4.00732123105914</v>
+      </c>
+      <c r="I309" t="n">
+        <v>-1.299814162685677</v>
+      </c>
+      <c r="J309" t="n">
+        <v>0</v>
+      </c>
+      <c r="K309" t="b">
+        <v>0</v>
+      </c>
+      <c r="L309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>ORDI</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>ordi</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/30162/large/ordi.png?1696529082</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr"/>
+      <c r="E310" t="n">
+        <v>156279059</v>
+      </c>
+      <c r="F310" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="G310" t="n">
+        <v>-2.666208340237463</v>
+      </c>
+      <c r="H310" t="n">
+        <v>-0.397118645190299</v>
+      </c>
+      <c r="I310" t="n">
+        <v>-12.79945679381139</v>
+      </c>
+      <c r="J310" t="n">
+        <v>0</v>
+      </c>
+      <c r="K310" t="b">
+        <v>0</v>
+      </c>
+      <c r="L310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Threshold Network</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/22228/large/nFPNiSbL_400x400.jpg?1696521570</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr"/>
+      <c r="E311" t="n">
+        <v>155620775</v>
+      </c>
+      <c r="F311" t="n">
+        <v>0.01538858</v>
+      </c>
+      <c r="G311" t="n">
+        <v>-1.400888891943648</v>
+      </c>
+      <c r="H311" t="n">
+        <v>-9.628363676819511</v>
+      </c>
+      <c r="I311" t="n">
+        <v>4.392008408060252</v>
+      </c>
+      <c r="J311" t="n">
+        <v>0</v>
+      </c>
+      <c r="K311" t="b">
+        <v>0</v>
+      </c>
+      <c r="L311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Qubic</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>qubic</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/32949/large/QubicLogo-Token.png?1731185925</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr"/>
+      <c r="E312" t="n">
+        <v>155588831</v>
+      </c>
+      <c r="F312" t="n">
+        <v>1.3e-06</v>
+      </c>
+      <c r="G312" t="n">
+        <v>-3.367959441288828</v>
+      </c>
+      <c r="H312" t="n">
+        <v>-6.443663224406889</v>
+      </c>
+      <c r="I312" t="n">
+        <v>-9.269192371854864</v>
+      </c>
+      <c r="J312" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K312" t="b">
+        <v>0</v>
+      </c>
+      <c r="L312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Sologenic</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>solo</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/10771/large/solo.png?1696510734</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr"/>
+      <c r="E313" t="n">
+        <v>154156944</v>
+      </c>
+      <c r="F313" t="n">
+        <v>0.388828</v>
+      </c>
+      <c r="G313" t="n">
+        <v>30.55373104629811</v>
+      </c>
+      <c r="H313" t="n">
+        <v>53.02750692547342</v>
+      </c>
+      <c r="I313" t="n">
+        <v>57.46227086244219</v>
+      </c>
+      <c r="J313" t="n">
+        <v>0.8866666666666667</v>
+      </c>
+      <c r="K313" t="b">
+        <v>1</v>
+      </c>
+      <c r="L313" t="inlineStr">
+        <is>
+          <t>Buen rendimiento mensual (+30%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Kinesis Gold</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>kau</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/29788/large/kau-currency-ticker.png?1696528718</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr"/>
+      <c r="E314" t="n">
+        <v>154085058</v>
+      </c>
+      <c r="F314" t="n">
+        <v>107.23</v>
+      </c>
+      <c r="G314" t="n">
+        <v>-0.110488944025881</v>
+      </c>
+      <c r="H314" t="n">
+        <v>0.727584017234675</v>
+      </c>
+      <c r="I314" t="n">
+        <v>0.116753765151209</v>
+      </c>
+      <c r="J314" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K314" t="b">
+        <v>0</v>
+      </c>
+      <c r="L314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Fluid</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>fluid</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/14688/large/Logo_1_%28brighter%29.png?1734430693</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr"/>
+      <c r="E315" t="n">
+        <v>153275256</v>
+      </c>
+      <c r="F315" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="G315" t="n">
+        <v>-1.494363409187427</v>
+      </c>
+      <c r="H315" t="n">
+        <v>-2.506440709762445</v>
+      </c>
+      <c r="I315" t="n">
+        <v>-2.172282440318701</v>
+      </c>
+      <c r="J315" t="n">
+        <v>0</v>
+      </c>
+      <c r="K315" t="b">
+        <v>0</v>
+      </c>
+      <c r="L315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Banana For Scale</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>bananas31</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52230/large/Banana_token_image.png?1732801941</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr"/>
+      <c r="E316" t="n">
+        <v>152067331</v>
+      </c>
+      <c r="F316" t="n">
+        <v>0.01521073</v>
+      </c>
+      <c r="G316" t="n">
+        <v>-4.285533828526153</v>
+      </c>
+      <c r="H316" t="n">
+        <v>21.27925790625024</v>
+      </c>
+      <c r="I316" t="n">
+        <v>159.2683749555226</v>
+      </c>
+      <c r="J316" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="K316" t="b">
+        <v>1</v>
+      </c>
+      <c r="L316" t="inlineStr">
+        <is>
+          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>UXLINK</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>uxlink</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39229/large/uxlink.jpg?1721201390</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr"/>
+      <c r="E317" t="n">
+        <v>151645230</v>
+      </c>
+      <c r="F317" t="n">
+        <v>0.370845</v>
+      </c>
+      <c r="G317" t="n">
+        <v>-1.299384081890835</v>
+      </c>
+      <c r="H317" t="n">
+        <v>15.82055066921277</v>
+      </c>
+      <c r="I317" t="n">
+        <v>-4.551014439902161</v>
+      </c>
+      <c r="J317" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="K317" t="b">
+        <v>0</v>
+      </c>
+      <c r="L317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>aelf</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>elf</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/1371/large/aelf-logo.png?1696502429</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr"/>
+      <c r="E318" t="n">
+        <v>151483126</v>
+      </c>
+      <c r="F318" t="n">
+        <v>0.198146</v>
+      </c>
+      <c r="G318" t="n">
+        <v>2.652283807491153</v>
+      </c>
+      <c r="H318" t="n">
+        <v>7.007799435200565</v>
+      </c>
+      <c r="I318" t="n">
+        <v>-10.65008778482681</v>
+      </c>
+      <c r="J318" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K318" t="b">
+        <v>0</v>
+      </c>
+      <c r="L318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Polymesh</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>polyx</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/23496/large/Polymesh-symbol.png?1696522706</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr"/>
+      <c r="E319" t="n">
+        <v>151479265</v>
+      </c>
+      <c r="F319" t="n">
+        <v>0.128668</v>
+      </c>
+      <c r="G319" t="n">
+        <v>0.09683156796684901</v>
+      </c>
+      <c r="H319" t="n">
+        <v>4.024895527975034</v>
+      </c>
+      <c r="I319" t="n">
+        <v>-8.53412708937161</v>
+      </c>
+      <c r="J319" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="K319" t="b">
+        <v>0</v>
+      </c>
+      <c r="L319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Rekt</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>rekt</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/51727/large/rektcion_trans_200px.png?1731910587</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr"/>
+      <c r="E320" t="n">
+        <v>150400545</v>
+      </c>
+      <c r="F320" t="n">
+        <v>3.57695e-07</v>
+      </c>
+      <c r="G320" t="n">
+        <v>9.035445356863391</v>
+      </c>
+      <c r="H320" t="n">
+        <v>23.41619637610157</v>
+      </c>
+      <c r="I320" t="n">
+        <v>37.21380388528376</v>
+      </c>
+      <c r="J320" t="n">
+        <v>0.8866666666666667</v>
+      </c>
+      <c r="K320" t="b">
+        <v>1</v>
+      </c>
+      <c r="L320" t="inlineStr">
+        <is>
+          <t>Buen rendimiento mensual (+30%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>AgentFun.AI</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>agentfun</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52133/large/AIFUN_%282%29.png?1732639482</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr"/>
+      <c r="E321" t="n">
+        <v>150119308</v>
+      </c>
+      <c r="F321" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G321" t="n">
+        <v>-1.297182832576729</v>
+      </c>
+      <c r="H321" t="n">
+        <v>0.149676508485657</v>
+      </c>
+      <c r="I321" t="n">
+        <v>-21.43936690564185</v>
+      </c>
+      <c r="J321" t="n">
+        <v>0</v>
+      </c>
+      <c r="K321" t="b">
+        <v>0</v>
+      </c>
+      <c r="L321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>giga</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/34755/large/IMG_0015.png?1705957165</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr"/>
+      <c r="E322" t="n">
+        <v>148274965</v>
+      </c>
+      <c r="F322" t="n">
+        <v>0.01543907</v>
+      </c>
+      <c r="G322" t="n">
+        <v>-6.109580917731808</v>
+      </c>
+      <c r="H322" t="n">
+        <v>-10.00275577700833</v>
+      </c>
+      <c r="I322" t="n">
+        <v>-31.17611753946589</v>
+      </c>
+      <c r="J322" t="n">
+        <v>0</v>
+      </c>
+      <c r="K322" t="b">
+        <v>0</v>
+      </c>
+      <c r="L322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Zano</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>zano</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/8370/large/zano.png?1696508563</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr"/>
+      <c r="E323" t="n">
+        <v>147125434</v>
+      </c>
+      <c r="F323" t="n">
+        <v>9.92</v>
+      </c>
+      <c r="G323" t="n">
+        <v>8.610324701499897</v>
+      </c>
+      <c r="H323" t="n">
+        <v>0.123147332484865</v>
+      </c>
+      <c r="I323" t="n">
+        <v>-2.709078235406632</v>
+      </c>
+      <c r="J323" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="K323" t="b">
+        <v>0</v>
+      </c>
+      <c r="L323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Holo</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>hot</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/3348/large/hot-mark-med.png?1747766692</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr"/>
+      <c r="E324" t="n">
+        <v>146657892</v>
+      </c>
+      <c r="F324" t="n">
+        <v>0.00082622</v>
+      </c>
+      <c r="G324" t="n">
+        <v>-2.063265708731876</v>
+      </c>
+      <c r="H324" t="n">
+        <v>-1.546859323078864</v>
+      </c>
+      <c r="I324" t="n">
+        <v>-14.93767147981043</v>
+      </c>
+      <c r="J324" t="n">
+        <v>0</v>
+      </c>
+      <c r="K324" t="b">
+        <v>0</v>
+      </c>
+      <c r="L324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Stargate Finance</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>stg</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/24413/large/STG_LOGO.png?1696523595</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr"/>
+      <c r="E325" t="n">
+        <v>145976324</v>
+      </c>
+      <c r="F325" t="n">
+        <v>0.150589</v>
+      </c>
+      <c r="G325" t="n">
+        <v>-1.554695266419381</v>
+      </c>
+      <c r="H325" t="n">
+        <v>-1.815628615889379</v>
+      </c>
+      <c r="I325" t="n">
+        <v>-16.92291943985111</v>
+      </c>
+      <c r="J325" t="n">
+        <v>0</v>
+      </c>
+      <c r="K325" t="b">
+        <v>0</v>
+      </c>
+      <c r="L325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Nexus Mutual</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>nxm</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/11810/large/NXMmain.png?1696511684</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr"/>
+      <c r="E326" t="n">
+        <v>144743401</v>
+      </c>
+      <c r="F326" t="n">
+        <v>59.12</v>
+      </c>
+      <c r="G326" t="n">
+        <v>-1.315535979403141</v>
+      </c>
+      <c r="H326" t="n">
+        <v>4.243685478962562</v>
+      </c>
+      <c r="I326" t="n">
+        <v>-0.047427938148765</v>
+      </c>
+      <c r="J326" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K326" t="b">
+        <v>0</v>
+      </c>
+      <c r="L326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>STASIS EURO</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>eurs</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/5164/large/EURS_300x300.png?1696505680</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr"/>
+      <c r="E327" t="n">
+        <v>144283443</v>
+      </c>
+      <c r="F327" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="G327" t="n">
+        <v>-1.349361644656841</v>
+      </c>
+      <c r="H327" t="n">
+        <v>-0.7814677985861921</v>
+      </c>
+      <c r="I327" t="n">
+        <v>2.140891045728902</v>
+      </c>
+      <c r="J327" t="n">
+        <v>0</v>
+      </c>
+      <c r="K327" t="b">
+        <v>0</v>
+      </c>
+      <c r="L327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>CoW Protocol</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>cow</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/24384/large/CoW-token_logo.png?1719524382</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr"/>
+      <c r="E328" t="n">
+        <v>141882266</v>
+      </c>
+      <c r="F328" t="n">
+        <v>0.290601</v>
+      </c>
+      <c r="G328" t="n">
+        <v>-1.905896063659856</v>
+      </c>
+      <c r="H328" t="n">
+        <v>2.591243195878043</v>
+      </c>
+      <c r="I328" t="n">
+        <v>-22.68250106939329</v>
+      </c>
+      <c r="J328" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K328" t="b">
+        <v>0</v>
+      </c>
+      <c r="L328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>EthereumPoW</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>ethw</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/26997/large/logo-clear.png?1696526049</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr"/>
+      <c r="E329" t="n">
+        <v>140686652</v>
+      </c>
+      <c r="F329" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="G329" t="n">
+        <v>-0.7600893210176111</v>
+      </c>
+      <c r="H329" t="n">
+        <v>-0.403944476866815</v>
+      </c>
+      <c r="I329" t="n">
+        <v>-8.29251934296121</v>
+      </c>
+      <c r="J329" t="n">
+        <v>0</v>
+      </c>
+      <c r="K329" t="b">
+        <v>0</v>
+      </c>
+      <c r="L329" t="inlineStr"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Kinesis Silver</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>kag</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/29789/large/kag-currency-ticker.png?1696528719</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr"/>
+      <c r="E330" t="n">
+        <v>140632200</v>
+      </c>
+      <c r="F330" t="n">
+        <v>36.81</v>
+      </c>
+      <c r="G330" t="n">
+        <v>-1.168146123093157</v>
+      </c>
+      <c r="H330" t="n">
+        <v>1.783346593837996</v>
+      </c>
+      <c r="I330" t="n">
+        <v>0.06846773131718101</v>
+      </c>
+      <c r="J330" t="n">
+        <v>0</v>
+      </c>
+      <c r="K330" t="b">
+        <v>0</v>
+      </c>
+      <c r="L330" t="inlineStr"/>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>GMX</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>gmx</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/18323/large/arbit.png?1696517814</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr"/>
+      <c r="E331" t="n">
+        <v>140217945</v>
+      </c>
+      <c r="F331" t="n">
+        <v>13.76</v>
+      </c>
+      <c r="G331" t="n">
+        <v>-2.349585586546924</v>
+      </c>
+      <c r="H331" t="n">
+        <v>-0.5789781450671291</v>
+      </c>
+      <c r="I331" t="n">
+        <v>-15.10919686112438</v>
+      </c>
+      <c r="J331" t="n">
+        <v>0</v>
+      </c>
+      <c r="K331" t="b">
+        <v>0</v>
+      </c>
+      <c r="L331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Prom</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>prom</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/8825/large/Ticker.png?1696508978</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr"/>
+      <c r="E332" t="n">
+        <v>139956532</v>
+      </c>
+      <c r="F332" t="n">
+        <v>7.67</v>
+      </c>
+      <c r="G332" t="n">
+        <v>0.8186967834672221</v>
+      </c>
+      <c r="H332" t="n">
+        <v>22.38256633732004</v>
+      </c>
+      <c r="I332" t="n">
+        <v>43.17450146034166</v>
+      </c>
+      <c r="J332" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="K332" t="b">
+        <v>1</v>
+      </c>
+      <c r="L332" t="inlineStr">
+        <is>
+          <t>Buen rendimiento mensual (+30%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>Ankr Network</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>ankr</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/4324/large/U85xTl2.png?1696504928</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr"/>
+      <c r="E333" t="n">
+        <v>139904559</v>
+      </c>
+      <c r="F333" t="n">
+        <v>0.01399748</v>
+      </c>
+      <c r="G333" t="n">
+        <v>-1.476541831583871</v>
+      </c>
+      <c r="H333" t="n">
+        <v>0.8958587418382531</v>
+      </c>
+      <c r="I333" t="n">
+        <v>-13.62772268067522</v>
+      </c>
+      <c r="J333" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="K333" t="b">
+        <v>0</v>
+      </c>
+      <c r="L333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Origin Ether</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>oeth</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/29733/large/OETH.png?1696528663</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr"/>
+      <c r="E334" t="n">
+        <v>139187273</v>
+      </c>
+      <c r="F334" t="n">
+        <v>2536.33</v>
+      </c>
+      <c r="G334" t="n">
+        <v>-1.377067499071108</v>
+      </c>
+      <c r="H334" t="n">
+        <v>1.832658354905808</v>
+      </c>
+      <c r="I334" t="n">
+        <v>-0.060574824621586</v>
+      </c>
+      <c r="J334" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K334" t="b">
+        <v>0</v>
+      </c>
+      <c r="L334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>FUNToken</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>fun</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/761/large/FUN.png?1696501914</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr"/>
+      <c r="E335" t="n">
+        <v>138997287</v>
+      </c>
+      <c r="F335" t="n">
+        <v>0.01315389</v>
+      </c>
+      <c r="G335" t="n">
+        <v>-0.235236154670854</v>
+      </c>
+      <c r="H335" t="n">
+        <v>31.51784134649767</v>
+      </c>
+      <c r="I335" t="n">
+        <v>266.4637033990667</v>
+      </c>
+      <c r="J335" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="K335" t="b">
+        <v>1</v>
+      </c>
+      <c r="L335" t="inlineStr">
+        <is>
+          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%) | Buena puntuacion en analisis multivariable</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>Infrared Bera</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>ibera</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54671/large/ibera.jpg?1740966414</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>/charts/ibera_chart.png</t>
+        </is>
+      </c>
+      <c r="E336" t="n">
+        <v>137615816</v>
+      </c>
+      <c r="F336" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="G336" t="n">
+        <v>-1.96225858646157</v>
+      </c>
+      <c r="H336" t="n">
+        <v>-2.677094688926385</v>
+      </c>
+      <c r="I336" t="n">
+        <v>-29.0214076253454</v>
+      </c>
+      <c r="J336" t="n">
+        <v>0</v>
+      </c>
+      <c r="K336" t="b">
+        <v>0</v>
+      </c>
+      <c r="L336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>Casper Network</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>cspr</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/15279/large/Casper_Monogram_Favicon_White_on_Red_Circle_RGB_200px.png?1749832573</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>/charts/cspr_chart.png</t>
+        </is>
+      </c>
+      <c r="E337" t="n">
+        <v>137071938</v>
+      </c>
+      <c r="F337" t="n">
+        <v>0.01036343</v>
+      </c>
+      <c r="G337" t="n">
+        <v>-2.484483976761112</v>
+      </c>
+      <c r="H337" t="n">
+        <v>-6.164714931044064</v>
+      </c>
+      <c r="I337" t="n">
+        <v>-21.36335714978747</v>
+      </c>
+      <c r="J337" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K337" t="b">
+        <v>0</v>
+      </c>
+      <c r="L337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>Freysa AI</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>fai</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52315/large/FAI.png?1733076295</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>/charts/fai_chart.png</t>
+        </is>
+      </c>
+      <c r="E338" t="n">
+        <v>136263036</v>
+      </c>
+      <c r="F338" t="n">
+        <v>0.01663553</v>
+      </c>
+      <c r="G338" t="n">
+        <v>-0.199139872497529</v>
+      </c>
+      <c r="H338" t="n">
+        <v>-4.28818986405169</v>
+      </c>
+      <c r="I338" t="n">
+        <v>-12.30027189053258</v>
+      </c>
+      <c r="J338" t="n">
+        <v>0</v>
+      </c>
+      <c r="K338" t="b">
+        <v>0</v>
+      </c>
+      <c r="L338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>MAG7.ssi</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>mag7.ssi</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52962/large/mag7.png?1734863745</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr"/>
+      <c r="E339" t="n">
+        <v>136113939</v>
+      </c>
+      <c r="F339" t="n">
+        <v>0.767292</v>
+      </c>
+      <c r="G339" t="n">
+        <v>-0.483757698407588</v>
+      </c>
+      <c r="H339" t="n">
+        <v>0.7129195425765621</v>
+      </c>
+      <c r="I339" t="n">
+        <v>-0.8430173740105851</v>
+      </c>
+      <c r="J339" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K339" t="b">
+        <v>0</v>
+      </c>
+      <c r="L339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Chia</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>xch</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/15174/large/zV5K5y9f_400x400.png?1696514829</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr"/>
+      <c r="E340" t="n">
+        <v>134751665</v>
+      </c>
+      <c r="F340" t="n">
+        <v>9.210000000000001</v>
+      </c>
+      <c r="G340" t="n">
+        <v>-3.316635531478009</v>
+      </c>
+      <c r="H340" t="n">
+        <v>-6.242986772151665</v>
+      </c>
+      <c r="I340" t="n">
+        <v>-16.28692181705772</v>
+      </c>
+      <c r="J340" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K340" t="b">
+        <v>0</v>
+      </c>
+      <c r="L340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>Drift Protocol</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>drift</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/37509/large/DRIFT.png?1715842607</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr"/>
+      <c r="E341" t="n">
+        <v>134464837</v>
+      </c>
+      <c r="F341" t="n">
+        <v>0.394441</v>
+      </c>
+      <c r="G341" t="n">
+        <v>-0.5624415781067851</v>
+      </c>
+      <c r="H341" t="n">
+        <v>5.646295769942792</v>
+      </c>
+      <c r="I341" t="n">
+        <v>-20.13485927990476</v>
+      </c>
+      <c r="J341" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="K341" t="b">
+        <v>0</v>
+      </c>
+      <c r="L341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>Snek</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>snek</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/30496/large/snek_icon_200_v2.png?1737994261</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr"/>
+      <c r="E342" t="n">
+        <v>134272137</v>
+      </c>
+      <c r="F342" t="n">
+        <v>0.00180139</v>
+      </c>
+      <c r="G342" t="n">
+        <v>-5.338223353713698</v>
+      </c>
+      <c r="H342" t="n">
+        <v>-9.340110610186503</v>
+      </c>
+      <c r="I342" t="n">
+        <v>-29.19520734166939</v>
+      </c>
+      <c r="J342" t="n">
+        <v>0</v>
+      </c>
+      <c r="K342" t="b">
+        <v>0</v>
+      </c>
+      <c r="L342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>Harmony</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>one</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/4344/large/Y88JAze.png?1696504947</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr"/>
+      <c r="E343" t="n">
+        <v>134235827</v>
+      </c>
+      <c r="F343" t="n">
+        <v>0.00916113</v>
+      </c>
+      <c r="G343" t="n">
+        <v>-2.815157951132257</v>
+      </c>
+      <c r="H343" t="n">
+        <v>-6.497665436841836</v>
+      </c>
+      <c r="I343" t="n">
+        <v>-21.31820318937763</v>
+      </c>
+      <c r="J343" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="K343" t="b">
+        <v>0</v>
+      </c>
+      <c r="L343" t="inlineStr"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>CoinEx</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>cet</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/4817/large/coinex-token.png?1696505367</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr"/>
+      <c r="E344" t="n">
+        <v>134083550</v>
+      </c>
+      <c r="F344" t="n">
+        <v>0.050366</v>
+      </c>
+      <c r="G344" t="n">
+        <v>0.333578451287538</v>
+      </c>
+      <c r="H344" t="n">
+        <v>-6.882762557421142</v>
+      </c>
+      <c r="I344" t="n">
+        <v>-19.51476990991648</v>
+      </c>
+      <c r="J344" t="n">
+        <v>0</v>
+      </c>
+      <c r="K344" t="b">
+        <v>0</v>
+      </c>
+      <c r="L344" t="inlineStr"/>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>Resolv RLP</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>rlp</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/40017/large/orangeLogo..png?1725344586</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr"/>
+      <c r="E345" t="n">
+        <v>132930883</v>
+      </c>
+      <c r="F345" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G345" t="n">
+        <v>0.603523393167491</v>
+      </c>
+      <c r="H345" t="n">
+        <v>0.360753647187372</v>
+      </c>
+      <c r="I345" t="n">
+        <v>0.543455327093184</v>
+      </c>
+      <c r="J345" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="K345" t="b">
+        <v>0</v>
+      </c>
+      <c r="L345" t="inlineStr"/>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>KUB Coin</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>kub</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/15760/large/KUB_Coin_2025.png?1741751451</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr"/>
+      <c r="E346" t="n">
+        <v>131571742</v>
+      </c>
+      <c r="F346" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="G346" t="n">
+        <v>-0.298603647549984</v>
+      </c>
+      <c r="H346" t="n">
+        <v>-1.943759151501483</v>
+      </c>
+      <c r="I346" t="n">
+        <v>1.452860414381445</v>
+      </c>
+      <c r="J346" t="n">
+        <v>0</v>
+      </c>
+      <c r="K346" t="b">
+        <v>0</v>
+      </c>
+      <c r="L346" t="inlineStr"/>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>TDCCP</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>tdccp</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55581/large/tdccp-logo.jpg?1746787823</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr"/>
+      <c r="E347" t="n">
+        <v>129953388</v>
+      </c>
+      <c r="F347" t="n">
+        <v>0.203052</v>
+      </c>
+      <c r="G347" t="n">
+        <v>-2.454978580760825</v>
+      </c>
+      <c r="H347" t="n">
+        <v>-5.069449043633151</v>
+      </c>
+      <c r="I347" t="n">
+        <v>-4.011050559946679</v>
+      </c>
+      <c r="J347" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K347" t="b">
+        <v>0</v>
+      </c>
+      <c r="L347" t="inlineStr"/>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>Conscious Token</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>conscious</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55111/large/conscious_token_logo.png?1743754945</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr"/>
+      <c r="E348" t="n">
+        <v>129946144</v>
+      </c>
+      <c r="F348" t="n">
+        <v>0.129947</v>
+      </c>
+      <c r="G348" t="n">
+        <v>1.916533700658077</v>
+      </c>
+      <c r="H348" t="n">
+        <v>9.447578592726991</v>
+      </c>
+      <c r="I348" t="n">
+        <v>23.925163867219</v>
+      </c>
+      <c r="J348" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="K348" t="b">
+        <v>1</v>
+      </c>
+      <c r="L348" t="inlineStr">
+        <is>
+          <t>Tendencia semanal positiva | Alta confianza del modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>DigiByte</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>dgb</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/63/large/digibyte.png?1696501454</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr"/>
+      <c r="E349" t="n">
+        <v>129940861</v>
+      </c>
+      <c r="F349" t="n">
+        <v>0.007303899999999999</v>
+      </c>
+      <c r="G349" t="n">
+        <v>-2.383960444779298</v>
+      </c>
+      <c r="H349" t="n">
+        <v>-3.463150240093763</v>
+      </c>
+      <c r="I349" t="n">
+        <v>-18.67734229487051</v>
+      </c>
+      <c r="J349" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="K349" t="b">
+        <v>0</v>
+      </c>
+      <c r="L349" t="inlineStr"/>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>AUSD</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>ausd</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39284/large/Circle_Agora_White_on_Olive_1080px.png?1722961274</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr"/>
+      <c r="E350" t="n">
+        <v>129816235</v>
+      </c>
+      <c r="F350" t="n">
+        <v>0.9991819999999999</v>
+      </c>
+      <c r="G350" t="n">
+        <v>-0.04216970136813501</v>
+      </c>
+      <c r="H350" t="n">
+        <v>-0.023764863961875</v>
+      </c>
+      <c r="I350" t="n">
+        <v>0.010699752596621</v>
+      </c>
+      <c r="J350" t="n">
+        <v>0</v>
+      </c>
+      <c r="K350" t="b">
+        <v>0</v>
+      </c>
+      <c r="L350" t="inlineStr"/>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>ICON</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>icx</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/1060/large/ICON-symbol-coingecko_latest.png?1706638336</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr"/>
+      <c r="E351" t="n">
+        <v>129714469</v>
+      </c>
+      <c r="F351" t="n">
+        <v>0.121311</v>
+      </c>
+      <c r="G351" t="n">
+        <v>-1.25684031741597</v>
+      </c>
+      <c r="H351" t="n">
+        <v>-2.498098283203195</v>
+      </c>
+      <c r="I351" t="n">
+        <v>-22.51186307466467</v>
+      </c>
+      <c r="J351" t="n">
+        <v>0</v>
+      </c>
+      <c r="K351" t="b">
+        <v>0</v>
+      </c>
+      <c r="L351" t="inlineStr"/>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>Vana</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>vana</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/51404/large/logo.png?1731086679</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr"/>
+      <c r="E352" t="n">
+        <v>129363133</v>
+      </c>
+      <c r="F352" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="G352" t="n">
+        <v>-3.465187631110382</v>
+      </c>
+      <c r="H352" t="n">
+        <v>-3.918396711569448</v>
+      </c>
+      <c r="I352" t="n">
+        <v>-33.49167283221084</v>
+      </c>
+      <c r="J352" t="n">
+        <v>0</v>
+      </c>
+      <c r="K352" t="b">
+        <v>0</v>
+      </c>
+      <c r="L352" t="inlineStr"/>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>Function ƒBTC</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>fbtc</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39182/large/fbtc.png?1740123952</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr"/>
+      <c r="E353" t="n">
+        <v>129143415</v>
+      </c>
+      <c r="F353" t="n">
+        <v>107354</v>
+      </c>
+      <c r="G353" t="n">
+        <v>-1.920941626058651</v>
+      </c>
+      <c r="H353" t="n">
+        <v>0.207992666500588</v>
+      </c>
+      <c r="I353" t="n">
+        <v>1.448375432435249</v>
+      </c>
+      <c r="J353" t="n">
+        <v>0</v>
+      </c>
+      <c r="K353" t="b">
+        <v>0</v>
+      </c>
+      <c r="L353" t="inlineStr"/>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>Coinshift USDL Morpho Vault</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>csusdl</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52413/large/csUSDL-badge_2_2x.png?1738166925</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr"/>
+      <c r="E354" t="n">
+        <v>128090215</v>
+      </c>
+      <c r="F354" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="G354" t="n">
+        <v>0.013404068186482</v>
+      </c>
+      <c r="H354" t="n">
+        <v>0.088913317379001</v>
+      </c>
+      <c r="I354" t="n">
+        <v>0.3848671968665751</v>
+      </c>
+      <c r="J354" t="n">
+        <v>0</v>
+      </c>
+      <c r="K354" t="b">
+        <v>0</v>
+      </c>
+      <c r="L354" t="inlineStr"/>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>cETH</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>ceth</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/10643/large/ceth.png?1696510617</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr"/>
+      <c r="E355" t="n">
+        <v>127975554</v>
+      </c>
+      <c r="F355" t="n">
+        <v>50.79</v>
+      </c>
+      <c r="G355" t="n">
+        <v>-1.719417965399076</v>
+      </c>
+      <c r="H355" t="n">
+        <v>1.462691278363529</v>
+      </c>
+      <c r="I355" t="n">
+        <v>0.358636478921627</v>
+      </c>
+      <c r="J355" t="n">
+        <v>0</v>
+      </c>
+      <c r="K355" t="b">
+        <v>0</v>
+      </c>
+      <c r="L355" t="inlineStr"/>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>Noble Dollar (USDN)</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>usdn</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55257/large/USDN.png?1745046774</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr"/>
+      <c r="E356" t="n">
+        <v>127962328</v>
+      </c>
+      <c r="F356" t="n">
+        <v>0.999903</v>
+      </c>
+      <c r="G356" t="n">
+        <v>0.000307406503892</v>
+      </c>
+      <c r="H356" t="n">
+        <v>2.781601148392004e-05</v>
+      </c>
+      <c r="I356" t="n">
+        <v>0.010118894397678</v>
+      </c>
+      <c r="J356" t="n">
+        <v>0</v>
+      </c>
+      <c r="K356" t="b">
+        <v>0</v>
+      </c>
+      <c r="L356" t="inlineStr"/>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>GOHOME</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>gohome</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54909/large/20250314_132950.png?1742455637</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr"/>
+      <c r="E357" t="n">
+        <v>127849857</v>
+      </c>
+      <c r="F357" t="n">
+        <v>243.83</v>
+      </c>
+      <c r="G357" t="n">
+        <v>-0.09729613752128501</v>
+      </c>
+      <c r="H357" t="n">
+        <v>-0.065291529576688</v>
+      </c>
+      <c r="I357" t="n">
+        <v>-2.556513792205956</v>
+      </c>
+      <c r="J357" t="n">
+        <v>0</v>
+      </c>
+      <c r="K357" t="b">
+        <v>0</v>
+      </c>
+      <c r="L357" t="inlineStr"/>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>Solayer</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>layer</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/53498/large/Layer_Green.png?1744950002</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr"/>
+      <c r="E358" t="n">
+        <v>126719910</v>
+      </c>
+      <c r="F358" t="n">
+        <v>0.603447</v>
+      </c>
+      <c r="G358" t="n">
+        <v>-3.304391627236192</v>
+      </c>
+      <c r="H358" t="n">
+        <v>-7.05755495758265</v>
+      </c>
+      <c r="I358" t="n">
+        <v>-20.61154401074652</v>
+      </c>
+      <c r="J358" t="n">
+        <v>0</v>
+      </c>
+      <c r="K358" t="b">
+        <v>0</v>
+      </c>
+      <c r="L358" t="inlineStr"/>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>WOO</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>woo</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12921/large/WOO_Logos_2023_Profile_Pic_WOO.png?1696512709</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr"/>
+      <c r="E359" t="n">
+        <v>126624944</v>
+      </c>
+      <c r="F359" t="n">
+        <v>0.066328</v>
+      </c>
+      <c r="G359" t="n">
+        <v>-2.722162652004423</v>
+      </c>
+      <c r="H359" t="n">
+        <v>-2.069125360097008</v>
+      </c>
+      <c r="I359" t="n">
+        <v>-12.61581678804914</v>
+      </c>
+      <c r="J359" t="n">
+        <v>0</v>
+      </c>
+      <c r="K359" t="b">
+        <v>0</v>
+      </c>
+      <c r="L359" t="inlineStr"/>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>Kamino</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>kmno</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/35801/large/tP0Lcgwp_400x400.jpg?1709824189</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr"/>
+      <c r="E360" t="n">
+        <v>125249848</v>
+      </c>
+      <c r="F360" t="n">
+        <v>0.055339</v>
+      </c>
+      <c r="G360" t="n">
+        <v>-3.28295628292807</v>
+      </c>
+      <c r="H360" t="n">
+        <v>-6.90536354174418</v>
+      </c>
+      <c r="I360" t="n">
+        <v>4.613843273766828</v>
+      </c>
+      <c r="J360" t="n">
+        <v>0</v>
+      </c>
+      <c r="K360" t="b">
+        <v>0</v>
+      </c>
+      <c r="L360" t="inlineStr"/>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>AI Companions</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>aic</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/40130/large/AI_Companions.png?1725942702</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr"/>
+      <c r="E361" t="n">
+        <v>124806924</v>
+      </c>
+      <c r="F361" t="n">
+        <v>0.124807</v>
+      </c>
+      <c r="G361" t="n">
+        <v>-3.761588587726594</v>
+      </c>
+      <c r="H361" t="n">
+        <v>-16.85362247456233</v>
+      </c>
+      <c r="I361" t="n">
+        <v>19.85002231336454</v>
+      </c>
+      <c r="J361" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K361" t="b">
+        <v>0</v>
+      </c>
+      <c r="L361" t="inlineStr"/>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>XYO Network</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>xyo</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/4519/large/XYO_Network-logo.png?1696505103</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr"/>
+      <c r="E362" t="n">
+        <v>123880856</v>
+      </c>
+      <c r="F362" t="n">
+        <v>0.00889153</v>
+      </c>
+      <c r="G362" t="n">
+        <v>-2.228750869447759</v>
+      </c>
+      <c r="H362" t="n">
+        <v>-0.6959385141627761</v>
+      </c>
+      <c r="I362" t="n">
+        <v>-15.893109279352</v>
+      </c>
+      <c r="J362" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K362" t="b">
+        <v>0</v>
+      </c>
+      <c r="L362" t="inlineStr"/>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>GMT</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>gmt</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/23597/large/token-gmt-200x200.png?1703153841</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr"/>
+      <c r="E363" t="n">
+        <v>123786836</v>
+      </c>
+      <c r="F363" t="n">
+        <v>0.04218409</v>
+      </c>
+      <c r="G363" t="n">
+        <v>-3.362321985581733</v>
+      </c>
+      <c r="H363" t="n">
+        <v>-3.588971264373914</v>
+      </c>
+      <c r="I363" t="n">
+        <v>-16.18022690345209</v>
+      </c>
+      <c r="J363" t="n">
+        <v>0</v>
+      </c>
+      <c r="K363" t="b">
+        <v>0</v>
+      </c>
+      <c r="L363" t="inlineStr"/>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Melania Meme</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>melania</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/53775/large/melania-meme.png?1737329885</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr"/>
+      <c r="E364" t="n">
+        <v>122283008</v>
+      </c>
+      <c r="F364" t="n">
+        <v>0.189612</v>
+      </c>
+      <c r="G364" t="n">
+        <v>-4.091320556995107</v>
+      </c>
+      <c r="H364" t="n">
+        <v>-4.763131309838747</v>
+      </c>
+      <c r="I364" t="n">
+        <v>-37.21193217157764</v>
+      </c>
+      <c r="J364" t="n">
+        <v>0</v>
+      </c>
+      <c r="K364" t="b">
+        <v>0</v>
+      </c>
+      <c r="L364" t="inlineStr"/>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>Non-Playable Coin</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>npc</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/31193/large/NPC_200x200.png?1696530021</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr"/>
+      <c r="E365" t="n">
+        <v>121818399</v>
+      </c>
+      <c r="F365" t="n">
+        <v>0.01512068</v>
+      </c>
+      <c r="G365" t="n">
+        <v>-2.466118163498936</v>
+      </c>
+      <c r="H365" t="n">
+        <v>0.449616546776388</v>
+      </c>
+      <c r="I365" t="n">
+        <v>19.18852432655161</v>
+      </c>
+      <c r="J365" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="K365" t="b">
+        <v>1</v>
+      </c>
+      <c r="L365" t="inlineStr">
+        <is>
+          <t>Buena puntuacion en analisis multivariable</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>Anzen USDz</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>usdz</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/38039/large/usdz-image-200x200.png?1716334412</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr"/>
+      <c r="E366" t="n">
+        <v>121128362</v>
+      </c>
+      <c r="F366" t="n">
+        <v>0.9852379999999999</v>
+      </c>
+      <c r="G366" t="n">
+        <v>-0.409615703487786</v>
+      </c>
+      <c r="H366" t="n">
+        <v>0.16318712049164</v>
+      </c>
+      <c r="I366" t="n">
+        <v>0.8427581444355841</v>
+      </c>
+      <c r="J366" t="n">
+        <v>0</v>
+      </c>
+      <c r="K366" t="b">
+        <v>0</v>
+      </c>
+      <c r="L366" t="inlineStr"/>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>aura</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>aura</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/38376/large/aura_logo_200x200-01-01.png?1751114135</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr"/>
+      <c r="E367" t="n">
+        <v>120701979</v>
+      </c>
+      <c r="F367" t="n">
+        <v>0.125335</v>
+      </c>
+      <c r="G367" t="n">
+        <v>-11.73592268897098</v>
+      </c>
+      <c r="H367" t="n">
+        <v>14.36553593152547</v>
+      </c>
+      <c r="I367" t="n">
+        <v>13701.95877798988</v>
+      </c>
+      <c r="J367" t="n">
+        <v>0.6466666666666666</v>
+      </c>
+      <c r="K367" t="b">
+        <v>1</v>
+      </c>
+      <c r="L367" t="inlineStr">
+        <is>
+          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%) | Buena puntuacion en analisis multivariable</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>Kadena</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>kda</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/3693/large/Social_-_Profile_Picture.png?1723001308</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr"/>
+      <c r="E368" t="n">
+        <v>120615551</v>
+      </c>
+      <c r="F368" t="n">
+        <v>0.372636</v>
+      </c>
+      <c r="G368" t="n">
+        <v>-3.790234403799128</v>
+      </c>
+      <c r="H368" t="n">
+        <v>-4.131192172790647</v>
+      </c>
+      <c r="I368" t="n">
+        <v>-16.22938341587612</v>
+      </c>
+      <c r="J368" t="n">
+        <v>0</v>
+      </c>
+      <c r="K368" t="b">
+        <v>0</v>
+      </c>
+      <c r="L368" t="inlineStr"/>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>SQD</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>sqd</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/37869/large/New_Logo_SQD_Icon.png?1720048443</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr"/>
+      <c r="E369" t="n">
+        <v>120204240</v>
+      </c>
+      <c r="F369" t="n">
+        <v>0.162931</v>
+      </c>
+      <c r="G369" t="n">
+        <v>-0.05306986317568101</v>
+      </c>
+      <c r="H369" t="n">
+        <v>0.198073248504389</v>
+      </c>
+      <c r="I369" t="n">
+        <v>-21.77795502089348</v>
+      </c>
+      <c r="J369" t="n">
+        <v>0</v>
+      </c>
+      <c r="K369" t="b">
+        <v>0</v>
+      </c>
+      <c r="L369" t="inlineStr"/>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>Enjin Coin</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>enj</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/1102/large/Symbol_Only_-_Purple.png?1709725966</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr"/>
+      <c r="E370" t="n">
+        <v>119619281</v>
+      </c>
+      <c r="F370" t="n">
+        <v>0.06424299999999999</v>
+      </c>
+      <c r="G370" t="n">
+        <v>-2.6665129723761</v>
+      </c>
+      <c r="H370" t="n">
+        <v>-0.924011964249375</v>
+      </c>
+      <c r="I370" t="n">
+        <v>-15.23149167880798</v>
+      </c>
+      <c r="J370" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K370" t="b">
+        <v>0</v>
+      </c>
+      <c r="L370" t="inlineStr"/>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>Mask Network</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>mask</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/14051/large/Mask_Network.jpg?1696513776</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr"/>
+      <c r="E371" t="n">
+        <v>119609481</v>
+      </c>
+      <c r="F371" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G371" t="n">
+        <v>-2.701063593131716</v>
+      </c>
+      <c r="H371" t="n">
+        <v>-0.019495255235594</v>
+      </c>
+      <c r="I371" t="n">
+        <v>-35.34586872125161</v>
+      </c>
+      <c r="J371" t="n">
+        <v>0</v>
+      </c>
+      <c r="K371" t="b">
+        <v>0</v>
+      </c>
+      <c r="L371" t="inlineStr"/>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>Echelon Prime</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>prime</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/29053/large/prime-logo-small-border_%282%29.png?1696528020</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr"/>
+      <c r="E372" t="n">
+        <v>119537787</v>
+      </c>
+      <c r="F372" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="G372" t="n">
+        <v>-5.29113376237221</v>
+      </c>
+      <c r="H372" t="n">
+        <v>-2.082096807620838</v>
+      </c>
+      <c r="I372" t="n">
+        <v>-13.95299240008044</v>
+      </c>
+      <c r="J372" t="n">
+        <v>0</v>
+      </c>
+      <c r="K372" t="b">
+        <v>0</v>
+      </c>
+      <c r="L372" t="inlineStr"/>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>Resolv wstUSR</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>wstusr</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/51880/large/USR_LOGO.png?1732098841</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr"/>
+      <c r="E373" t="n">
+        <v>119258453</v>
+      </c>
+      <c r="F373" t="n">
+        <v>1.089</v>
+      </c>
+      <c r="G373" t="n">
+        <v>0</v>
+      </c>
+      <c r="H373" t="n">
+        <v>0</v>
+      </c>
+      <c r="I373" t="n">
+        <v>80.44094641780181</v>
+      </c>
+      <c r="J373" t="n">
+        <v>0.1466666666666667</v>
+      </c>
+      <c r="K373" t="b">
+        <v>0</v>
+      </c>
+      <c r="L373" t="inlineStr"/>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>Launch Coin on Believe</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>launchcoin</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/53916/large/launchcoin.jpg?1747131421</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr"/>
+      <c r="E374" t="n">
+        <v>119257893</v>
+      </c>
+      <c r="F374" t="n">
+        <v>0.11888</v>
+      </c>
+      <c r="G374" t="n">
+        <v>-3.419662470672686</v>
+      </c>
+      <c r="H374" t="n">
+        <v>-15.84945925871644</v>
+      </c>
+      <c r="I374" t="n">
+        <v>-27.44468937358589</v>
+      </c>
+      <c r="J374" t="n">
+        <v>0</v>
+      </c>
+      <c r="K374" t="b">
+        <v>0</v>
+      </c>
+      <c r="L374" t="inlineStr"/>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>Horizen</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>zen</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/691/large/Horizen2.0-logo_icon-on-yellow_%281%29.png?1751696763</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr"/>
+      <c r="E375" t="n">
+        <v>118797064</v>
+      </c>
+      <c r="F375" t="n">
+        <v>7.39</v>
+      </c>
+      <c r="G375" t="n">
+        <v>-2.469860716508022</v>
+      </c>
+      <c r="H375" t="n">
+        <v>2.553878248375264</v>
+      </c>
+      <c r="I375" t="n">
+        <v>-26.89075749106678</v>
+      </c>
+      <c r="J375" t="n">
+        <v>0.04666666666666667</v>
+      </c>
+      <c r="K375" t="b">
+        <v>0</v>
+      </c>
+      <c r="L375" t="inlineStr"/>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>aixbt by Virtuals</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>aixbt</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/51784/large/3.png?1731981138</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr"/>
+      <c r="E376" t="n">
+        <v>118011361</v>
+      </c>
+      <c r="F376" t="n">
+        <v>0.123671</v>
+      </c>
+      <c r="G376" t="n">
+        <v>-9.115426933568124</v>
+      </c>
+      <c r="H376" t="n">
+        <v>-3.943298725454398</v>
+      </c>
+      <c r="I376" t="n">
+        <v>-29.6219212145108</v>
+      </c>
+      <c r="J376" t="n">
+        <v>0</v>
+      </c>
+      <c r="K376" t="b">
+        <v>0</v>
+      </c>
+      <c r="L376" t="inlineStr"/>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>ZIGChain</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>zig</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/14796/large/zig.jpg?1731990265</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr"/>
+      <c r="E377" t="n">
+        <v>117873681</v>
+      </c>
+      <c r="F377" t="n">
+        <v>0.083715</v>
+      </c>
+      <c r="G377" t="n">
+        <v>-3.701897607801124</v>
+      </c>
+      <c r="H377" t="n">
+        <v>-6.367743214743764</v>
+      </c>
+      <c r="I377" t="n">
+        <v>-8.633462820536764</v>
+      </c>
+      <c r="J377" t="n">
+        <v>0</v>
+      </c>
+      <c r="K377" t="b">
+        <v>0</v>
+      </c>
+      <c r="L377" t="inlineStr"/>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>Incrypt</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>inc</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55966/large/Incrypt_Token_Logo_%281%29.png?1747887506</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr"/>
+      <c r="E378" t="n">
+        <v>117066706</v>
+      </c>
+      <c r="F378" t="n">
+        <v>0.01820899</v>
+      </c>
+      <c r="G378" t="n">
+        <v>24.58896648544549</v>
+      </c>
+      <c r="H378" t="n">
+        <v>25.83591927257465</v>
+      </c>
+      <c r="I378" t="n">
+        <v>-18.19267425855399</v>
+      </c>
+      <c r="J378" t="n">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="K378" t="b">
+        <v>0</v>
+      </c>
+      <c r="L378" t="inlineStr"/>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>Liquity</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>lqty</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/14665/large/logo_V2.png?1725437146</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr"/>
+      <c r="E379" t="n">
+        <v>115289570</v>
+      </c>
+      <c r="F379" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="G379" t="n">
+        <v>-4.538411709520306</v>
+      </c>
+      <c r="H379" t="n">
+        <v>-13.84444620980381</v>
+      </c>
+      <c r="I379" t="n">
+        <v>34.3077215472813</v>
+      </c>
+      <c r="J379" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="K379" t="b">
+        <v>0</v>
+      </c>
+      <c r="L379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Spiko US T-Bills Money Market Fund</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>ustbl</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39666/large/USTB.png?1723541269</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr"/>
+      <c r="E380" t="n">
+        <v>115219588</v>
+      </c>
+      <c r="F380" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="G380" t="n">
+        <v>0.037535391873302</v>
+      </c>
+      <c r="H380" t="n">
+        <v>0.079677174014572</v>
+      </c>
+      <c r="I380" t="n">
+        <v>0.342287728096258</v>
+      </c>
+      <c r="J380" t="n">
+        <v>0</v>
+      </c>
+      <c r="K380" t="b">
+        <v>0</v>
+      </c>
+      <c r="L380" t="inlineStr"/>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>Orca</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>orca</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/17547/large/Orca_Logo.png?1696517083</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr"/>
+      <c r="E381" t="n">
+        <v>114503396</v>
+      </c>
+      <c r="F381" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="G381" t="n">
+        <v>-3.177906239540469</v>
+      </c>
+      <c r="H381" t="n">
+        <v>-1.491845646058031</v>
+      </c>
+      <c r="I381" t="n">
+        <v>-19.36614766735637</v>
+      </c>
+      <c r="J381" t="n">
+        <v>0</v>
+      </c>
+      <c r="K381" t="b">
+        <v>0</v>
+      </c>
+      <c r="L381" t="inlineStr"/>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>crvUSD</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>crvusd</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/30118/large/crvusd.jpg?1746670973</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr"/>
+      <c r="E382" t="n">
+        <v>114401431</v>
+      </c>
+      <c r="F382" t="n">
+        <v>0.9996959999999999</v>
+      </c>
+      <c r="G382" t="n">
+        <v>-0.033295537704368</v>
+      </c>
+      <c r="H382" t="n">
+        <v>-0.016320631990266</v>
+      </c>
+      <c r="I382" t="n">
+        <v>-0.007056848834443001</v>
+      </c>
+      <c r="J382" t="n">
+        <v>0</v>
+      </c>
+      <c r="K382" t="b">
+        <v>0</v>
+      </c>
+      <c r="L382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>Sushi</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>sushi</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12271/large/512x512_Logo_no_chop.png?1696512101</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr"/>
+      <c r="E383" t="n">
+        <v>113687721</v>
+      </c>
+      <c r="F383" t="n">
+        <v>0.5897089999999999</v>
+      </c>
+      <c r="G383" t="n">
+        <v>-3.511315430571598</v>
+      </c>
+      <c r="H383" t="n">
+        <v>-1.420799821966875</v>
+      </c>
+      <c r="I383" t="n">
+        <v>-9.506945432329656</v>
+      </c>
+      <c r="J383" t="n">
+        <v>0</v>
+      </c>
+      <c r="K383" t="b">
+        <v>0</v>
+      </c>
+      <c r="L383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>io.net</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>io</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/37754/large/io_blackbg.png?1715446363</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr"/>
+      <c r="E384" t="n">
+        <v>111695493</v>
+      </c>
+      <c r="F384" t="n">
+        <v>0.662449</v>
+      </c>
+      <c r="G384" t="n">
+        <v>-5.159997437871057</v>
+      </c>
+      <c r="H384" t="n">
+        <v>-6.178764158928822</v>
+      </c>
+      <c r="I384" t="n">
+        <v>-14.82530951891758</v>
+      </c>
+      <c r="J384" t="n">
+        <v>0</v>
+      </c>
+      <c r="K384" t="b">
+        <v>0</v>
+      </c>
+      <c r="L384" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update cryptocurrency predictions and recommendations with new data and adjustments
- Replaced Sei with Bitcoin Cash in criptos_predichas.json, updating market cap, current price, and reasons for prediction.
- Added new cryptocurrencies RealLink and ONFA to criptos_predichas.json with detailed metrics.
- Adjusted scores and reasons for several cryptocurrencies in criptos_predichas.json to reflect recent performance.
- Updated Sologenic and Rekt entries in recomendaciones.json with revised units and projected values.
- Replaced Rekt with Conscious Token in recomendaciones.json, including updated metrics and projections.
- Added RealLink to recomendaciones.json with new metrics and projections.
- Updated Prom and Euler entries in recomendaciones.json with revised values and projections.
</commit_message>
<xml_diff>
--- a/data/predicciones_criptos.xlsx
+++ b/data/predicciones_criptos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L384"/>
+  <dimension ref="A1:L430"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,7 +532,7 @@
         <v>3.404126761127093</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
@@ -576,7 +576,7 @@
         <v>-1.413630270690066</v>
       </c>
       <c r="J3" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
@@ -704,7 +704,7 @@
         <v>-0.969268928301472</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
@@ -984,7 +984,7 @@
         <v>3.310589202212904</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
@@ -1064,7 +1064,7 @@
         <v>-0.674209286023263</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K15" t="b">
         <v>0</v>
@@ -1104,7 +1104,7 @@
         <v>-9.331747974351638</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K16" t="b">
         <v>0</v>
@@ -1144,12 +1144,16 @@
         <v>22.08120425105527</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1066666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="K17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Buena puntuacion en analisis multivariable</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1184,7 +1188,7 @@
         <v>-4.336743214979863</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K18" t="b">
         <v>0</v>
@@ -1224,7 +1228,7 @@
         <v>2.186606821604448</v>
       </c>
       <c r="J19" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K19" t="b">
         <v>0</v>
@@ -1624,7 +1628,7 @@
         <v>39.17162961148887</v>
       </c>
       <c r="J29" t="n">
-        <v>0.04</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K29" t="b">
         <v>0</v>
@@ -1904,7 +1908,7 @@
         <v>13.88295718228861</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K36" t="b">
         <v>0</v>
@@ -2224,7 +2228,7 @@
         <v>-14.88173006709638</v>
       </c>
       <c r="J44" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K44" t="b">
         <v>0</v>
@@ -2304,7 +2308,7 @@
         <v>-11.71712559028115</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K46" t="b">
         <v>0</v>
@@ -2636,7 +2640,7 @@
         <v>-13.60086853440658</v>
       </c>
       <c r="J54" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K54" t="b">
         <v>0</v>
@@ -2756,7 +2760,7 @@
         <v>-19.01774212095845</v>
       </c>
       <c r="J57" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K57" t="b">
         <v>0</v>
@@ -2960,7 +2964,7 @@
         <v>-23.37237596293679</v>
       </c>
       <c r="J62" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K62" t="b">
         <v>0</v>
@@ -3040,7 +3044,7 @@
         <v>3.672065484066418</v>
       </c>
       <c r="J64" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.02</v>
       </c>
       <c r="K64" t="b">
         <v>0</v>
@@ -3240,7 +3244,7 @@
         <v>-9.556828834635429</v>
       </c>
       <c r="J69" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K69" t="b">
         <v>0</v>
@@ -3280,7 +3284,7 @@
         <v>-22.95847335923886</v>
       </c>
       <c r="J70" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K70" t="b">
         <v>0</v>
@@ -3440,16 +3444,12 @@
         <v>34.02739822198766</v>
       </c>
       <c r="J74" t="n">
-        <v>0.76</v>
+        <v>0.34</v>
       </c>
       <c r="K74" t="b">
-        <v>1</v>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>Buen rendimiento mensual (+30%) | Buena puntuacion en analisis multivariable</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3484,7 +3484,7 @@
         <v>-0.002877455154935</v>
       </c>
       <c r="J75" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K75" t="b">
         <v>0</v>
@@ -3524,7 +3524,7 @@
         <v>-0.035522872151087</v>
       </c>
       <c r="J76" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K76" t="b">
         <v>0</v>
@@ -3724,7 +3724,7 @@
         <v>-5.46076904273847</v>
       </c>
       <c r="J81" t="n">
-        <v>0.02666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K81" t="b">
         <v>0</v>
@@ -3844,7 +3844,7 @@
         <v>3.4530988051059</v>
       </c>
       <c r="J84" t="n">
-        <v>0.09333333333333334</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K84" t="b">
         <v>0</v>
@@ -3964,7 +3964,7 @@
         <v>-7.558543714704253</v>
       </c>
       <c r="J87" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K87" t="b">
         <v>0</v>
@@ -4004,7 +4004,7 @@
         <v>-29.16914736896904</v>
       </c>
       <c r="J88" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K88" t="b">
         <v>0</v>
@@ -4044,7 +4044,7 @@
         <v>-11.37185206377279</v>
       </c>
       <c r="J89" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K89" t="b">
         <v>0</v>
@@ -4164,7 +4164,7 @@
         <v>-20.73487845027156</v>
       </c>
       <c r="J92" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K92" t="b">
         <v>0</v>
@@ -4204,7 +4204,7 @@
         <v>-16.34997855450167</v>
       </c>
       <c r="J93" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K93" t="b">
         <v>0</v>
@@ -4244,7 +4244,7 @@
         <v>-1.190710980089554</v>
       </c>
       <c r="J94" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K94" t="b">
         <v>0</v>
@@ -4284,7 +4284,7 @@
         <v>-0.021382708202666</v>
       </c>
       <c r="J95" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K95" t="b">
         <v>0</v>
@@ -4324,14 +4324,14 @@
         <v>40.64601967701537</v>
       </c>
       <c r="J96" t="n">
-        <v>0.8066666666666666</v>
+        <v>0.4266666666666667</v>
       </c>
       <c r="K96" t="b">
         <v>1</v>
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>Buen rendimiento mensual (+30%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
+          <t>Buen rendimiento mensual (+30%) | Fuerte tendencia semanal (+10%)</t>
         </is>
       </c>
     </row>
@@ -4368,7 +4368,7 @@
         <v>-1.157675008301329</v>
       </c>
       <c r="J97" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K97" t="b">
         <v>0</v>
@@ -4408,7 +4408,7 @@
         <v>40.59617452460589</v>
       </c>
       <c r="J98" t="n">
-        <v>0.12</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K98" t="b">
         <v>0</v>
@@ -4452,7 +4452,7 @@
         <v>-0.886004824973551</v>
       </c>
       <c r="J99" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K99" t="b">
         <v>0</v>
@@ -4624,7 +4624,7 @@
         <v>-0.405621828180371</v>
       </c>
       <c r="J103" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K103" t="b">
         <v>0</v>
@@ -4916,7 +4916,7 @@
         <v>-0.8559408883874851</v>
       </c>
       <c r="J110" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K110" t="b">
         <v>0</v>
@@ -4956,7 +4956,7 @@
         <v>-23.79567837798205</v>
       </c>
       <c r="J111" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K111" t="b">
         <v>0</v>
@@ -5156,7 +5156,7 @@
         <v>-4.60285756728105</v>
       </c>
       <c r="J116" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K116" t="b">
         <v>0</v>
@@ -5396,7 +5396,7 @@
         <v>0.335258106868906</v>
       </c>
       <c r="J122" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K122" t="b">
         <v>0</v>
@@ -5516,7 +5516,7 @@
         <v>41.49245405224639</v>
       </c>
       <c r="J125" t="n">
-        <v>0.08666666666666667</v>
+        <v>0.08</v>
       </c>
       <c r="K125" t="b">
         <v>0</v>
@@ -5796,7 +5796,7 @@
         <v>-17.93144710419026</v>
       </c>
       <c r="J132" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K132" t="b">
         <v>0</v>
@@ -5836,7 +5836,7 @@
         <v>-11.84038380620835</v>
       </c>
       <c r="J133" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K133" t="b">
         <v>0</v>
@@ -5916,7 +5916,7 @@
         <v>-16.29308794843877</v>
       </c>
       <c r="J135" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K135" t="b">
         <v>0</v>
@@ -6276,7 +6276,7 @@
         <v>20.92562740792459</v>
       </c>
       <c r="J144" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K144" t="b">
         <v>0</v>
@@ -6316,7 +6316,7 @@
         <v>-1.190735470056644</v>
       </c>
       <c r="J145" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K145" t="b">
         <v>0</v>
@@ -6968,7 +6968,7 @@
         <v>-19.52762854189784</v>
       </c>
       <c r="J161" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K161" t="b">
         <v>0</v>
@@ -7088,7 +7088,7 @@
         <v>2.389421059170124</v>
       </c>
       <c r="J164" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K164" t="b">
         <v>0</v>
@@ -7248,7 +7248,7 @@
         <v>-15.97653267700319</v>
       </c>
       <c r="J168" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K168" t="b">
         <v>0</v>
@@ -7408,7 +7408,7 @@
         <v>-3.513577102122658</v>
       </c>
       <c r="J172" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K172" t="b">
         <v>0</v>
@@ -7448,7 +7448,7 @@
         <v>66.6628647616337</v>
       </c>
       <c r="J173" t="n">
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
       <c r="K173" t="b">
         <v>1</v>
@@ -8052,7 +8052,7 @@
         <v>-2.090806463705334</v>
       </c>
       <c r="J188" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K188" t="b">
         <v>0</v>
@@ -8172,7 +8172,7 @@
         <v>-35.88781794455505</v>
       </c>
       <c r="J191" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K191" t="b">
         <v>0</v>
@@ -8252,7 +8252,7 @@
         <v>-12.26553879250178</v>
       </c>
       <c r="J193" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K193" t="b">
         <v>0</v>
@@ -8340,7 +8340,7 @@
         <v>-16.61065655844157</v>
       </c>
       <c r="J195" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K195" t="b">
         <v>0</v>
@@ -8540,7 +8540,7 @@
         <v>1.046832409288845</v>
       </c>
       <c r="J200" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K200" t="b">
         <v>0</v>
@@ -8620,7 +8620,7 @@
         <v>-7.532973615214416</v>
       </c>
       <c r="J202" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K202" t="b">
         <v>0</v>
@@ -8660,7 +8660,7 @@
         <v>-15.68666441754651</v>
       </c>
       <c r="J203" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K203" t="b">
         <v>0</v>
@@ -8700,7 +8700,7 @@
         <v>-4.853434536256496</v>
       </c>
       <c r="J204" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K204" t="b">
         <v>0</v>
@@ -8740,7 +8740,7 @@
         <v>-14.9165130167515</v>
       </c>
       <c r="J205" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K205" t="b">
         <v>0</v>
@@ -8780,7 +8780,7 @@
         <v>2.905883419452508</v>
       </c>
       <c r="J206" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K206" t="b">
         <v>0</v>
@@ -9060,7 +9060,7 @@
         <v>-1.248286493569382</v>
       </c>
       <c r="J213" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K213" t="b">
         <v>0</v>
@@ -9100,7 +9100,7 @@
         <v>-22.68415905786022</v>
       </c>
       <c r="J214" t="n">
-        <v>0.04</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K214" t="b">
         <v>0</v>
@@ -9140,7 +9140,7 @@
         <v>-3.287565598806175</v>
       </c>
       <c r="J215" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K215" t="b">
         <v>0</v>
@@ -9220,7 +9220,7 @@
         <v>3.945279934292688</v>
       </c>
       <c r="J217" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K217" t="b">
         <v>0</v>
@@ -9260,7 +9260,7 @@
         <v>26.22562127291115</v>
       </c>
       <c r="J218" t="n">
-        <v>0.6533333333333333</v>
+        <v>0.7733333333333333</v>
       </c>
       <c r="K218" t="b">
         <v>1</v>
@@ -9344,7 +9344,7 @@
         <v>-11.54370801710428</v>
       </c>
       <c r="J220" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K220" t="b">
         <v>0</v>
@@ -9384,7 +9384,7 @@
         <v>-14.5006863679377</v>
       </c>
       <c r="J221" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K221" t="b">
         <v>0</v>
@@ -9424,7 +9424,7 @@
         <v>-13.46085981617814</v>
       </c>
       <c r="J222" t="n">
-        <v>0.02</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K222" t="b">
         <v>0</v>
@@ -9464,7 +9464,7 @@
         <v>3.561986898496721</v>
       </c>
       <c r="J223" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.04</v>
       </c>
       <c r="K223" t="b">
         <v>0</v>
@@ -9664,7 +9664,7 @@
         <v>-7.047057697558206</v>
       </c>
       <c r="J228" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K228" t="b">
         <v>0</v>
@@ -9744,7 +9744,7 @@
         <v>3.497110880270336</v>
       </c>
       <c r="J230" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.02</v>
       </c>
       <c r="K230" t="b">
         <v>0</v>
@@ -9824,7 +9824,7 @@
         <v>-21.8776275833068</v>
       </c>
       <c r="J232" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K232" t="b">
         <v>0</v>
@@ -9944,7 +9944,7 @@
         <v>-27.32384950826589</v>
       </c>
       <c r="J235" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K235" t="b">
         <v>0</v>
@@ -10024,7 +10024,7 @@
         <v>-43.76879679502572</v>
       </c>
       <c r="J237" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K237" t="b">
         <v>0</v>
@@ -10228,7 +10228,7 @@
         <v>-8.159484776092002</v>
       </c>
       <c r="J242" t="n">
-        <v>0</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K242" t="b">
         <v>0</v>
@@ -10308,7 +10308,7 @@
         <v>4.666919234985784</v>
       </c>
       <c r="J244" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K244" t="b">
         <v>0</v>
@@ -10428,7 +10428,7 @@
         <v>2525.507647713709</v>
       </c>
       <c r="J247" t="n">
-        <v>0.8133333333333334</v>
+        <v>0.84</v>
       </c>
       <c r="K247" t="b">
         <v>1</v>
@@ -10512,7 +10512,7 @@
         <v>-1.492962025010192</v>
       </c>
       <c r="J249" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K249" t="b">
         <v>0</v>
@@ -10552,7 +10552,7 @@
         <v>-16.69381951840755</v>
       </c>
       <c r="J250" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K250" t="b">
         <v>0</v>
@@ -10592,7 +10592,7 @@
         <v>-0.9817093419727571</v>
       </c>
       <c r="J251" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K251" t="b">
         <v>0</v>
@@ -10672,7 +10672,7 @@
         <v>-16.15281694130593</v>
       </c>
       <c r="J253" t="n">
-        <v>0.02</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K253" t="b">
         <v>0</v>
@@ -10952,7 +10952,7 @@
         <v>0.0008543484464590001</v>
       </c>
       <c r="J260" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K260" t="b">
         <v>0</v>
@@ -10992,7 +10992,7 @@
         <v>-2.31383761637606</v>
       </c>
       <c r="J261" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K261" t="b">
         <v>0</v>
@@ -11032,7 +11032,7 @@
         <v>29.82231551932909</v>
       </c>
       <c r="J262" t="n">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="K262" t="b">
         <v>1</v>
@@ -11076,7 +11076,7 @@
         <v>-6.86437034928737</v>
       </c>
       <c r="J263" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K263" t="b">
         <v>0</v>
@@ -11116,7 +11116,7 @@
         <v>-14.56847243700389</v>
       </c>
       <c r="J264" t="n">
-        <v>0.02</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K264" t="b">
         <v>0</v>
@@ -11156,7 +11156,7 @@
         <v>-19.0911853939931</v>
       </c>
       <c r="J265" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K265" t="b">
         <v>0</v>
@@ -11196,7 +11196,7 @@
         <v>-35.03024650942063</v>
       </c>
       <c r="J266" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K266" t="b">
         <v>0</v>
@@ -11236,7 +11236,7 @@
         <v>28.88513513513513</v>
       </c>
       <c r="J267" t="n">
-        <v>0.06</v>
+        <v>0.1133333333333333</v>
       </c>
       <c r="K267" t="b">
         <v>0</v>
@@ -11276,7 +11276,7 @@
         <v>-33.35010980697314</v>
       </c>
       <c r="J268" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K268" t="b">
         <v>0</v>
@@ -11316,7 +11316,7 @@
         <v>-7.061042783279207</v>
       </c>
       <c r="J269" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K269" t="b">
         <v>0</v>
@@ -11396,7 +11396,7 @@
         <v>18.71815613677644</v>
       </c>
       <c r="J271" t="n">
-        <v>0.06</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K271" t="b">
         <v>0</v>
@@ -11476,7 +11476,7 @@
         <v>-17.97829771807034</v>
       </c>
       <c r="J273" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.02</v>
       </c>
       <c r="K273" t="b">
         <v>0</v>
@@ -11556,7 +11556,7 @@
         <v>-18.32687472125039</v>
       </c>
       <c r="J275" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K275" t="b">
         <v>0</v>
@@ -11596,7 +11596,7 @@
         <v>-0.8378535525696531</v>
       </c>
       <c r="J276" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K276" t="b">
         <v>0</v>
@@ -11676,7 +11676,7 @@
         <v>-12.35924248375612</v>
       </c>
       <c r="J278" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K278" t="b">
         <v>0</v>
@@ -11876,7 +11876,7 @@
         <v>-4.227749140768728</v>
       </c>
       <c r="J283" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.04</v>
       </c>
       <c r="K283" t="b">
         <v>0</v>
@@ -11956,7 +11956,7 @@
         <v>-16.00654861182379</v>
       </c>
       <c r="J285" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K285" t="b">
         <v>0</v>
@@ -12076,7 +12076,7 @@
         <v>5.559773032294486</v>
       </c>
       <c r="J288" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K288" t="b">
         <v>0</v>
@@ -12120,7 +12120,7 @@
         <v>-12.48789007620941</v>
       </c>
       <c r="J289" t="n">
-        <v>0.05333333333333334</v>
+        <v>0.04</v>
       </c>
       <c r="K289" t="b">
         <v>0</v>
@@ -12292,7 +12292,7 @@
         <v>-3.233286290414927</v>
       </c>
       <c r="J293" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K293" t="b">
         <v>0</v>
@@ -12412,7 +12412,7 @@
         <v>-0.756420963240059</v>
       </c>
       <c r="J296" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K296" t="b">
         <v>0</v>
@@ -12572,7 +12572,7 @@
         <v>-14.1267229746276</v>
       </c>
       <c r="J300" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K300" t="b">
         <v>0</v>
@@ -12652,7 +12652,7 @@
         <v>21.18961591278832</v>
       </c>
       <c r="J302" t="n">
-        <v>0.4066666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="K302" t="b">
         <v>1</v>
@@ -12696,7 +12696,7 @@
         <v>-8.65285976745222</v>
       </c>
       <c r="J303" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K303" t="b">
         <v>0</v>
@@ -12816,7 +12816,7 @@
         <v>-15.16888882484637</v>
       </c>
       <c r="J306" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K306" t="b">
         <v>0</v>
@@ -13016,7 +13016,7 @@
         <v>4.392008408060252</v>
       </c>
       <c r="J311" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K311" t="b">
         <v>0</v>
@@ -13056,7 +13056,7 @@
         <v>-9.269192371854864</v>
       </c>
       <c r="J312" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K312" t="b">
         <v>0</v>
@@ -13140,7 +13140,7 @@
         <v>0.116753765151209</v>
       </c>
       <c r="J314" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K314" t="b">
         <v>0</v>
@@ -13220,7 +13220,7 @@
         <v>159.2683749555226</v>
       </c>
       <c r="J316" t="n">
-        <v>0.86</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="K316" t="b">
         <v>1</v>
@@ -13264,7 +13264,7 @@
         <v>-4.551014439902161</v>
       </c>
       <c r="J317" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K317" t="b">
         <v>0</v>
@@ -13304,7 +13304,7 @@
         <v>-10.65008778482681</v>
       </c>
       <c r="J318" t="n">
-        <v>0.06</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K318" t="b">
         <v>0</v>
@@ -13344,7 +13344,7 @@
         <v>-8.53412708937161</v>
       </c>
       <c r="J319" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K319" t="b">
         <v>0</v>
@@ -13384,7 +13384,7 @@
         <v>37.21380388528376</v>
       </c>
       <c r="J320" t="n">
-        <v>0.8866666666666667</v>
+        <v>0.8266666666666667</v>
       </c>
       <c r="K320" t="b">
         <v>1</v>
@@ -13468,7 +13468,7 @@
         <v>-31.17611753946589</v>
       </c>
       <c r="J322" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K322" t="b">
         <v>0</v>
@@ -13508,7 +13508,7 @@
         <v>-2.709078235406632</v>
       </c>
       <c r="J323" t="n">
-        <v>0.04</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K323" t="b">
         <v>0</v>
@@ -13628,7 +13628,7 @@
         <v>-0.047427938148765</v>
       </c>
       <c r="J326" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K326" t="b">
         <v>0</v>
@@ -13708,7 +13708,7 @@
         <v>-22.68250106939329</v>
       </c>
       <c r="J328" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K328" t="b">
         <v>0</v>
@@ -13868,7 +13868,7 @@
         <v>43.17450146034166</v>
       </c>
       <c r="J332" t="n">
-        <v>0.84</v>
+        <v>0.8466666666666667</v>
       </c>
       <c r="K332" t="b">
         <v>1</v>
@@ -13912,7 +13912,7 @@
         <v>-13.62772268067522</v>
       </c>
       <c r="J333" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.02</v>
       </c>
       <c r="K333" t="b">
         <v>0</v>
@@ -13952,7 +13952,7 @@
         <v>-0.060574824621586</v>
       </c>
       <c r="J334" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K334" t="b">
         <v>0</v>
@@ -13992,7 +13992,7 @@
         <v>266.4637033990667</v>
       </c>
       <c r="J335" t="n">
-        <v>0.76</v>
+        <v>0.7866666666666666</v>
       </c>
       <c r="K335" t="b">
         <v>1</v>
@@ -14084,7 +14084,7 @@
         <v>-21.36335714978747</v>
       </c>
       <c r="J337" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K337" t="b">
         <v>0</v>
@@ -14168,7 +14168,7 @@
         <v>-0.8430173740105851</v>
       </c>
       <c r="J339" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K339" t="b">
         <v>0</v>
@@ -14208,7 +14208,7 @@
         <v>-16.28692181705772</v>
       </c>
       <c r="J340" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K340" t="b">
         <v>0</v>
@@ -14248,7 +14248,7 @@
         <v>-20.13485927990476</v>
       </c>
       <c r="J341" t="n">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K341" t="b">
         <v>0</v>
@@ -14288,7 +14288,7 @@
         <v>-29.19520734166939</v>
       </c>
       <c r="J342" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K342" t="b">
         <v>0</v>
@@ -14328,7 +14328,7 @@
         <v>-21.31820318937763</v>
       </c>
       <c r="J343" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K343" t="b">
         <v>0</v>
@@ -14408,7 +14408,7 @@
         <v>0.543455327093184</v>
       </c>
       <c r="J345" t="n">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K345" t="b">
         <v>0</v>
@@ -14488,7 +14488,7 @@
         <v>-4.011050559946679</v>
       </c>
       <c r="J347" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K347" t="b">
         <v>0</v>
@@ -14528,7 +14528,7 @@
         <v>23.925163867219</v>
       </c>
       <c r="J348" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.88</v>
       </c>
       <c r="K348" t="b">
         <v>1</v>
@@ -14572,7 +14572,7 @@
         <v>-18.67734229487051</v>
       </c>
       <c r="J349" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K349" t="b">
         <v>0</v>
@@ -14812,7 +14812,7 @@
         <v>0.358636478921627</v>
       </c>
       <c r="J355" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K355" t="b">
         <v>0</v>
@@ -15052,7 +15052,7 @@
         <v>19.85002231336454</v>
       </c>
       <c r="J361" t="n">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="K361" t="b">
         <v>0</v>
@@ -15092,7 +15092,7 @@
         <v>-15.893109279352</v>
       </c>
       <c r="J362" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K362" t="b">
         <v>0</v>
@@ -15212,7 +15212,7 @@
         <v>19.18852432655161</v>
       </c>
       <c r="J365" t="n">
-        <v>0.62</v>
+        <v>0.6266666666666667</v>
       </c>
       <c r="K365" t="b">
         <v>1</v>
@@ -15296,7 +15296,7 @@
         <v>13701.95877798988</v>
       </c>
       <c r="J367" t="n">
-        <v>0.6466666666666666</v>
+        <v>0.7866666666666666</v>
       </c>
       <c r="K367" t="b">
         <v>1</v>
@@ -15380,7 +15380,7 @@
         <v>-21.77795502089348</v>
       </c>
       <c r="J369" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K369" t="b">
         <v>0</v>
@@ -15420,7 +15420,7 @@
         <v>-15.23149167880798</v>
       </c>
       <c r="J370" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K370" t="b">
         <v>0</v>
@@ -15540,7 +15540,7 @@
         <v>80.44094641780181</v>
       </c>
       <c r="J373" t="n">
-        <v>0.1466666666666667</v>
+        <v>0.16</v>
       </c>
       <c r="K373" t="b">
         <v>0</v>
@@ -15620,7 +15620,7 @@
         <v>-26.89075749106678</v>
       </c>
       <c r="J375" t="n">
-        <v>0.04666666666666667</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K375" t="b">
         <v>0</v>
@@ -15740,7 +15740,7 @@
         <v>-18.19267425855399</v>
       </c>
       <c r="J378" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="K378" t="b">
         <v>0</v>
@@ -15780,7 +15780,7 @@
         <v>34.3077215472813</v>
       </c>
       <c r="J379" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.06</v>
       </c>
       <c r="K379" t="b">
         <v>0</v>
@@ -15986,6 +15986,1866 @@
         <v>0</v>
       </c>
       <c r="L384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>Alchemist AI</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>alch</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52302/large/small-logo.png?1733053544</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>/charts/alch_chart.png</t>
+        </is>
+      </c>
+      <c r="E385" t="n">
+        <v>112070389</v>
+      </c>
+      <c r="F385" t="n">
+        <v>0.131894</v>
+      </c>
+      <c r="G385" t="n">
+        <v>-2.115461700264835</v>
+      </c>
+      <c r="H385" t="n">
+        <v>0.171357510626919</v>
+      </c>
+      <c r="I385" t="n">
+        <v>-2.316426379109076</v>
+      </c>
+      <c r="J385" t="n">
+        <v>0</v>
+      </c>
+      <c r="K385" t="b">
+        <v>0</v>
+      </c>
+      <c r="L385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>Solar</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>sxp</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/9368/large/Solar_Blockchain_Foundation_Sun_CG.png?1742975137</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>/charts/sxp_chart.png</t>
+        </is>
+      </c>
+      <c r="E386" t="n">
+        <v>111136045</v>
+      </c>
+      <c r="F386" t="n">
+        <v>0.171718</v>
+      </c>
+      <c r="G386" t="n">
+        <v>-1.921646624666889</v>
+      </c>
+      <c r="H386" t="n">
+        <v>3.759937084759865</v>
+      </c>
+      <c r="I386" t="n">
+        <v>-3.403403677417287</v>
+      </c>
+      <c r="J386" t="n">
+        <v>0</v>
+      </c>
+      <c r="K386" t="b">
+        <v>0</v>
+      </c>
+      <c r="L386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>Nano</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>xno</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/756/large/nano.png?1696501910</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>/charts/xno_chart.png</t>
+        </is>
+      </c>
+      <c r="E387" t="n">
+        <v>111039204</v>
+      </c>
+      <c r="F387" t="n">
+        <v>0.833191</v>
+      </c>
+      <c r="G387" t="n">
+        <v>-1.653172367319784</v>
+      </c>
+      <c r="H387" t="n">
+        <v>-3.131010820706118</v>
+      </c>
+      <c r="I387" t="n">
+        <v>-19.27255073417001</v>
+      </c>
+      <c r="J387" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K387" t="b">
+        <v>0</v>
+      </c>
+      <c r="L387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>Solayer Staked SOL</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>ssol</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39933/large/Green_Back_01a_%282%29.png?1744950020</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr"/>
+      <c r="E388" t="n">
+        <v>110701788</v>
+      </c>
+      <c r="F388" t="n">
+        <v>162.06</v>
+      </c>
+      <c r="G388" t="n">
+        <v>-2.587098361616363</v>
+      </c>
+      <c r="H388" t="n">
+        <v>-3.028850720896867</v>
+      </c>
+      <c r="I388" t="n">
+        <v>-0.409410595247796</v>
+      </c>
+      <c r="J388" t="n">
+        <v>0</v>
+      </c>
+      <c r="K388" t="b">
+        <v>0</v>
+      </c>
+      <c r="L388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>ViciCoin</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>vcnt</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/31305/large/ViciCoin_-_small.png?1696530124</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr"/>
+      <c r="E389" t="n">
+        <v>110643844</v>
+      </c>
+      <c r="F389" t="n">
+        <v>19.41</v>
+      </c>
+      <c r="G389" t="n">
+        <v>-0.425210346803901</v>
+      </c>
+      <c r="H389" t="n">
+        <v>-0.28363234236042</v>
+      </c>
+      <c r="I389" t="n">
+        <v>-0.883416721374863</v>
+      </c>
+      <c r="J389" t="n">
+        <v>0</v>
+      </c>
+      <c r="K389" t="b">
+        <v>0</v>
+      </c>
+      <c r="L389" t="inlineStr"/>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>BORA</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>bora</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/7646/large/mqFw8hxm_400x400.jpeg?1696507900</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr"/>
+      <c r="E390" t="n">
+        <v>110330475</v>
+      </c>
+      <c r="F390" t="n">
+        <v>0.095708</v>
+      </c>
+      <c r="G390" t="n">
+        <v>-1.744924675626522</v>
+      </c>
+      <c r="H390" t="n">
+        <v>-9.147581973674095</v>
+      </c>
+      <c r="I390" t="n">
+        <v>10.10831411126945</v>
+      </c>
+      <c r="J390" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K390" t="b">
+        <v>0</v>
+      </c>
+      <c r="L390" t="inlineStr"/>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>Lorenzo stBTC</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>stbtc</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/50978/large/a.jpg?1730208372</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr"/>
+      <c r="E391" t="n">
+        <v>110281061</v>
+      </c>
+      <c r="F391" t="n">
+        <v>107465</v>
+      </c>
+      <c r="G391" t="n">
+        <v>-1.276110370181595</v>
+      </c>
+      <c r="H391" t="n">
+        <v>0.912645422247764</v>
+      </c>
+      <c r="I391" t="n">
+        <v>2.490034337162576</v>
+      </c>
+      <c r="J391" t="n">
+        <v>0</v>
+      </c>
+      <c r="K391" t="b">
+        <v>0</v>
+      </c>
+      <c r="L391" t="inlineStr"/>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>Level USD</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>lvlusd</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/53150/large/lvlusd-logo.png?1735406507</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr"/>
+      <c r="E392" t="n">
+        <v>109884507</v>
+      </c>
+      <c r="F392" t="n">
+        <v>0.9997189999999999</v>
+      </c>
+      <c r="G392" t="n">
+        <v>0.030284335013107</v>
+      </c>
+      <c r="H392" t="n">
+        <v>-0.04823158811917101</v>
+      </c>
+      <c r="I392" t="n">
+        <v>-0.01658825450012</v>
+      </c>
+      <c r="J392" t="n">
+        <v>0</v>
+      </c>
+      <c r="K392" t="b">
+        <v>0</v>
+      </c>
+      <c r="L392" t="inlineStr"/>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>Chintai</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>chex</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/10349/large/logo-white-bg-dark.png?1733475849</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr"/>
+      <c r="E393" t="n">
+        <v>109684345</v>
+      </c>
+      <c r="F393" t="n">
+        <v>0.109803</v>
+      </c>
+      <c r="G393" t="n">
+        <v>-11.41363254663542</v>
+      </c>
+      <c r="H393" t="n">
+        <v>-24.83804125682378</v>
+      </c>
+      <c r="I393" t="n">
+        <v>-42.57130740671312</v>
+      </c>
+      <c r="J393" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="K393" t="b">
+        <v>0</v>
+      </c>
+      <c r="L393" t="inlineStr"/>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>AWE Network</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>awe</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/8713/large/awe-network.jpg?1747816016</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr"/>
+      <c r="E394" t="n">
+        <v>109495163</v>
+      </c>
+      <c r="F394" t="n">
+        <v>0.056447</v>
+      </c>
+      <c r="G394" t="n">
+        <v>-0.6294275587850371</v>
+      </c>
+      <c r="H394" t="n">
+        <v>1.200641411191949</v>
+      </c>
+      <c r="I394" t="n">
+        <v>10.76738933375865</v>
+      </c>
+      <c r="J394" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="K394" t="b">
+        <v>0</v>
+      </c>
+      <c r="L394" t="inlineStr"/>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>Amnis Aptos</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>amapt</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/32567/large/amAPT.png?1730240666</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr"/>
+      <c r="E395" t="n">
+        <v>109329899</v>
+      </c>
+      <c r="F395" t="n">
+        <v>4.34</v>
+      </c>
+      <c r="G395" t="n">
+        <v>-2.388195628760377</v>
+      </c>
+      <c r="H395" t="n">
+        <v>-10.93727348694143</v>
+      </c>
+      <c r="I395" t="n">
+        <v>-8.463204051357451</v>
+      </c>
+      <c r="J395" t="n">
+        <v>0</v>
+      </c>
+      <c r="K395" t="b">
+        <v>0</v>
+      </c>
+      <c r="L395" t="inlineStr"/>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>Ontology</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>ont</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/3447/large/ONT.png?1696504138</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr"/>
+      <c r="E396" t="n">
+        <v>109069737</v>
+      </c>
+      <c r="F396" t="n">
+        <v>0.119244</v>
+      </c>
+      <c r="G396" t="n">
+        <v>-2.728582957980613</v>
+      </c>
+      <c r="H396" t="n">
+        <v>0.181235177663725</v>
+      </c>
+      <c r="I396" t="n">
+        <v>-13.43698847755994</v>
+      </c>
+      <c r="J396" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K396" t="b">
+        <v>0</v>
+      </c>
+      <c r="L396" t="inlineStr"/>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>World Mobile Token</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>wmtx</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/17333/large/Token_icon_round_1024.png?1741247846</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr"/>
+      <c r="E397" t="n">
+        <v>108961277</v>
+      </c>
+      <c r="F397" t="n">
+        <v>0.145943</v>
+      </c>
+      <c r="G397" t="n">
+        <v>-0.214983316712133</v>
+      </c>
+      <c r="H397" t="n">
+        <v>-4.892228220026445</v>
+      </c>
+      <c r="I397" t="n">
+        <v>-13.01382461034718</v>
+      </c>
+      <c r="J397" t="n">
+        <v>0</v>
+      </c>
+      <c r="K397" t="b">
+        <v>0</v>
+      </c>
+      <c r="L397" t="inlineStr"/>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>Magic Eden</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39850/large/_ME_Profile_Dark_2x.png?1734013082</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr"/>
+      <c r="E398" t="n">
+        <v>108943159</v>
+      </c>
+      <c r="F398" t="n">
+        <v>0.7257779999999999</v>
+      </c>
+      <c r="G398" t="n">
+        <v>-2.29477689930092</v>
+      </c>
+      <c r="H398" t="n">
+        <v>-0.007989541290359</v>
+      </c>
+      <c r="I398" t="n">
+        <v>-16.25296316576334</v>
+      </c>
+      <c r="J398" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K398" t="b">
+        <v>0</v>
+      </c>
+      <c r="L398" t="inlineStr"/>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>Apollo Diversified Credit Securitize Fund</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>acred</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54809/large/ACRED.png?1741801356</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr"/>
+      <c r="E399" t="n">
+        <v>108671111</v>
+      </c>
+      <c r="F399" t="n">
+        <v>1035.72</v>
+      </c>
+      <c r="G399" t="n">
+        <v>-0.004749977626563</v>
+      </c>
+      <c r="H399" t="n">
+        <v>0.196974865556406</v>
+      </c>
+      <c r="I399" t="n">
+        <v>0.9143018892115361</v>
+      </c>
+      <c r="J399" t="n">
+        <v>0</v>
+      </c>
+      <c r="K399" t="b">
+        <v>0</v>
+      </c>
+      <c r="L399" t="inlineStr"/>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>COTI</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>coti</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/2962/large/Coti.png?1696503705</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr"/>
+      <c r="E400" t="n">
+        <v>108072036</v>
+      </c>
+      <c r="F400" t="n">
+        <v>0.04881149</v>
+      </c>
+      <c r="G400" t="n">
+        <v>-3.186094782178738</v>
+      </c>
+      <c r="H400" t="n">
+        <v>-4.258192262654258</v>
+      </c>
+      <c r="I400" t="n">
+        <v>-16.89699918439059</v>
+      </c>
+      <c r="J400" t="n">
+        <v>0</v>
+      </c>
+      <c r="K400" t="b">
+        <v>0</v>
+      </c>
+      <c r="L400" t="inlineStr"/>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>Osmosis</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>osmo</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/16724/large/osmo.png?1696516298</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr"/>
+      <c r="E401" t="n">
+        <v>108024047</v>
+      </c>
+      <c r="F401" t="n">
+        <v>0.146798</v>
+      </c>
+      <c r="G401" t="n">
+        <v>0.7884676629607491</v>
+      </c>
+      <c r="H401" t="n">
+        <v>4.782349487386696</v>
+      </c>
+      <c r="I401" t="n">
+        <v>-26.39629894322639</v>
+      </c>
+      <c r="J401" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K401" t="b">
+        <v>0</v>
+      </c>
+      <c r="L401" t="inlineStr"/>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>sBTC</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>sbtc</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54285/large/sbtc-logo-orange-bg-white-circle-1000px_2.png?1739000556</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr"/>
+      <c r="E402" t="n">
+        <v>107990041</v>
+      </c>
+      <c r="F402" t="n">
+        <v>107980</v>
+      </c>
+      <c r="G402" t="n">
+        <v>0.000209522085396</v>
+      </c>
+      <c r="H402" t="n">
+        <v>0.96044647373809</v>
+      </c>
+      <c r="I402" t="n">
+        <v>2.444250700483026</v>
+      </c>
+      <c r="J402" t="n">
+        <v>0</v>
+      </c>
+      <c r="K402" t="b">
+        <v>0</v>
+      </c>
+      <c r="L402" t="inlineStr"/>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>Zenrock BTC</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>zenbtc</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55147/large/zen_brandmark_%28blue%29_%281%29.png?1745550508</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr"/>
+      <c r="E403" t="n">
+        <v>107897368</v>
+      </c>
+      <c r="F403" t="n">
+        <v>107897</v>
+      </c>
+      <c r="G403" t="n">
+        <v>-1.228478231239065</v>
+      </c>
+      <c r="H403" t="n">
+        <v>0.359221852024467</v>
+      </c>
+      <c r="I403" t="n">
+        <v>1.635839035844116</v>
+      </c>
+      <c r="J403" t="n">
+        <v>0</v>
+      </c>
+      <c r="K403" t="b">
+        <v>0</v>
+      </c>
+      <c r="L403" t="inlineStr"/>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>Paycoin</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>pci</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/9330/large/new_logo_square.png?1696509434</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr"/>
+      <c r="E404" t="n">
+        <v>107041395</v>
+      </c>
+      <c r="F404" t="n">
+        <v>0.104678</v>
+      </c>
+      <c r="G404" t="n">
+        <v>-7.122350559942456</v>
+      </c>
+      <c r="H404" t="n">
+        <v>-0.8461000028928861</v>
+      </c>
+      <c r="I404" t="n">
+        <v>57.09169107227211</v>
+      </c>
+      <c r="J404" t="n">
+        <v>0.1133333333333333</v>
+      </c>
+      <c r="K404" t="b">
+        <v>0</v>
+      </c>
+      <c r="L404" t="inlineStr"/>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>Centrifuge [OLD]</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>cfg</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/15380/large/centrifuge.PNG?1696515027</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr"/>
+      <c r="E405" t="n">
+        <v>106621922</v>
+      </c>
+      <c r="F405" t="n">
+        <v>0.19015</v>
+      </c>
+      <c r="G405" t="n">
+        <v>-8.908959798799927</v>
+      </c>
+      <c r="H405" t="n">
+        <v>11.05909825126799</v>
+      </c>
+      <c r="I405" t="n">
+        <v>7.287386578484954</v>
+      </c>
+      <c r="J405" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K405" t="b">
+        <v>0</v>
+      </c>
+      <c r="L405" t="inlineStr"/>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>Babylon</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>baby</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55092/large/Baby-Symbol-Mint_%281%29.png?1744788866</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr"/>
+      <c r="E406" t="n">
+        <v>106557960</v>
+      </c>
+      <c r="F406" t="n">
+        <v>0.04645102</v>
+      </c>
+      <c r="G406" t="n">
+        <v>-6.837403927901804</v>
+      </c>
+      <c r="H406" t="n">
+        <v>-2.204797728955765</v>
+      </c>
+      <c r="I406" t="n">
+        <v>-27.36379578329637</v>
+      </c>
+      <c r="J406" t="n">
+        <v>0</v>
+      </c>
+      <c r="K406" t="b">
+        <v>0</v>
+      </c>
+      <c r="L406" t="inlineStr"/>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>Ozone Chain</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>ozo</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/31385/large/ozonechain-momogram-200x200.png?1696530201</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr"/>
+      <c r="E407" t="n">
+        <v>106356759</v>
+      </c>
+      <c r="F407" t="n">
+        <v>0.127745</v>
+      </c>
+      <c r="G407" t="n">
+        <v>-2.619106904430868</v>
+      </c>
+      <c r="H407" t="n">
+        <v>-1.050927827612261</v>
+      </c>
+      <c r="I407" t="n">
+        <v>-3.084471549414936</v>
+      </c>
+      <c r="J407" t="n">
+        <v>0</v>
+      </c>
+      <c r="K407" t="b">
+        <v>0</v>
+      </c>
+      <c r="L407" t="inlineStr"/>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>Undeads Games</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>uds</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/36308/large/01_avatar.jpg?1711090303</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr"/>
+      <c r="E408" t="n">
+        <v>106265248</v>
+      </c>
+      <c r="F408" t="n">
+        <v>1.051</v>
+      </c>
+      <c r="G408" t="n">
+        <v>-0.197546726373764</v>
+      </c>
+      <c r="H408" t="n">
+        <v>-9.978897479118739</v>
+      </c>
+      <c r="I408" t="n">
+        <v>18.6816527210375</v>
+      </c>
+      <c r="J408" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="K408" t="b">
+        <v>0</v>
+      </c>
+      <c r="L408" t="inlineStr"/>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>Purr</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>purr</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/37125/large/PURR_CG.png?1713368828</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr"/>
+      <c r="E409" t="n">
+        <v>106151456</v>
+      </c>
+      <c r="F409" t="n">
+        <v>0.178039</v>
+      </c>
+      <c r="G409" t="n">
+        <v>-9.552678769648661</v>
+      </c>
+      <c r="H409" t="n">
+        <v>-11.40977351557322</v>
+      </c>
+      <c r="I409" t="n">
+        <v>-19.78718861893022</v>
+      </c>
+      <c r="J409" t="n">
+        <v>0</v>
+      </c>
+      <c r="K409" t="b">
+        <v>0</v>
+      </c>
+      <c r="L409" t="inlineStr"/>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>BOOK OF MEME</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>bome</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/36071/large/bome.png?1710407255</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr"/>
+      <c r="E410" t="n">
+        <v>105489868</v>
+      </c>
+      <c r="F410" t="n">
+        <v>0.00153179</v>
+      </c>
+      <c r="G410" t="n">
+        <v>-5.100003308878838</v>
+      </c>
+      <c r="H410" t="n">
+        <v>-0.261103219018307</v>
+      </c>
+      <c r="I410" t="n">
+        <v>-15.16518882818578</v>
+      </c>
+      <c r="J410" t="n">
+        <v>0</v>
+      </c>
+      <c r="K410" t="b">
+        <v>0</v>
+      </c>
+      <c r="L410" t="inlineStr"/>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>snt</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/779/large/status.png?1696501931</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr"/>
+      <c r="E411" t="n">
+        <v>105175316</v>
+      </c>
+      <c r="F411" t="n">
+        <v>0.02654231</v>
+      </c>
+      <c r="G411" t="n">
+        <v>-4.688310145332312</v>
+      </c>
+      <c r="H411" t="n">
+        <v>-1.474372963530206</v>
+      </c>
+      <c r="I411" t="n">
+        <v>-12.35911633799233</v>
+      </c>
+      <c r="J411" t="n">
+        <v>0</v>
+      </c>
+      <c r="K411" t="b">
+        <v>0</v>
+      </c>
+      <c r="L411" t="inlineStr"/>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>LCX</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>lcx</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/9985/large/zRPSu_0o_400x400.jpg?1696510023</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr"/>
+      <c r="E412" t="n">
+        <v>104877674</v>
+      </c>
+      <c r="F412" t="n">
+        <v>0.111455</v>
+      </c>
+      <c r="G412" t="n">
+        <v>-2.466669678281989</v>
+      </c>
+      <c r="H412" t="n">
+        <v>-0.06494326647722901</v>
+      </c>
+      <c r="I412" t="n">
+        <v>-11.85134331021512</v>
+      </c>
+      <c r="J412" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K412" t="b">
+        <v>0</v>
+      </c>
+      <c r="L412" t="inlineStr"/>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>Rocket Pool</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>rpl</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/2090/large/rocket_pool_%28RPL%29.png?1696503058</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr"/>
+      <c r="E413" t="n">
+        <v>104032993</v>
+      </c>
+      <c r="F413" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="G413" t="n">
+        <v>-1.825675257851306</v>
+      </c>
+      <c r="H413" t="n">
+        <v>-1.782677391927074</v>
+      </c>
+      <c r="I413" t="n">
+        <v>-11.17226609030467</v>
+      </c>
+      <c r="J413" t="n">
+        <v>0</v>
+      </c>
+      <c r="K413" t="b">
+        <v>0</v>
+      </c>
+      <c r="L413" t="inlineStr"/>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>Hive</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>hive</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/10840/large/logo_transparent_4x.png?1696510797</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr"/>
+      <c r="E414" t="n">
+        <v>104012929</v>
+      </c>
+      <c r="F414" t="n">
+        <v>0.216285</v>
+      </c>
+      <c r="G414" t="n">
+        <v>2.829267282572865</v>
+      </c>
+      <c r="H414" t="n">
+        <v>7.756967271830177</v>
+      </c>
+      <c r="I414" t="n">
+        <v>-8.305565071363974</v>
+      </c>
+      <c r="J414" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="K414" t="b">
+        <v>0</v>
+      </c>
+      <c r="L414" t="inlineStr"/>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>Request</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>req</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/1031/large/Request_icon_green.png?1696502140</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr"/>
+      <c r="E415" t="n">
+        <v>103606999</v>
+      </c>
+      <c r="F415" t="n">
+        <v>0.13919</v>
+      </c>
+      <c r="G415" t="n">
+        <v>-1.110270792007949</v>
+      </c>
+      <c r="H415" t="n">
+        <v>3.101230323954515</v>
+      </c>
+      <c r="I415" t="n">
+        <v>-3.207831201026868</v>
+      </c>
+      <c r="J415" t="n">
+        <v>0</v>
+      </c>
+      <c r="K415" t="b">
+        <v>0</v>
+      </c>
+      <c r="L415" t="inlineStr"/>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>Sui Bridged USDT (Sui)</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>sbusdt</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/56062/large/usdt.jpg?1748225088</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr"/>
+      <c r="E416" t="n">
+        <v>103133168</v>
+      </c>
+      <c r="F416" t="n">
+        <v>0.9999749999999999</v>
+      </c>
+      <c r="G416" t="n">
+        <v>-0.008298691669175001</v>
+      </c>
+      <c r="H416" t="n">
+        <v>-0.04319993919455</v>
+      </c>
+      <c r="I416" t="n">
+        <v>-0.012658098303397</v>
+      </c>
+      <c r="J416" t="n">
+        <v>0</v>
+      </c>
+      <c r="K416" t="b">
+        <v>0</v>
+      </c>
+      <c r="L416" t="inlineStr"/>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>SWFTCOIN</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>swftc</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/2346/large/SWFTCoin.jpg?1696503223</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr"/>
+      <c r="E417" t="n">
+        <v>101761439</v>
+      </c>
+      <c r="F417" t="n">
+        <v>0.01017706</v>
+      </c>
+      <c r="G417" t="n">
+        <v>-2.026463302975086</v>
+      </c>
+      <c r="H417" t="n">
+        <v>-4.657685644278857</v>
+      </c>
+      <c r="I417" t="n">
+        <v>-13.76071106211771</v>
+      </c>
+      <c r="J417" t="n">
+        <v>0</v>
+      </c>
+      <c r="K417" t="b">
+        <v>0</v>
+      </c>
+      <c r="L417" t="inlineStr"/>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>Acet</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>act</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/18205/large/ACET-LOGO.png?1696517703</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr"/>
+      <c r="E418" t="n">
+        <v>101756816</v>
+      </c>
+      <c r="F418" t="n">
+        <v>0.05951099999999999</v>
+      </c>
+      <c r="G418" t="n">
+        <v>-2.023196425357325</v>
+      </c>
+      <c r="H418" t="n">
+        <v>-1.734367238941677</v>
+      </c>
+      <c r="I418" t="n">
+        <v>-13.12547116681166</v>
+      </c>
+      <c r="J418" t="n">
+        <v>0</v>
+      </c>
+      <c r="K418" t="b">
+        <v>0</v>
+      </c>
+      <c r="L418" t="inlineStr"/>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>RealLink</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/20665/large/TGBfBt6Y2Dm3RHdNpZAdqywBsvfdysf834.jpeg?1749135788</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr"/>
+      <c r="E419" t="n">
+        <v>101348624</v>
+      </c>
+      <c r="F419" t="n">
+        <v>0.03607436</v>
+      </c>
+      <c r="G419" t="n">
+        <v>-1.359653863896551</v>
+      </c>
+      <c r="H419" t="n">
+        <v>24.06744616934971</v>
+      </c>
+      <c r="I419" t="n">
+        <v>64.51589806840326</v>
+      </c>
+      <c r="J419" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="K419" t="b">
+        <v>1</v>
+      </c>
+      <c r="L419" t="inlineStr">
+        <is>
+          <t>Crecimiento mensual sobresaliente (+60%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>Terra</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>luna</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/25767/large/01_Luna_color.png?1696524851</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr"/>
+      <c r="E420" t="n">
+        <v>101172403</v>
+      </c>
+      <c r="F420" t="n">
+        <v>0.147081</v>
+      </c>
+      <c r="G420" t="n">
+        <v>-3.521378274132744</v>
+      </c>
+      <c r="H420" t="n">
+        <v>0.9321928917238971</v>
+      </c>
+      <c r="I420" t="n">
+        <v>-11.44588027320056</v>
+      </c>
+      <c r="J420" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="K420" t="b">
+        <v>0</v>
+      </c>
+      <c r="L420" t="inlineStr"/>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>Solv Protocol SolvBTC Jupiter</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>solvbtc.jup</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54834/large/solvBTC_Jupiter.png?1741969449</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr"/>
+      <c r="E421" t="n">
+        <v>101161501</v>
+      </c>
+      <c r="F421" t="n">
+        <v>113845</v>
+      </c>
+      <c r="G421" t="n">
+        <v>-1.422508981706614</v>
+      </c>
+      <c r="H421" t="n">
+        <v>0.686450759793733</v>
+      </c>
+      <c r="I421" t="n">
+        <v>2.418870753659049</v>
+      </c>
+      <c r="J421" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K421" t="b">
+        <v>0</v>
+      </c>
+      <c r="L421" t="inlineStr"/>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>QL1 Bridged USDT (QL1)</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>qusdt</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52913/large/usdt.jpg?1734677175</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr"/>
+      <c r="E422" t="n">
+        <v>99996010</v>
+      </c>
+      <c r="F422" t="n">
+        <v>0.9999600000000001</v>
+      </c>
+      <c r="G422" t="n">
+        <v>-0.006893851757589001</v>
+      </c>
+      <c r="H422" t="n">
+        <v>-0.026126788035713</v>
+      </c>
+      <c r="I422" t="n">
+        <v>-0.036690557960992</v>
+      </c>
+      <c r="J422" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K422" t="b">
+        <v>0</v>
+      </c>
+      <c r="L422" t="inlineStr"/>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>ONFA</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>oft</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/39159/large/logo-onfa-circle-green.png?1720776070</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr"/>
+      <c r="E423" t="n">
+        <v>99569440</v>
+      </c>
+      <c r="F423" t="n">
+        <v>0.8699359999999999</v>
+      </c>
+      <c r="G423" t="n">
+        <v>3.053352050176332</v>
+      </c>
+      <c r="H423" t="n">
+        <v>139.2336339816779</v>
+      </c>
+      <c r="I423" t="n">
+        <v>278.4348970892472</v>
+      </c>
+      <c r="J423" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K423" t="b">
+        <v>1</v>
+      </c>
+      <c r="L423" t="inlineStr">
+        <is>
+          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>Moonwell</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>well</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/26133/large/WELL.png?1696525221</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr"/>
+      <c r="E424" t="n">
+        <v>97449292</v>
+      </c>
+      <c r="F424" t="n">
+        <v>0.02786171</v>
+      </c>
+      <c r="G424" t="n">
+        <v>-5.088413064368699</v>
+      </c>
+      <c r="H424" t="n">
+        <v>9.238751471336048</v>
+      </c>
+      <c r="I424" t="n">
+        <v>-14.31999929500089</v>
+      </c>
+      <c r="J424" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K424" t="b">
+        <v>0</v>
+      </c>
+      <c r="L424" t="inlineStr"/>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>Tellor Tributes</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>trb</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/9644/large/TRB-New_Logo.png?1737722143</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr"/>
+      <c r="E425" t="n">
+        <v>97252468</v>
+      </c>
+      <c r="F425" t="n">
+        <v>36.19</v>
+      </c>
+      <c r="G425" t="n">
+        <v>-2.397845291095618</v>
+      </c>
+      <c r="H425" t="n">
+        <v>-1.020591601330493</v>
+      </c>
+      <c r="I425" t="n">
+        <v>-25.74847109752198</v>
+      </c>
+      <c r="J425" t="n">
+        <v>0</v>
+      </c>
+      <c r="K425" t="b">
+        <v>0</v>
+      </c>
+      <c r="L425" t="inlineStr"/>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>AltLayer</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>alt</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/34608/large/Logomark_200x200.png?1715107868</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr"/>
+      <c r="E426" t="n">
+        <v>97129494</v>
+      </c>
+      <c r="F426" t="n">
+        <v>0.02586527</v>
+      </c>
+      <c r="G426" t="n">
+        <v>-4.52857432813512</v>
+      </c>
+      <c r="H426" t="n">
+        <v>-0.320436891944607</v>
+      </c>
+      <c r="I426" t="n">
+        <v>-1.91357632706648</v>
+      </c>
+      <c r="J426" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K426" t="b">
+        <v>0</v>
+      </c>
+      <c r="L426" t="inlineStr"/>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>Waves</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>waves</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/425/large/waves.png?1696501700</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr"/>
+      <c r="E427" t="n">
+        <v>97108758</v>
+      </c>
+      <c r="F427" t="n">
+        <v>0.971479</v>
+      </c>
+      <c r="G427" t="n">
+        <v>-2.463754323088179</v>
+      </c>
+      <c r="H427" t="n">
+        <v>1.681799234888228</v>
+      </c>
+      <c r="I427" t="n">
+        <v>-9.695491705106143</v>
+      </c>
+      <c r="J427" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="K427" t="b">
+        <v>0</v>
+      </c>
+      <c r="L427" t="inlineStr"/>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>Venus</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>xvs</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12677/large/XVS_Token.jpg?1727454303</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr"/>
+      <c r="E428" t="n">
+        <v>96694267</v>
+      </c>
+      <c r="F428" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="G428" t="n">
+        <v>-2.641229064024655</v>
+      </c>
+      <c r="H428" t="n">
+        <v>-0.6042645105986431</v>
+      </c>
+      <c r="I428" t="n">
+        <v>-3.864510659080766</v>
+      </c>
+      <c r="J428" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K428" t="b">
+        <v>0</v>
+      </c>
+      <c r="L428" t="inlineStr"/>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>Illuvium</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>ilv</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/14468/large/logo-200x200.png?1696514154</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr"/>
+      <c r="E429" t="n">
+        <v>96421135</v>
+      </c>
+      <c r="F429" t="n">
+        <v>10.19</v>
+      </c>
+      <c r="G429" t="n">
+        <v>-2.207524215727887</v>
+      </c>
+      <c r="H429" t="n">
+        <v>1.093079610024772</v>
+      </c>
+      <c r="I429" t="n">
+        <v>-16.22192345188167</v>
+      </c>
+      <c r="J429" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="K429" t="b">
+        <v>0</v>
+      </c>
+      <c r="L429" t="inlineStr"/>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>BitMart</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>bmx</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/5236/large/bitmart-token.png?1696505741</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr"/>
+      <c r="E430" t="n">
+        <v>96372920</v>
+      </c>
+      <c r="F430" t="n">
+        <v>0.283926</v>
+      </c>
+      <c r="G430" t="n">
+        <v>-1.220919186663259</v>
+      </c>
+      <c r="H430" t="n">
+        <v>0.80366916723916</v>
+      </c>
+      <c r="I430" t="n">
+        <v>2.136232220300422</v>
+      </c>
+      <c r="J430" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="K430" t="b">
+        <v>0</v>
+      </c>
+      <c r="L430" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: actualizar datos de criptomonedas con nuevas predicciones y gráficos
</commit_message>
<xml_diff>
--- a/data/predicciones_criptos.xlsx
+++ b/data/predicciones_criptos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L430"/>
+  <dimension ref="A1:L476"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,7 +532,7 @@
         <v>3.404126761127093</v>
       </c>
       <c r="J2" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
@@ -704,7 +704,7 @@
         <v>-0.969268928301472</v>
       </c>
       <c r="J6" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
@@ -864,7 +864,7 @@
         <v>-12.65917503513083</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K10" t="b">
         <v>0</v>
@@ -984,7 +984,7 @@
         <v>3.310589202212904</v>
       </c>
       <c r="J13" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
@@ -1064,7 +1064,7 @@
         <v>-0.674209286023263</v>
       </c>
       <c r="J15" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K15" t="b">
         <v>0</v>
@@ -1104,7 +1104,7 @@
         <v>-9.331747974351638</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K16" t="b">
         <v>0</v>
@@ -1144,16 +1144,12 @@
         <v>22.08120425105527</v>
       </c>
       <c r="J17" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K17" t="b">
-        <v>1</v>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Buena puntuacion en analisis multivariable</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1188,7 +1184,7 @@
         <v>-4.336743214979863</v>
       </c>
       <c r="J18" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K18" t="b">
         <v>0</v>
@@ -1308,7 +1304,7 @@
         <v>-11.83220447784404</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K21" t="b">
         <v>0</v>
@@ -1468,7 +1464,7 @@
         <v>-10.32749746727879</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K25" t="b">
         <v>0</v>
@@ -1548,7 +1544,7 @@
         <v>-8.852584643610301</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K27" t="b">
         <v>0</v>
@@ -1628,7 +1624,7 @@
         <v>39.17162961148887</v>
       </c>
       <c r="J29" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K29" t="b">
         <v>0</v>
@@ -1908,7 +1904,7 @@
         <v>13.88295718228861</v>
       </c>
       <c r="J36" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K36" t="b">
         <v>0</v>
@@ -1988,7 +1984,7 @@
         <v>-21.11312970592905</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K38" t="b">
         <v>0</v>
@@ -2308,7 +2304,7 @@
         <v>-11.71712559028115</v>
       </c>
       <c r="J46" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K46" t="b">
         <v>0</v>
@@ -2760,7 +2756,7 @@
         <v>-19.01774212095845</v>
       </c>
       <c r="J57" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K57" t="b">
         <v>0</v>
@@ -3044,7 +3040,7 @@
         <v>3.672065484066418</v>
       </c>
       <c r="J64" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K64" t="b">
         <v>0</v>
@@ -3164,7 +3160,7 @@
         <v>-14.20939130068742</v>
       </c>
       <c r="J67" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K67" t="b">
         <v>0</v>
@@ -3244,7 +3240,7 @@
         <v>-9.556828834635429</v>
       </c>
       <c r="J69" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K69" t="b">
         <v>0</v>
@@ -3324,7 +3320,7 @@
         <v>-9.083725837365744</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K71" t="b">
         <v>0</v>
@@ -3444,12 +3440,16 @@
         <v>34.02739822198766</v>
       </c>
       <c r="J74" t="n">
-        <v>0.34</v>
+        <v>0.68</v>
       </c>
       <c r="K74" t="b">
-        <v>0</v>
-      </c>
-      <c r="L74" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Buen rendimiento mensual (+30%) | Buena puntuacion en analisis multivariable</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3724,7 +3724,7 @@
         <v>-5.46076904273847</v>
       </c>
       <c r="J81" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="K81" t="b">
         <v>0</v>
@@ -3844,7 +3844,7 @@
         <v>3.4530988051059</v>
       </c>
       <c r="J84" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.1</v>
       </c>
       <c r="K84" t="b">
         <v>0</v>
@@ -3964,7 +3964,7 @@
         <v>-7.558543714704253</v>
       </c>
       <c r="J87" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K87" t="b">
         <v>0</v>
@@ -4044,7 +4044,7 @@
         <v>-11.37185206377279</v>
       </c>
       <c r="J89" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K89" t="b">
         <v>0</v>
@@ -4284,7 +4284,7 @@
         <v>-0.021382708202666</v>
       </c>
       <c r="J95" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K95" t="b">
         <v>0</v>
@@ -4324,14 +4324,14 @@
         <v>40.64601967701537</v>
       </c>
       <c r="J96" t="n">
-        <v>0.4266666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="K96" t="b">
         <v>1</v>
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>Buen rendimiento mensual (+30%) | Fuerte tendencia semanal (+10%)</t>
+          <t>Buen rendimiento mensual (+30%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
         </is>
       </c>
     </row>
@@ -4408,7 +4408,7 @@
         <v>40.59617452460589</v>
       </c>
       <c r="J98" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.1133333333333333</v>
       </c>
       <c r="K98" t="b">
         <v>0</v>
@@ -4452,7 +4452,7 @@
         <v>-0.886004824973551</v>
       </c>
       <c r="J99" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K99" t="b">
         <v>0</v>
@@ -4580,7 +4580,7 @@
         <v>-10.54919185994349</v>
       </c>
       <c r="J102" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K102" t="b">
         <v>0</v>
@@ -4624,7 +4624,7 @@
         <v>-0.405621828180371</v>
       </c>
       <c r="J103" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K103" t="b">
         <v>0</v>
@@ -4668,7 +4668,7 @@
         <v>-0.472745469733487</v>
       </c>
       <c r="J104" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K104" t="b">
         <v>0</v>
@@ -4712,7 +4712,7 @@
         <v>-21.35993819296908</v>
       </c>
       <c r="J105" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K105" t="b">
         <v>0</v>
@@ -4916,7 +4916,7 @@
         <v>-0.8559408883874851</v>
       </c>
       <c r="J110" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K110" t="b">
         <v>0</v>
@@ -4956,7 +4956,7 @@
         <v>-23.79567837798205</v>
       </c>
       <c r="J111" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K111" t="b">
         <v>0</v>
@@ -5356,7 +5356,7 @@
         <v>-11.02243559720266</v>
       </c>
       <c r="J121" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K121" t="b">
         <v>0</v>
@@ -5516,7 +5516,7 @@
         <v>41.49245405224639</v>
       </c>
       <c r="J125" t="n">
-        <v>0.08</v>
+        <v>0.1133333333333333</v>
       </c>
       <c r="K125" t="b">
         <v>0</v>
@@ -5636,7 +5636,7 @@
         <v>10.32845530727019</v>
       </c>
       <c r="J128" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K128" t="b">
         <v>0</v>
@@ -5836,7 +5836,7 @@
         <v>-11.84038380620835</v>
       </c>
       <c r="J133" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K133" t="b">
         <v>0</v>
@@ -5916,7 +5916,7 @@
         <v>-16.29308794843877</v>
       </c>
       <c r="J135" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K135" t="b">
         <v>0</v>
@@ -6076,7 +6076,7 @@
         <v>-5.75363722103801</v>
       </c>
       <c r="J139" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K139" t="b">
         <v>0</v>
@@ -6276,7 +6276,7 @@
         <v>20.92562740792459</v>
       </c>
       <c r="J144" t="n">
-        <v>0.05333333333333334</v>
+        <v>0.06</v>
       </c>
       <c r="K144" t="b">
         <v>0</v>
@@ -6316,7 +6316,7 @@
         <v>-1.190735470056644</v>
       </c>
       <c r="J145" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K145" t="b">
         <v>0</v>
@@ -6968,7 +6968,7 @@
         <v>-19.52762854189784</v>
       </c>
       <c r="J161" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K161" t="b">
         <v>0</v>
@@ -7088,7 +7088,7 @@
         <v>2.389421059170124</v>
       </c>
       <c r="J164" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K164" t="b">
         <v>0</v>
@@ -7248,7 +7248,7 @@
         <v>-15.97653267700319</v>
       </c>
       <c r="J168" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K168" t="b">
         <v>0</v>
@@ -7408,7 +7408,7 @@
         <v>-3.513577102122658</v>
       </c>
       <c r="J172" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K172" t="b">
         <v>0</v>
@@ -7448,14 +7448,14 @@
         <v>66.6628647616337</v>
       </c>
       <c r="J173" t="n">
-        <v>0.44</v>
+        <v>0.86</v>
       </c>
       <c r="K173" t="b">
         <v>1</v>
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>Crecimiento mensual sobresaliente (+60%) | Fuerte tendencia semanal (+10%)</t>
+          <t>Crecimiento mensual sobresaliente (+60%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
         </is>
       </c>
     </row>
@@ -7492,7 +7492,7 @@
         <v>5.317709580767196</v>
       </c>
       <c r="J174" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K174" t="b">
         <v>0</v>
@@ -7692,7 +7692,7 @@
         <v>3.166285552351646</v>
       </c>
       <c r="J179" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K179" t="b">
         <v>0</v>
@@ -8052,7 +8052,7 @@
         <v>-2.090806463705334</v>
       </c>
       <c r="J188" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K188" t="b">
         <v>0</v>
@@ -8172,7 +8172,7 @@
         <v>-35.88781794455505</v>
       </c>
       <c r="J191" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K191" t="b">
         <v>0</v>
@@ -8212,7 +8212,7 @@
         <v>-24.11678545003828</v>
       </c>
       <c r="J192" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K192" t="b">
         <v>0</v>
@@ -8340,7 +8340,7 @@
         <v>-16.61065655844157</v>
       </c>
       <c r="J195" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K195" t="b">
         <v>0</v>
@@ -8540,7 +8540,7 @@
         <v>1.046832409288845</v>
       </c>
       <c r="J200" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K200" t="b">
         <v>0</v>
@@ -8700,7 +8700,7 @@
         <v>-4.853434536256496</v>
       </c>
       <c r="J204" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="K204" t="b">
         <v>0</v>
@@ -8780,7 +8780,7 @@
         <v>2.905883419452508</v>
       </c>
       <c r="J206" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K206" t="b">
         <v>0</v>
@@ -9060,7 +9060,7 @@
         <v>-1.248286493569382</v>
       </c>
       <c r="J213" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K213" t="b">
         <v>0</v>
@@ -9100,7 +9100,7 @@
         <v>-22.68415905786022</v>
       </c>
       <c r="J214" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.02</v>
       </c>
       <c r="K214" t="b">
         <v>0</v>
@@ -9220,7 +9220,7 @@
         <v>3.945279934292688</v>
       </c>
       <c r="J217" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K217" t="b">
         <v>0</v>
@@ -9260,16 +9260,12 @@
         <v>26.22562127291115</v>
       </c>
       <c r="J218" t="n">
-        <v>0.7733333333333333</v>
+        <v>0.2266666666666667</v>
       </c>
       <c r="K218" t="b">
-        <v>1</v>
-      </c>
-      <c r="L218" t="inlineStr">
-        <is>
-          <t>Buena puntuacion en analisis multivariable</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -9304,7 +9300,7 @@
         <v>0.02617310131229</v>
       </c>
       <c r="J219" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K219" t="b">
         <v>0</v>
@@ -9344,7 +9340,7 @@
         <v>-11.54370801710428</v>
       </c>
       <c r="J220" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K220" t="b">
         <v>0</v>
@@ -9384,7 +9380,7 @@
         <v>-14.5006863679377</v>
       </c>
       <c r="J221" t="n">
-        <v>0.02666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K221" t="b">
         <v>0</v>
@@ -9424,7 +9420,7 @@
         <v>-13.46085981617814</v>
       </c>
       <c r="J222" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K222" t="b">
         <v>0</v>
@@ -9464,7 +9460,7 @@
         <v>3.561986898496721</v>
       </c>
       <c r="J223" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="K223" t="b">
         <v>0</v>
@@ -9504,7 +9500,7 @@
         <v>-0.4917969429396941</v>
       </c>
       <c r="J224" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K224" t="b">
         <v>0</v>
@@ -9664,7 +9660,7 @@
         <v>-7.047057697558206</v>
       </c>
       <c r="J228" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K228" t="b">
         <v>0</v>
@@ -9744,7 +9740,7 @@
         <v>3.497110880270336</v>
       </c>
       <c r="J230" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K230" t="b">
         <v>0</v>
@@ -9824,7 +9820,7 @@
         <v>-21.8776275833068</v>
       </c>
       <c r="J232" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.02</v>
       </c>
       <c r="K232" t="b">
         <v>0</v>
@@ -9944,7 +9940,7 @@
         <v>-27.32384950826589</v>
       </c>
       <c r="J235" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K235" t="b">
         <v>0</v>
@@ -10024,7 +10020,7 @@
         <v>-43.76879679502572</v>
       </c>
       <c r="J237" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K237" t="b">
         <v>0</v>
@@ -10064,7 +10060,7 @@
         <v>-2.501966759931275</v>
       </c>
       <c r="J238" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K238" t="b">
         <v>0</v>
@@ -10228,7 +10224,7 @@
         <v>-8.159484776092002</v>
       </c>
       <c r="J242" t="n">
-        <v>0.02666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K242" t="b">
         <v>0</v>
@@ -10268,7 +10264,7 @@
         <v>-17.54306165994133</v>
       </c>
       <c r="J243" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K243" t="b">
         <v>0</v>
@@ -10308,7 +10304,7 @@
         <v>4.666919234985784</v>
       </c>
       <c r="J244" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K244" t="b">
         <v>0</v>
@@ -10348,7 +10344,7 @@
         <v>-13.11399128219771</v>
       </c>
       <c r="J245" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K245" t="b">
         <v>0</v>
@@ -10388,7 +10384,7 @@
         <v>-22.79465392201658</v>
       </c>
       <c r="J246" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K246" t="b">
         <v>0</v>
@@ -10428,7 +10424,7 @@
         <v>2525.507647713709</v>
       </c>
       <c r="J247" t="n">
-        <v>0.84</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="K247" t="b">
         <v>1</v>
@@ -10512,7 +10508,7 @@
         <v>-1.492962025010192</v>
       </c>
       <c r="J249" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K249" t="b">
         <v>0</v>
@@ -10552,7 +10548,7 @@
         <v>-16.69381951840755</v>
       </c>
       <c r="J250" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K250" t="b">
         <v>0</v>
@@ -10592,7 +10588,7 @@
         <v>-0.9817093419727571</v>
       </c>
       <c r="J251" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K251" t="b">
         <v>0</v>
@@ -10672,7 +10668,7 @@
         <v>-16.15281694130593</v>
       </c>
       <c r="J253" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.02</v>
       </c>
       <c r="K253" t="b">
         <v>0</v>
@@ -10712,7 +10708,7 @@
         <v>-8.028313723126248</v>
       </c>
       <c r="J254" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K254" t="b">
         <v>0</v>
@@ -10952,7 +10948,7 @@
         <v>0.0008543484464590001</v>
       </c>
       <c r="J260" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K260" t="b">
         <v>0</v>
@@ -10992,7 +10988,7 @@
         <v>-2.31383761637606</v>
       </c>
       <c r="J261" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K261" t="b">
         <v>0</v>
@@ -11032,7 +11028,7 @@
         <v>29.82231551932909</v>
       </c>
       <c r="J262" t="n">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="K262" t="b">
         <v>1</v>
@@ -11116,7 +11112,7 @@
         <v>-14.56847243700389</v>
       </c>
       <c r="J264" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K264" t="b">
         <v>0</v>
@@ -11156,7 +11152,7 @@
         <v>-19.0911853939931</v>
       </c>
       <c r="J265" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K265" t="b">
         <v>0</v>
@@ -11196,7 +11192,7 @@
         <v>-35.03024650942063</v>
       </c>
       <c r="J266" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K266" t="b">
         <v>0</v>
@@ -11236,7 +11232,7 @@
         <v>28.88513513513513</v>
       </c>
       <c r="J267" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.09333333333333334</v>
       </c>
       <c r="K267" t="b">
         <v>0</v>
@@ -11396,7 +11392,7 @@
         <v>18.71815613677644</v>
       </c>
       <c r="J271" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.02</v>
       </c>
       <c r="K271" t="b">
         <v>0</v>
@@ -11476,7 +11472,7 @@
         <v>-17.97829771807034</v>
       </c>
       <c r="J273" t="n">
-        <v>0.02</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K273" t="b">
         <v>0</v>
@@ -11596,7 +11592,7 @@
         <v>-0.8378535525696531</v>
       </c>
       <c r="J276" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K276" t="b">
         <v>0</v>
@@ -11836,7 +11832,7 @@
         <v>-9.748815501129522</v>
       </c>
       <c r="J282" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K282" t="b">
         <v>0</v>
@@ -11876,7 +11872,7 @@
         <v>-4.227749140768728</v>
       </c>
       <c r="J283" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="K283" t="b">
         <v>0</v>
@@ -12076,7 +12072,7 @@
         <v>5.559773032294486</v>
       </c>
       <c r="J288" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.08</v>
       </c>
       <c r="K288" t="b">
         <v>0</v>
@@ -12120,7 +12116,7 @@
         <v>-12.48789007620941</v>
       </c>
       <c r="J289" t="n">
-        <v>0.04</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K289" t="b">
         <v>0</v>
@@ -12160,7 +12156,7 @@
         <v>-1.129843369938731</v>
       </c>
       <c r="J290" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K290" t="b">
         <v>0</v>
@@ -12292,7 +12288,7 @@
         <v>-3.233286290414927</v>
       </c>
       <c r="J293" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K293" t="b">
         <v>0</v>
@@ -12412,7 +12408,7 @@
         <v>-0.756420963240059</v>
       </c>
       <c r="J296" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K296" t="b">
         <v>0</v>
@@ -12612,7 +12608,7 @@
         <v>-30.79976552723882</v>
       </c>
       <c r="J301" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K301" t="b">
         <v>0</v>
@@ -12652,14 +12648,14 @@
         <v>21.18961591278832</v>
       </c>
       <c r="J302" t="n">
-        <v>0.4</v>
+        <v>0.66</v>
       </c>
       <c r="K302" t="b">
         <v>1</v>
       </c>
       <c r="L302" t="inlineStr">
         <is>
-          <t>Recomendacion por analisis multivariable</t>
+          <t>Buena puntuacion en analisis multivariable</t>
         </is>
       </c>
     </row>
@@ -12696,7 +12692,7 @@
         <v>-8.65285976745222</v>
       </c>
       <c r="J303" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.02</v>
       </c>
       <c r="K303" t="b">
         <v>0</v>
@@ -12816,7 +12812,7 @@
         <v>-15.16888882484637</v>
       </c>
       <c r="J306" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K306" t="b">
         <v>0</v>
@@ -13056,7 +13052,7 @@
         <v>-9.269192371854864</v>
       </c>
       <c r="J312" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K312" t="b">
         <v>0</v>
@@ -13096,7 +13092,7 @@
         <v>57.46227086244219</v>
       </c>
       <c r="J313" t="n">
-        <v>0.8866666666666667</v>
+        <v>0.92</v>
       </c>
       <c r="K313" t="b">
         <v>1</v>
@@ -13140,7 +13136,7 @@
         <v>0.116753765151209</v>
       </c>
       <c r="J314" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K314" t="b">
         <v>0</v>
@@ -13220,7 +13216,7 @@
         <v>159.2683749555226</v>
       </c>
       <c r="J316" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="K316" t="b">
         <v>1</v>
@@ -13264,7 +13260,7 @@
         <v>-4.551014439902161</v>
       </c>
       <c r="J317" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K317" t="b">
         <v>0</v>
@@ -13304,7 +13300,7 @@
         <v>-10.65008778482681</v>
       </c>
       <c r="J318" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K318" t="b">
         <v>0</v>
@@ -13344,7 +13340,7 @@
         <v>-8.53412708937161</v>
       </c>
       <c r="J319" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K319" t="b">
         <v>0</v>
@@ -13384,7 +13380,7 @@
         <v>37.21380388528376</v>
       </c>
       <c r="J320" t="n">
-        <v>0.8266666666666667</v>
+        <v>0.8533333333333334</v>
       </c>
       <c r="K320" t="b">
         <v>1</v>
@@ -13508,7 +13504,7 @@
         <v>-2.709078235406632</v>
       </c>
       <c r="J323" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K323" t="b">
         <v>0</v>
@@ -13828,7 +13824,7 @@
         <v>-15.10919686112438</v>
       </c>
       <c r="J331" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K331" t="b">
         <v>0</v>
@@ -13868,7 +13864,7 @@
         <v>43.17450146034166</v>
       </c>
       <c r="J332" t="n">
-        <v>0.8466666666666667</v>
+        <v>0.8133333333333334</v>
       </c>
       <c r="K332" t="b">
         <v>1</v>
@@ -13912,7 +13908,7 @@
         <v>-13.62772268067522</v>
       </c>
       <c r="J333" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K333" t="b">
         <v>0</v>
@@ -13952,7 +13948,7 @@
         <v>-0.060574824621586</v>
       </c>
       <c r="J334" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K334" t="b">
         <v>0</v>
@@ -13992,14 +13988,14 @@
         <v>266.4637033990667</v>
       </c>
       <c r="J335" t="n">
-        <v>0.7866666666666666</v>
+        <v>0.96</v>
       </c>
       <c r="K335" t="b">
         <v>1</v>
       </c>
       <c r="L335" t="inlineStr">
         <is>
-          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%) | Buena puntuacion en analisis multivariable</t>
+          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
         </is>
       </c>
     </row>
@@ -14248,7 +14244,7 @@
         <v>-20.13485927990476</v>
       </c>
       <c r="J341" t="n">
-        <v>0</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="K341" t="b">
         <v>0</v>
@@ -14288,7 +14284,7 @@
         <v>-29.19520734166939</v>
       </c>
       <c r="J342" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K342" t="b">
         <v>0</v>
@@ -14528,14 +14524,14 @@
         <v>23.925163867219</v>
       </c>
       <c r="J348" t="n">
-        <v>0.88</v>
+        <v>0.4933333333333333</v>
       </c>
       <c r="K348" t="b">
         <v>1</v>
       </c>
       <c r="L348" t="inlineStr">
         <is>
-          <t>Tendencia semanal positiva | Alta confianza del modelo</t>
+          <t>Tendencia semanal positiva</t>
         </is>
       </c>
     </row>
@@ -14812,7 +14808,7 @@
         <v>0.358636478921627</v>
       </c>
       <c r="J355" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K355" t="b">
         <v>0</v>
@@ -15052,7 +15048,7 @@
         <v>19.85002231336454</v>
       </c>
       <c r="J361" t="n">
-        <v>0.2</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K361" t="b">
         <v>0</v>
@@ -15212,16 +15208,12 @@
         <v>19.18852432655161</v>
       </c>
       <c r="J365" t="n">
-        <v>0.6266666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K365" t="b">
-        <v>1</v>
-      </c>
-      <c r="L365" t="inlineStr">
-        <is>
-          <t>Buena puntuacion en analisis multivariable</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -15296,14 +15288,14 @@
         <v>13701.95877798988</v>
       </c>
       <c r="J367" t="n">
-        <v>0.7866666666666666</v>
+        <v>0.54</v>
       </c>
       <c r="K367" t="b">
         <v>1</v>
       </c>
       <c r="L367" t="inlineStr">
         <is>
-          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%) | Buena puntuacion en analisis multivariable</t>
+          <t>Explosion mensual (+100%) | Fuerte tendencia semanal (+10%)</t>
         </is>
       </c>
     </row>
@@ -15380,7 +15372,7 @@
         <v>-21.77795502089348</v>
       </c>
       <c r="J369" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K369" t="b">
         <v>0</v>
@@ -15500,7 +15492,7 @@
         <v>-13.95299240008044</v>
       </c>
       <c r="J372" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K372" t="b">
         <v>0</v>
@@ -15540,7 +15532,7 @@
         <v>80.44094641780181</v>
       </c>
       <c r="J373" t="n">
-        <v>0.16</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="K373" t="b">
         <v>0</v>
@@ -15620,7 +15612,7 @@
         <v>-26.89075749106678</v>
       </c>
       <c r="J375" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K375" t="b">
         <v>0</v>
@@ -15740,7 +15732,7 @@
         <v>-18.19267425855399</v>
       </c>
       <c r="J378" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.04</v>
       </c>
       <c r="K378" t="b">
         <v>0</v>
@@ -15780,7 +15772,7 @@
         <v>34.3077215472813</v>
       </c>
       <c r="J379" t="n">
-        <v>0.06</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="K379" t="b">
         <v>0</v>
@@ -15980,7 +15972,7 @@
         <v>-14.82530951891758</v>
       </c>
       <c r="J384" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K384" t="b">
         <v>0</v>
@@ -16068,7 +16060,7 @@
         <v>-3.403403677417287</v>
       </c>
       <c r="J386" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K386" t="b">
         <v>0</v>
@@ -16112,7 +16104,7 @@
         <v>-19.27255073417001</v>
       </c>
       <c r="J387" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K387" t="b">
         <v>0</v>
@@ -16232,7 +16224,7 @@
         <v>10.10831411126945</v>
       </c>
       <c r="J390" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K390" t="b">
         <v>0</v>
@@ -16352,7 +16344,7 @@
         <v>-42.57130740671312</v>
       </c>
       <c r="J393" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K393" t="b">
         <v>0</v>
@@ -16392,7 +16384,7 @@
         <v>10.76738933375865</v>
       </c>
       <c r="J394" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="K394" t="b">
         <v>0</v>
@@ -16472,7 +16464,7 @@
         <v>-13.43698847755994</v>
       </c>
       <c r="J396" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K396" t="b">
         <v>0</v>
@@ -16552,7 +16544,7 @@
         <v>-16.25296316576334</v>
       </c>
       <c r="J398" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K398" t="b">
         <v>0</v>
@@ -16792,7 +16784,7 @@
         <v>57.09169107227211</v>
       </c>
       <c r="J404" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.1266666666666667</v>
       </c>
       <c r="K404" t="b">
         <v>0</v>
@@ -16832,7 +16824,7 @@
         <v>7.287386578484954</v>
       </c>
       <c r="J405" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="K405" t="b">
         <v>0</v>
@@ -16952,7 +16944,7 @@
         <v>18.6816527210375</v>
       </c>
       <c r="J408" t="n">
-        <v>0.02666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K408" t="b">
         <v>0</v>
@@ -17112,7 +17104,7 @@
         <v>-11.85134331021512</v>
       </c>
       <c r="J412" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K412" t="b">
         <v>0</v>
@@ -17312,7 +17304,7 @@
         <v>-13.76071106211771</v>
       </c>
       <c r="J417" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K417" t="b">
         <v>0</v>
@@ -17352,7 +17344,7 @@
         <v>-13.12547116681166</v>
       </c>
       <c r="J418" t="n">
-        <v>0</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K418" t="b">
         <v>0</v>
@@ -17392,7 +17384,7 @@
         <v>64.51589806840326</v>
       </c>
       <c r="J419" t="n">
-        <v>0.86</v>
+        <v>0.8733333333333333</v>
       </c>
       <c r="K419" t="b">
         <v>1</v>
@@ -17436,7 +17428,7 @@
         <v>-11.44588027320056</v>
       </c>
       <c r="J420" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="K420" t="b">
         <v>0</v>
@@ -17476,7 +17468,7 @@
         <v>2.418870753659049</v>
       </c>
       <c r="J421" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K421" t="b">
         <v>0</v>
@@ -17516,7 +17508,7 @@
         <v>-0.036690557960992</v>
       </c>
       <c r="J422" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K422" t="b">
         <v>0</v>
@@ -17556,7 +17548,7 @@
         <v>278.4348970892472</v>
       </c>
       <c r="J423" t="n">
-        <v>0.88</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="K423" t="b">
         <v>1</v>
@@ -17600,7 +17592,7 @@
         <v>-14.31999929500089</v>
       </c>
       <c r="J424" t="n">
-        <v>0.06</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="K424" t="b">
         <v>0</v>
@@ -17680,7 +17672,7 @@
         <v>-1.91357632706648</v>
       </c>
       <c r="J426" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K426" t="b">
         <v>0</v>
@@ -17720,7 +17712,7 @@
         <v>-9.695491705106143</v>
       </c>
       <c r="J427" t="n">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K427" t="b">
         <v>0</v>
@@ -17760,7 +17752,7 @@
         <v>-3.864510659080766</v>
       </c>
       <c r="J428" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K428" t="b">
         <v>0</v>
@@ -17800,7 +17792,7 @@
         <v>-16.22192345188167</v>
       </c>
       <c r="J429" t="n">
-        <v>0.02666666666666667</v>
+        <v>0</v>
       </c>
       <c r="K429" t="b">
         <v>0</v>
@@ -17840,12 +17832,1876 @@
         <v>2.136232220300422</v>
       </c>
       <c r="J430" t="n">
+        <v>0</v>
+      </c>
+      <c r="K430" t="b">
+        <v>0</v>
+      </c>
+      <c r="L430" t="inlineStr"/>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>VVS Finance</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>vvs</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/20210/large/8glAYOTM_400x400.jpg?1696519620</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>/charts/vvs_chart.png</t>
+        </is>
+      </c>
+      <c r="E431" t="n">
+        <v>104726514</v>
+      </c>
+      <c r="F431" t="n">
+        <v>2.16e-06</v>
+      </c>
+      <c r="G431" t="n">
+        <v>15.71013677066031</v>
+      </c>
+      <c r="H431" t="n">
+        <v>15.92464040111533</v>
+      </c>
+      <c r="I431" t="n">
+        <v>-7.710040462111606</v>
+      </c>
+      <c r="J431" t="n">
         <v>0.03333333333333333</v>
       </c>
-      <c r="K430" t="b">
-        <v>0</v>
-      </c>
-      <c r="L430" t="inlineStr"/>
+      <c r="K431" t="b">
+        <v>0</v>
+      </c>
+      <c r="L431" t="inlineStr"/>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>SKALE</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>skl</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/13245/large/SKALE_token_300x300.png?1696513021</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>/charts/skl_chart.png</t>
+        </is>
+      </c>
+      <c r="E432" t="n">
+        <v>97284695</v>
+      </c>
+      <c r="F432" t="n">
+        <v>0.016831</v>
+      </c>
+      <c r="G432" t="n">
+        <v>1.218214575693852</v>
+      </c>
+      <c r="H432" t="n">
+        <v>-5.62630428628989</v>
+      </c>
+      <c r="I432" t="n">
+        <v>-20.29432201389429</v>
+      </c>
+      <c r="J432" t="n">
+        <v>0</v>
+      </c>
+      <c r="K432" t="b">
+        <v>0</v>
+      </c>
+      <c r="L432" t="inlineStr"/>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>Rei</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>rei</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52005/large/TIAutjcd_400x400.jpg?1741519600</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>/charts/rei_chart.png</t>
+        </is>
+      </c>
+      <c r="E433" t="n">
+        <v>97110697</v>
+      </c>
+      <c r="F433" t="n">
+        <v>0.09744499999999999</v>
+      </c>
+      <c r="G433" t="n">
+        <v>5.559234516424017</v>
+      </c>
+      <c r="H433" t="n">
+        <v>-10.21169720582954</v>
+      </c>
+      <c r="I433" t="n">
+        <v>63.59658648207511</v>
+      </c>
+      <c r="J433" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="K433" t="b">
+        <v>0</v>
+      </c>
+      <c r="L433" t="inlineStr"/>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>Big Time</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>bigtime</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/32251/large/-6136155493475923781_121.jpg?1696998691</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr"/>
+      <c r="E434" t="n">
+        <v>96411044</v>
+      </c>
+      <c r="F434" t="n">
+        <v>0.050496</v>
+      </c>
+      <c r="G434" t="n">
+        <v>-0.511143533376993</v>
+      </c>
+      <c r="H434" t="n">
+        <v>1.095167171848813</v>
+      </c>
+      <c r="I434" t="n">
+        <v>-14.79188557967054</v>
+      </c>
+      <c r="J434" t="n">
+        <v>0</v>
+      </c>
+      <c r="K434" t="b">
+        <v>0</v>
+      </c>
+      <c r="L434" t="inlineStr"/>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>Lift Dollar</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>usdl</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/38484/large/USDL-Token-200px.png?1725022887</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr"/>
+      <c r="E435" t="n">
+        <v>96093061</v>
+      </c>
+      <c r="F435" t="n">
+        <v>0.999651</v>
+      </c>
+      <c r="G435" t="n">
+        <v>-0.009519300912774</v>
+      </c>
+      <c r="H435" t="n">
+        <v>-0.026889401082196</v>
+      </c>
+      <c r="I435" t="n">
+        <v>0.006067910883572</v>
+      </c>
+      <c r="J435" t="n">
+        <v>0</v>
+      </c>
+      <c r="K435" t="b">
+        <v>0</v>
+      </c>
+      <c r="L435" t="inlineStr"/>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>Velo</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>velo</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12538/large/Logo_200x_200.png?1696512350</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr"/>
+      <c r="E436" t="n">
+        <v>96054907</v>
+      </c>
+      <c r="F436" t="n">
+        <v>0.01299363</v>
+      </c>
+      <c r="G436" t="n">
+        <v>0.365105966415385</v>
+      </c>
+      <c r="H436" t="n">
+        <v>-3.553714302544732</v>
+      </c>
+      <c r="I436" t="n">
+        <v>-0.9026938254210071</v>
+      </c>
+      <c r="J436" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K436" t="b">
+        <v>0</v>
+      </c>
+      <c r="L436" t="inlineStr"/>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>Goatseus Maximus</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>goat</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/50717/large/GOAT_LOGO_NEW.jpg?1731292759</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr"/>
+      <c r="E437" t="n">
+        <v>95952973</v>
+      </c>
+      <c r="F437" t="n">
+        <v>0.095786</v>
+      </c>
+      <c r="G437" t="n">
+        <v>-1.1253484940813</v>
+      </c>
+      <c r="H437" t="n">
+        <v>1.38845040174543</v>
+      </c>
+      <c r="I437" t="n">
+        <v>-19.88658602769759</v>
+      </c>
+      <c r="J437" t="n">
+        <v>0</v>
+      </c>
+      <c r="K437" t="b">
+        <v>0</v>
+      </c>
+      <c r="L437" t="inlineStr"/>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>Lagrange</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>la</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/55550/large/Lagrange-logo-png-gradient.png?1746637731</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr"/>
+      <c r="E438" t="n">
+        <v>95579734</v>
+      </c>
+      <c r="F438" t="n">
+        <v>0.495018</v>
+      </c>
+      <c r="G438" t="n">
+        <v>-0.7724502824613571</v>
+      </c>
+      <c r="H438" t="n">
+        <v>1.22248025392056</v>
+      </c>
+      <c r="I438" t="n">
+        <v>-51.78758782685565</v>
+      </c>
+      <c r="J438" t="n">
+        <v>0</v>
+      </c>
+      <c r="K438" t="b">
+        <v>0</v>
+      </c>
+      <c r="L438" t="inlineStr"/>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>L2 Standard Bridged frxUSD</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>frxusd</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54455/large/frxusd.png?1739790094</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr"/>
+      <c r="E439" t="n">
+        <v>94773919</v>
+      </c>
+      <c r="F439" t="n">
+        <v>0.9994600000000001</v>
+      </c>
+      <c r="G439" t="n">
+        <v>-0.033023531506404</v>
+      </c>
+      <c r="H439" t="n">
+        <v>0.1314494644545</v>
+      </c>
+      <c r="I439" t="n">
+        <v>-0.00019788232466</v>
+      </c>
+      <c r="J439" t="n">
+        <v>0</v>
+      </c>
+      <c r="K439" t="b">
+        <v>0</v>
+      </c>
+      <c r="L439" t="inlineStr"/>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>Constellation</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>dag</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/4645/large/Constellation_Network_Logo.png?1696505213</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr"/>
+      <c r="E440" t="n">
+        <v>93579209</v>
+      </c>
+      <c r="F440" t="n">
+        <v>0.03269595</v>
+      </c>
+      <c r="G440" t="n">
+        <v>-3.445812084849323</v>
+      </c>
+      <c r="H440" t="n">
+        <v>0.513108983059511</v>
+      </c>
+      <c r="I440" t="n">
+        <v>-17.48960164045483</v>
+      </c>
+      <c r="J440" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K440" t="b">
+        <v>0</v>
+      </c>
+      <c r="L440" t="inlineStr"/>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>Restaked Swell ETH</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>rsweth</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/34489/large/rswETH_Icon.png?1706865484</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr"/>
+      <c r="E441" t="n">
+        <v>93526337</v>
+      </c>
+      <c r="F441" t="n">
+        <v>2676.54</v>
+      </c>
+      <c r="G441" t="n">
+        <v>6.48304338422064</v>
+      </c>
+      <c r="H441" t="n">
+        <v>6.167008509575308</v>
+      </c>
+      <c r="I441" t="n">
+        <v>2.18579098287398</v>
+      </c>
+      <c r="J441" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="K441" t="b">
+        <v>0</v>
+      </c>
+      <c r="L441" t="inlineStr"/>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>UMA</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>uma</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/10951/large/UMA.png?1696510900</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr"/>
+      <c r="E442" t="n">
+        <v>93436458</v>
+      </c>
+      <c r="F442" t="n">
+        <v>1.059</v>
+      </c>
+      <c r="G442" t="n">
+        <v>-0.8525044830326031</v>
+      </c>
+      <c r="H442" t="n">
+        <v>-1.047255499236967</v>
+      </c>
+      <c r="I442" t="n">
+        <v>-19.83805462391854</v>
+      </c>
+      <c r="J442" t="n">
+        <v>0</v>
+      </c>
+      <c r="K442" t="b">
+        <v>0</v>
+      </c>
+      <c r="L442" t="inlineStr"/>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>NKYC Token</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>nkyc</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/30337/large/NKYC-Logo.png?1696529238</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr"/>
+      <c r="E443" t="n">
+        <v>93382818</v>
+      </c>
+      <c r="F443" t="n">
+        <v>23.36</v>
+      </c>
+      <c r="G443" t="n">
+        <v>0.114620730442197</v>
+      </c>
+      <c r="H443" t="n">
+        <v>0.198781266721632</v>
+      </c>
+      <c r="I443" t="n">
+        <v>-4.076415313471843</v>
+      </c>
+      <c r="J443" t="n">
+        <v>0</v>
+      </c>
+      <c r="K443" t="b">
+        <v>0</v>
+      </c>
+      <c r="L443" t="inlineStr"/>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>Metis</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>metis</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/15595/large/Metis_Black_Bg.png?1702968192</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr"/>
+      <c r="E444" t="n">
+        <v>92933669</v>
+      </c>
+      <c r="F444" t="n">
+        <v>14.43</v>
+      </c>
+      <c r="G444" t="n">
+        <v>-1.718460952630052</v>
+      </c>
+      <c r="H444" t="n">
+        <v>-10.18706544722492</v>
+      </c>
+      <c r="I444" t="n">
+        <v>-17.3343158669264</v>
+      </c>
+      <c r="J444" t="n">
+        <v>0</v>
+      </c>
+      <c r="K444" t="b">
+        <v>0</v>
+      </c>
+      <c r="L444" t="inlineStr"/>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>Elixir Staked deUSD</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>sdeusd</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52847/large/Staked_deUSD_%28sdeUSD%29_Logo.png?1734473339</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr"/>
+      <c r="E445" t="n">
+        <v>92813129</v>
+      </c>
+      <c r="F445" t="n">
+        <v>1.048</v>
+      </c>
+      <c r="G445" t="n">
+        <v>-0.035029871053175</v>
+      </c>
+      <c r="H445" t="n">
+        <v>0.183452523960722</v>
+      </c>
+      <c r="I445" t="n">
+        <v>0.453088902899591</v>
+      </c>
+      <c r="J445" t="n">
+        <v>0</v>
+      </c>
+      <c r="K445" t="b">
+        <v>0</v>
+      </c>
+      <c r="L445" t="inlineStr"/>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>Rollbit Coin</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>rlb</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/24552/large/unziL6wO_400x400.jpg?1696523729</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr"/>
+      <c r="E446" t="n">
+        <v>92664857</v>
+      </c>
+      <c r="F446" t="n">
+        <v>0.04556248</v>
+      </c>
+      <c r="G446" t="n">
+        <v>2.249119373532227</v>
+      </c>
+      <c r="H446" t="n">
+        <v>10.15099293963239</v>
+      </c>
+      <c r="I446" t="n">
+        <v>-24.94822582653359</v>
+      </c>
+      <c r="J446" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K446" t="b">
+        <v>0</v>
+      </c>
+      <c r="L446" t="inlineStr"/>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>Alchemy Pay</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>ach</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/12390/large/ACH_%281%29.png?1696512213</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr"/>
+      <c r="E447" t="n">
+        <v>91957285</v>
+      </c>
+      <c r="F447" t="n">
+        <v>0.01857476</v>
+      </c>
+      <c r="G447" t="n">
+        <v>-1.662780706649764</v>
+      </c>
+      <c r="H447" t="n">
+        <v>5.238823876703431</v>
+      </c>
+      <c r="I447" t="n">
+        <v>-10.94845642184715</v>
+      </c>
+      <c r="J447" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K447" t="b">
+        <v>0</v>
+      </c>
+      <c r="L447" t="inlineStr"/>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>DOLA</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>dola</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/14287/large/dola.png?1696513984</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr"/>
+      <c r="E448" t="n">
+        <v>91568566</v>
+      </c>
+      <c r="F448" t="n">
+        <v>0.997895</v>
+      </c>
+      <c r="G448" t="n">
+        <v>-0.023541738343394</v>
+      </c>
+      <c r="H448" t="n">
+        <v>-0.07679508855515201</v>
+      </c>
+      <c r="I448" t="n">
+        <v>-0.192151812436207</v>
+      </c>
+      <c r="J448" t="n">
+        <v>0</v>
+      </c>
+      <c r="K448" t="b">
+        <v>0</v>
+      </c>
+      <c r="L448" t="inlineStr"/>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>SpaceN</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>sn</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/27576/large/sn.png?1696526609</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr"/>
+      <c r="E449" t="n">
+        <v>91139920</v>
+      </c>
+      <c r="F449" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="G449" t="n">
+        <v>-12.23532727174345</v>
+      </c>
+      <c r="H449" t="n">
+        <v>43.39737942661318</v>
+      </c>
+      <c r="I449" t="n">
+        <v>79.28397871028986</v>
+      </c>
+      <c r="J449" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="K449" t="b">
+        <v>1</v>
+      </c>
+      <c r="L449" t="inlineStr">
+        <is>
+          <t>Crecimiento mensual sobresaliente (+60%) | Fuerte tendencia semanal (+10%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>ALEO</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>aleo</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/27916/large/secondary-icon-dark.png?1726770428</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr"/>
+      <c r="E450" t="n">
+        <v>90972833</v>
+      </c>
+      <c r="F450" t="n">
+        <v>0.211915</v>
+      </c>
+      <c r="G450" t="n">
+        <v>-4.086750398420591</v>
+      </c>
+      <c r="H450" t="n">
+        <v>6.837915061083058</v>
+      </c>
+      <c r="I450" t="n">
+        <v>17.41933801250743</v>
+      </c>
+      <c r="J450" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="K450" t="b">
+        <v>0</v>
+      </c>
+      <c r="L450" t="inlineStr"/>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>Verasity</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>vra</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/14025/large/logo_%281%29.png?1716968890</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr"/>
+      <c r="E451" t="n">
+        <v>90531211</v>
+      </c>
+      <c r="F451" t="n">
+        <v>0.00109679</v>
+      </c>
+      <c r="G451" t="n">
+        <v>0.384412884796638</v>
+      </c>
+      <c r="H451" t="n">
+        <v>4.392960640363028</v>
+      </c>
+      <c r="I451" t="n">
+        <v>-23.38632888983545</v>
+      </c>
+      <c r="J451" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K451" t="b">
+        <v>0</v>
+      </c>
+      <c r="L451" t="inlineStr"/>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>Metaplex</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>mplx</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/27344/large/mplx.png?1696526391</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr"/>
+      <c r="E452" t="n">
+        <v>90388773</v>
+      </c>
+      <c r="F452" t="n">
+        <v>0.108948</v>
+      </c>
+      <c r="G452" t="n">
+        <v>5.965229349120954</v>
+      </c>
+      <c r="H452" t="n">
+        <v>-5.568983632697615</v>
+      </c>
+      <c r="I452" t="n">
+        <v>-21.82906714324731</v>
+      </c>
+      <c r="J452" t="n">
+        <v>0</v>
+      </c>
+      <c r="K452" t="b">
+        <v>0</v>
+      </c>
+      <c r="L452" t="inlineStr"/>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>Blast</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>blast</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/35494/large/Blast.jpg?1719385662</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr"/>
+      <c r="E453" t="n">
+        <v>90229467</v>
+      </c>
+      <c r="F453" t="n">
+        <v>0.00217735</v>
+      </c>
+      <c r="G453" t="n">
+        <v>-8.594689580904953</v>
+      </c>
+      <c r="H453" t="n">
+        <v>9.72085737532397</v>
+      </c>
+      <c r="I453" t="n">
+        <v>-19.2047916008658</v>
+      </c>
+      <c r="J453" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K453" t="b">
+        <v>0</v>
+      </c>
+      <c r="L453" t="inlineStr"/>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>Diverge Loop</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>dlc</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/27323/large/dlr.png?1745232682</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr"/>
+      <c r="E454" t="n">
+        <v>90195661</v>
+      </c>
+      <c r="F454" t="n">
+        <v>0.101343</v>
+      </c>
+      <c r="G454" t="n">
+        <v>4.49280980036916</v>
+      </c>
+      <c r="H454" t="n">
+        <v>2.608596728681044</v>
+      </c>
+      <c r="I454" t="n">
+        <v>-46.47636596911948</v>
+      </c>
+      <c r="J454" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K454" t="b">
+        <v>0</v>
+      </c>
+      <c r="L454" t="inlineStr"/>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>ConstitutionDAO</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>people</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/20612/large/GN_UVm3d_400x400.jpg?1696520017</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr"/>
+      <c r="E455" t="n">
+        <v>89646210</v>
+      </c>
+      <c r="F455" t="n">
+        <v>0.01768698</v>
+      </c>
+      <c r="G455" t="n">
+        <v>-0.7431193890874971</v>
+      </c>
+      <c r="H455" t="n">
+        <v>1.328730397474849</v>
+      </c>
+      <c r="I455" t="n">
+        <v>-13.37942730749878</v>
+      </c>
+      <c r="J455" t="n">
+        <v>0</v>
+      </c>
+      <c r="K455" t="b">
+        <v>0</v>
+      </c>
+      <c r="L455" t="inlineStr"/>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>Clearpool</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>cpool</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/19252/large/photo_2022-08-31_12.45.02.jpeg?1696518697</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr"/>
+      <c r="E456" t="n">
+        <v>89563924</v>
+      </c>
+      <c r="F456" t="n">
+        <v>0.114122</v>
+      </c>
+      <c r="G456" t="n">
+        <v>-1.048443180410713</v>
+      </c>
+      <c r="H456" t="n">
+        <v>3.064198988609981</v>
+      </c>
+      <c r="I456" t="n">
+        <v>-8.375316027420304</v>
+      </c>
+      <c r="J456" t="n">
+        <v>0</v>
+      </c>
+      <c r="K456" t="b">
+        <v>0</v>
+      </c>
+      <c r="L456" t="inlineStr"/>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>Stratis</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>strax</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/531/large/stratis.png?1696501751</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr"/>
+      <c r="E457" t="n">
+        <v>89278460</v>
+      </c>
+      <c r="F457" t="n">
+        <v>0.04492797</v>
+      </c>
+      <c r="G457" t="n">
+        <v>-2.156326476205286</v>
+      </c>
+      <c r="H457" t="n">
+        <v>4.471167307331012</v>
+      </c>
+      <c r="I457" t="n">
+        <v>-0.15753400748836</v>
+      </c>
+      <c r="J457" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K457" t="b">
+        <v>0</v>
+      </c>
+      <c r="L457" t="inlineStr"/>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>BugsCoin</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>bgsc</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/52619/large/bnUmy-NT_400x400.png?1733784337</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr"/>
+      <c r="E458" t="n">
+        <v>89059906</v>
+      </c>
+      <c r="F458" t="n">
+        <v>0.0075739</v>
+      </c>
+      <c r="G458" t="n">
+        <v>-5.338676839717611</v>
+      </c>
+      <c r="H458" t="n">
+        <v>1.994136990124923</v>
+      </c>
+      <c r="I458" t="n">
+        <v>-6.317808607769174</v>
+      </c>
+      <c r="J458" t="n">
+        <v>0</v>
+      </c>
+      <c r="K458" t="b">
+        <v>0</v>
+      </c>
+      <c r="L458" t="inlineStr"/>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>IOST</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>iost</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/2523/large/IOST.png?1696503337</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr"/>
+      <c r="E459" t="n">
+        <v>88977696</v>
+      </c>
+      <c r="F459" t="n">
+        <v>0.00332462</v>
+      </c>
+      <c r="G459" t="n">
+        <v>0.7601197514151751</v>
+      </c>
+      <c r="H459" t="n">
+        <v>4.944622005451823</v>
+      </c>
+      <c r="I459" t="n">
+        <v>-14.80656210994365</v>
+      </c>
+      <c r="J459" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K459" t="b">
+        <v>0</v>
+      </c>
+      <c r="L459" t="inlineStr"/>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>Loopring</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>lrc</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/913/large/LRC.png?1696502034</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr"/>
+      <c r="E460" t="n">
+        <v>88929281</v>
+      </c>
+      <c r="F460" t="n">
+        <v>0.071353</v>
+      </c>
+      <c r="G460" t="n">
+        <v>-0.8839073635598701</v>
+      </c>
+      <c r="H460" t="n">
+        <v>-0.9640710690552601</v>
+      </c>
+      <c r="I460" t="n">
+        <v>-14.42585290207963</v>
+      </c>
+      <c r="J460" t="n">
+        <v>0</v>
+      </c>
+      <c r="K460" t="b">
+        <v>0</v>
+      </c>
+      <c r="L460" t="inlineStr"/>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>Band Protocol</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>band</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/9545/large/Band_token_blue_violet_token.png?1696509627</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr"/>
+      <c r="E461" t="n">
+        <v>88841746</v>
+      </c>
+      <c r="F461" t="n">
+        <v>0.568685</v>
+      </c>
+      <c r="G461" t="n">
+        <v>-0.502702291207846</v>
+      </c>
+      <c r="H461" t="n">
+        <v>4.58618000820494</v>
+      </c>
+      <c r="I461" t="n">
+        <v>-13.60934492963547</v>
+      </c>
+      <c r="J461" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="K461" t="b">
+        <v>0</v>
+      </c>
+      <c r="L461" t="inlineStr"/>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>HashKey Platform Token</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>hsk</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/29779/large/HSKlogo.jpg?1719445510</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr"/>
+      <c r="E462" t="n">
+        <v>88824901</v>
+      </c>
+      <c r="F462" t="n">
+        <v>0.670424</v>
+      </c>
+      <c r="G462" t="n">
+        <v>13.73511725373279</v>
+      </c>
+      <c r="H462" t="n">
+        <v>4.523522753306781</v>
+      </c>
+      <c r="I462" t="n">
+        <v>127.58243329045</v>
+      </c>
+      <c r="J462" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K462" t="b">
+        <v>1</v>
+      </c>
+      <c r="L462" t="inlineStr">
+        <is>
+          <t>Explosion mensual (+100%) | Buena puntuacion en analisis multivariable</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>NexusMind</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>nmd</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/35449/large/nmd-cg.jpg?1708664539</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr"/>
+      <c r="E463" t="n">
+        <v>88801648</v>
+      </c>
+      <c r="F463" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="G463" t="n">
+        <v>-0.09160846633159601</v>
+      </c>
+      <c r="H463" t="n">
+        <v>2.24263398161103</v>
+      </c>
+      <c r="I463" t="n">
+        <v>2.301196467225316</v>
+      </c>
+      <c r="J463" t="n">
+        <v>0</v>
+      </c>
+      <c r="K463" t="b">
+        <v>0</v>
+      </c>
+      <c r="L463" t="inlineStr"/>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>Coreum</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>coreum</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/24169/large/Coreum-Icon_%282%29.png?1738317497</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr"/>
+      <c r="E464" t="n">
+        <v>88691653</v>
+      </c>
+      <c r="F464" t="n">
+        <v>0.136514</v>
+      </c>
+      <c r="G464" t="n">
+        <v>6.242480690638005</v>
+      </c>
+      <c r="H464" t="n">
+        <v>13.35238326099936</v>
+      </c>
+      <c r="I464" t="n">
+        <v>4.819340752807322</v>
+      </c>
+      <c r="J464" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K464" t="b">
+        <v>0</v>
+      </c>
+      <c r="L464" t="inlineStr"/>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>Metal Blockchain</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>metal</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/27222/large/MB-Logo.png?1710514210</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr"/>
+      <c r="E465" t="n">
+        <v>88028637</v>
+      </c>
+      <c r="F465" t="n">
+        <v>0.173408</v>
+      </c>
+      <c r="G465" t="n">
+        <v>5.382591059636176</v>
+      </c>
+      <c r="H465" t="n">
+        <v>48.70987765015511</v>
+      </c>
+      <c r="I465" t="n">
+        <v>66.08180518192947</v>
+      </c>
+      <c r="J465" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="K465" t="b">
+        <v>1</v>
+      </c>
+      <c r="L465" t="inlineStr">
+        <is>
+          <t>Crecimiento mensual sobresaliente (+60%) | Fuerte tendencia semanal (+10%) | Alta confianza del modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>Bio Protocol</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>bio</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/53022/large/bio.jpg?1735011002</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr"/>
+      <c r="E466" t="n">
+        <v>87710941</v>
+      </c>
+      <c r="F466" t="n">
+        <v>0.04838689</v>
+      </c>
+      <c r="G466" t="n">
+        <v>-5.280276824096681</v>
+      </c>
+      <c r="H466" t="n">
+        <v>-5.089772200962483</v>
+      </c>
+      <c r="I466" t="n">
+        <v>-20.00107364864943</v>
+      </c>
+      <c r="J466" t="n">
+        <v>0</v>
+      </c>
+      <c r="K466" t="b">
+        <v>0</v>
+      </c>
+      <c r="L466" t="inlineStr"/>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>Animecoin</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>anime</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/53575/large/anime.jpg?1736748703</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr"/>
+      <c r="E467" t="n">
+        <v>87671117</v>
+      </c>
+      <c r="F467" t="n">
+        <v>0.01582205</v>
+      </c>
+      <c r="G467" t="n">
+        <v>-2.795023102020059</v>
+      </c>
+      <c r="H467" t="n">
+        <v>-4.898460058093431</v>
+      </c>
+      <c r="I467" t="n">
+        <v>-52.34039745009329</v>
+      </c>
+      <c r="J467" t="n">
+        <v>0</v>
+      </c>
+      <c r="K467" t="b">
+        <v>0</v>
+      </c>
+      <c r="L467" t="inlineStr"/>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>0x0.ai: AI Smart Contract</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>0x0</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/28880/large/0x0.png?1696527857</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr"/>
+      <c r="E468" t="n">
+        <v>87325069</v>
+      </c>
+      <c r="F468" t="n">
+        <v>0.09760199999999999</v>
+      </c>
+      <c r="G468" t="n">
+        <v>7.961228026740043</v>
+      </c>
+      <c r="H468" t="n">
+        <v>-3.832941298226657</v>
+      </c>
+      <c r="I468" t="n">
+        <v>17.60690974388485</v>
+      </c>
+      <c r="J468" t="n">
+        <v>0.04666666666666667</v>
+      </c>
+      <c r="K468" t="b">
+        <v>0</v>
+      </c>
+      <c r="L468" t="inlineStr"/>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>Biconomy</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>bico</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/21061/large/biconomy_logo.jpg?1696520444</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr"/>
+      <c r="E469" t="n">
+        <v>87031779</v>
+      </c>
+      <c r="F469" t="n">
+        <v>0.09024299999999999</v>
+      </c>
+      <c r="G469" t="n">
+        <v>-0.781582461749148</v>
+      </c>
+      <c r="H469" t="n">
+        <v>1.813077316119085</v>
+      </c>
+      <c r="I469" t="n">
+        <v>-9.752686317925798</v>
+      </c>
+      <c r="J469" t="n">
+        <v>0</v>
+      </c>
+      <c r="K469" t="b">
+        <v>0</v>
+      </c>
+      <c r="L469" t="inlineStr"/>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>XPR Network</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>xpr</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/10941/large/XPR.jpg?1696510891</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr"/>
+      <c r="E470" t="n">
+        <v>86758288</v>
+      </c>
+      <c r="F470" t="n">
+        <v>0.00312878</v>
+      </c>
+      <c r="G470" t="n">
+        <v>0.6879480535111161</v>
+      </c>
+      <c r="H470" t="n">
+        <v>6.770393076703206</v>
+      </c>
+      <c r="I470" t="n">
+        <v>-9.230004296791302</v>
+      </c>
+      <c r="J470" t="n">
+        <v>0</v>
+      </c>
+      <c r="K470" t="b">
+        <v>0</v>
+      </c>
+      <c r="L470" t="inlineStr"/>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>Orbs</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>orbs</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/4630/large/Orbs.jpg?1696505200</t>
+        </is>
+      </c>
+      <c r="D471" t="inlineStr"/>
+      <c r="E471" t="n">
+        <v>86745277</v>
+      </c>
+      <c r="F471" t="n">
+        <v>0.01852155</v>
+      </c>
+      <c r="G471" t="n">
+        <v>0.049808910335726</v>
+      </c>
+      <c r="H471" t="n">
+        <v>0.570536028131248</v>
+      </c>
+      <c r="I471" t="n">
+        <v>-3.846978598686662</v>
+      </c>
+      <c r="J471" t="n">
+        <v>0</v>
+      </c>
+      <c r="K471" t="b">
+        <v>0</v>
+      </c>
+      <c r="L471" t="inlineStr"/>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>Delysium</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>agi</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/29299/large/AGI_logo_200.png?1696528251</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr"/>
+      <c r="E472" t="n">
+        <v>86441529</v>
+      </c>
+      <c r="F472" t="n">
+        <v>0.04828397</v>
+      </c>
+      <c r="G472" t="n">
+        <v>-2.015170029820241</v>
+      </c>
+      <c r="H472" t="n">
+        <v>12.58234173892475</v>
+      </c>
+      <c r="I472" t="n">
+        <v>-12.50420591176875</v>
+      </c>
+      <c r="J472" t="n">
+        <v>0</v>
+      </c>
+      <c r="K472" t="b">
+        <v>0</v>
+      </c>
+      <c r="L472" t="inlineStr"/>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>PAAL AI</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>paal</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/30815/large/Paal_New_Logo_%281%29.png?1718160584</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr"/>
+      <c r="E473" t="n">
+        <v>86256895</v>
+      </c>
+      <c r="F473" t="n">
+        <v>0.09591899999999999</v>
+      </c>
+      <c r="G473" t="n">
+        <v>-3.434013184779078</v>
+      </c>
+      <c r="H473" t="n">
+        <v>2.976242830499873</v>
+      </c>
+      <c r="I473" t="n">
+        <v>-17.79534976415649</v>
+      </c>
+      <c r="J473" t="n">
+        <v>0</v>
+      </c>
+      <c r="K473" t="b">
+        <v>0</v>
+      </c>
+      <c r="L473" t="inlineStr"/>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>SingularityNET</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>agix</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/2138/large/singularitynet.png?1696503103</t>
+        </is>
+      </c>
+      <c r="D474" t="inlineStr"/>
+      <c r="E474" t="n">
+        <v>86103844</v>
+      </c>
+      <c r="F474" t="n">
+        <v>0.288453</v>
+      </c>
+      <c r="G474" t="n">
+        <v>-0.3469013946244801</v>
+      </c>
+      <c r="H474" t="n">
+        <v>1.274458165559376</v>
+      </c>
+      <c r="I474" t="n">
+        <v>-11.98353835824248</v>
+      </c>
+      <c r="J474" t="n">
+        <v>0</v>
+      </c>
+      <c r="K474" t="b">
+        <v>0</v>
+      </c>
+      <c r="L474" t="inlineStr"/>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>The Grays Currency</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>ptgc</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/32933/large/IMG_8413.jpeg?1738402400</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr"/>
+      <c r="E475" t="n">
+        <v>86012509</v>
+      </c>
+      <c r="F475" t="n">
+        <v>0.00029497</v>
+      </c>
+      <c r="G475" t="n">
+        <v>0.697034118477859</v>
+      </c>
+      <c r="H475" t="n">
+        <v>20.33322657563125</v>
+      </c>
+      <c r="I475" t="n">
+        <v>8.398283157897838</v>
+      </c>
+      <c r="J475" t="n">
+        <v>0.08666666666666667</v>
+      </c>
+      <c r="K475" t="b">
+        <v>0</v>
+      </c>
+      <c r="L475" t="inlineStr"/>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>Venice Token</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>vvv</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://coin-images.coingecko.com/coins/images/54023/large/VVV_Token_Transparent.png?1741856877</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr"/>
+      <c r="E476" t="n">
+        <v>85852104</v>
+      </c>
+      <c r="F476" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="G476" t="n">
+        <v>0.4438353487632961</v>
+      </c>
+      <c r="H476" t="n">
+        <v>-6.183021431044884</v>
+      </c>
+      <c r="I476" t="n">
+        <v>-3.443205488891702</v>
+      </c>
+      <c r="J476" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="K476" t="b">
+        <v>0</v>
+      </c>
+      <c r="L476" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>